<commit_message>
Atualização de Conferência LN - NFR
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_NFR.xlsx
+++ b/Documentação/Planilhas/Conferencia_NFR.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="236">
   <si>
     <t>1</t>
   </si>
@@ -83,9 +83,6 @@
     <t>60</t>
   </si>
   <si>
-    <t>da nf</t>
-  </si>
-  <si>
     <t>dbo.stg_nfr_rascunho_cab</t>
   </si>
   <si>
@@ -368,9 +365,6 @@
     <t>Venda de Mercadoria no Estado</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>A00200</t>
   </si>
   <si>
@@ -665,10 +659,74 @@
     <t>Fazer o detalhamento da Referência Fiscal. Na aba inferior Linhas, detalhar a linha apresentada. Em seguida, escolher a aba "Ordens Origem por linha do pré Recebimento". Pegar a informação da coluna Ordem</t>
   </si>
   <si>
-    <t>Fazer o detalhamento da Referência Fiscal. Na aba inferior Linhas, detalhar as linha apresentada. Em seguida, escolher a aba "Ordens Origem por linha do pré Recebimento". Copiar a informação da coluna Ordem. Em seguida, pedir o detalhamento da coluna ordem e colar a informação na coluna Ordem da tela apresentada. Pegar a segunda informação da coluna Origem</t>
-  </si>
-  <si>
     <t>Está pegando a mesma informação do VL_DESCONTO</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Referência Fiscal. Na aba Outros, pegar a informação da "Primeira Data de Verificação"</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Referência Fiscal. Na aba Geral, seção "Referência", pegar a informação de "Status"</t>
+  </si>
+  <si>
+    <t>Os códigos utilizados são:</t>
+  </si>
+  <si>
+    <t>1 - Não Aplicável
+2 - Aberto
+3 - NF com erro
+4 - A Agendar
+5 - Agendado</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Referência Fiscal. Na aba Geral, seção "Referência", pegar a informação de "Fiscal Receipt"</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Referência Fiscal. Na aba inferior Linhas, detalhar a linha apresentada. Na aba Geral, seção "Dados Fiscais", pegar a informação de "Código fiscal de operação"</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Referência Fiscal. Na aba inferior Impostos, pegar a informação da coluna "Valor" para o tipo de imposto ICMS</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Referência Fiscal. Na aba inferior Impostos, pegar a informação da coluna "Valor" para o tipo de imposto ICMS-ST</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Referência Fiscal. Na aba inferior Impostos, pegar a informação da coluna "Valor" para o tipo de imposto IPI</t>
+  </si>
+  <si>
+    <t>tdpur4100m000 [usar o Nr_PEDIDO como filtro na coluna "Ordem de Compra" desta sessão</t>
+  </si>
+  <si>
+    <t>No menu Specific, escolher "Detalhes". Na aba "Pagamento",  seção Pagamento, pegar a informação da Condição de Pagamento</t>
+  </si>
+  <si>
+    <t>No menu Specific, escolher "Detalhes". Na aba "Geral", pegar a informação de "PN Fornecedor"</t>
+  </si>
+  <si>
+    <t>No menu Specific, escolher "Detalhes". Na aba "Geral", seção "Expedição", pegar a informação de "Armazém"</t>
+  </si>
+  <si>
+    <t>tcmcsl115m00l</t>
+  </si>
+  <si>
+    <t>Informar o CD_NATUREZA_OPERACAO_COMPRA na coluna "CFO Oficial". Em seguida, pegar a primeira informação da coluna "Natureza da Operação"</t>
+  </si>
+  <si>
+    <t>Pegar a informação da coluna "Data da Ordem"</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Referência Fiscal. Na aba Valores, pegar a informação do Valor de Acréscimo/Desconto, apenas para os casos em que a compra é importação</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Referência Fiscal. Na aba inferior Impostos, pegar a informação da coluna "Valor" para o tipo de imposto PIS, apenas para os casos em que a compra é importação</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Referência Fiscal. Na aba inferior Impostos, pegar a informação da coluna "Valor" para o tipo de imposto COFINS, apenas para os casos em que a compra é importação</t>
+  </si>
+  <si>
+    <t>tdrecl504m50l</t>
+  </si>
+  <si>
+    <t>Para os casos em que existe o NR_NOTA_RECEBIMENTO, informar o mesmo na coluna "Referência fiscal" desta sessão e pedir o detalhamento da mesma. Na aba valores, pegar a informação de Despesas Aduaneiras</t>
   </si>
 </sst>
 </file>
@@ -829,7 +887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -871,24 +929,31 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,9 +962,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFCC"/>
+      <color rgb="FF99FFCC"/>
       <color rgb="FFFA7E7E"/>
-      <color rgb="FF99FFCC"/>
-      <color rgb="FFFFFFCC"/>
       <color rgb="FFCCECFF"/>
       <color rgb="FFFF5050"/>
     </mruColors>
@@ -1195,10 +1260,10 @@
   <sheetPr>
     <tabColor rgb="FFFA7E7E"/>
   </sheetPr>
-  <dimension ref="A2:AT27"/>
+  <dimension ref="A2:AT30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AH20" sqref="AH20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -1211,65 +1276,61 @@
     <col min="6" max="6" width="19.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="29.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="23.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="24.85546875" style="1" customWidth="1"/>
-    <col min="15" max="16" width="22.85546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="34.42578125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="30.5703125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="44.42578125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="25.85546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="30.42578125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="28" style="1" customWidth="1"/>
-    <col min="23" max="23" width="25.140625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="34.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28" style="1" customWidth="1"/>
+    <col min="10" max="10" width="29.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25" style="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="22.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="23.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="24.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="25.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="27.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="28.42578125" style="1" customWidth="1"/>
+    <col min="20" max="21" width="22.85546875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="34.42578125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="25.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="30.5703125" style="1" customWidth="1"/>
     <col min="25" max="25" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="26.28515625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="24.140625" style="1" customWidth="1"/>
     <col min="28" max="28" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.42578125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.28515625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="28.140625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="24.42578125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="27" style="1" customWidth="1"/>
+    <col min="33" max="33" width="29" style="1" customWidth="1"/>
+    <col min="34" max="34" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="25.7109375" style="1" customWidth="1"/>
+    <col min="42" max="42" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="44" max="45" width="31.42578125" style="1" customWidth="1"/>
-    <col min="46" max="46" width="100.42578125" style="1" customWidth="1"/>
+    <col min="46" max="46" width="29.28515625" style="1" customWidth="1"/>
     <col min="47" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="21">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="16"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:46" ht="21">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="16"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:46">
-      <c r="AT5" s="1" t="s">
-        <v>22</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:46">
@@ -1283,124 +1344,124 @@
         <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>49</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="O6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="U6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="N6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="U6" s="3" t="s">
+      <c r="V6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="V6" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="W6" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Z6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AA6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AB6" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="AC6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AD6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK6" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="AL6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AM6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AN6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO6" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="AP6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ6" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="AQ6" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:46">
@@ -1408,121 +1469,121 @@
         <v>2</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>0</v>
       </c>
       <c r="G7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="P7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q7" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="R7" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="S7" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="T7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="U7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="V7" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="W7" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="X7" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="H7" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="I7" s="11" t="s">
+      <c r="Y7" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z7" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC7" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD7" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE7" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF7" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="J7" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="N7" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="P7" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q7" s="11" t="s">
+      <c r="AG7" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="R7" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="S7" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AI7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AB7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE7" s="1" t="s">
+      <c r="AM7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN7" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="AF7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AH7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AK7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN7" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="AO7" s="1" t="s">
         <v>11</v>
@@ -1539,121 +1600,121 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="R8" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="S8" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="X8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="Y8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z8" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z8" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="AA8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="AF8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI8" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AG8" s="1" t="s">
+      <c r="AJ8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK8" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AH8" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AI8" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AJ8" s="1" t="s">
+      <c r="AL8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AK8" s="4" t="s">
+      <c r="AM8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AL8" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM8" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="AN8" s="1" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="AO8" s="1" t="s">
         <v>11</v>
@@ -1670,76 +1731,76 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="R9" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="S9" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X9" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="Y9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Z9" s="1" t="s">
         <v>11</v>
@@ -1751,40 +1812,40 @@
         <v>11</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>11</v>
+        <v>109</v>
       </c>
       <c r="AD9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE9" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AE9" s="1" t="s">
+      <c r="AF9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AL9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN9" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="AF9" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG9" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="AH9" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI9" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AJ9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AK9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL9" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN9" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="AO9" s="1" t="s">
         <v>11</v>
@@ -1801,121 +1862,121 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="K10" s="1" t="s">
+      <c r="M10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="R10" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="S10" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="V10" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="R10" s="1" t="s">
+      <c r="W10" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z10" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z10" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="AA10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>11</v>
+        <v>109</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="AE10" s="1" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="AF10" s="1" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="AG10" s="1" t="s">
-        <v>129</v>
+        <v>60</v>
       </c>
       <c r="AH10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AI10" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="AJ10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK10" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AL10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AK10" s="4" t="s">
+      <c r="AM10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AL10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM10" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="AN10" s="1" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="AO10" s="1" t="s">
         <v>11</v>
@@ -1932,383 +1993,386 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="K11" s="1" t="s">
+      <c r="M11" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="R11" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="S11" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="W11" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="R11" s="1" t="s">
+      <c r="X11" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z11" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="X11" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y11" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z11" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="AA11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AB11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AH11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI11" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AL11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN11" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="AC11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD11" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AE11" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG11" s="1" t="s">
+      <c r="AO11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AP11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" s="23" customFormat="1">
+      <c r="A12" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="J12" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="AH11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI11" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="AJ11" s="1" t="s">
+      <c r="K12" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="M12" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="N12" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="P12" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q12" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="R12" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="S12" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="T12" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="U12" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="V12" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="W12" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="X12" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y12" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z12" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA12" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="AK11" s="4" t="s">
+      <c r="AB12" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC12" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD12" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE12" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="AF12" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG12" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="AH12" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI12" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ12" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK12" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="AL12" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="AL11" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AM11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AO11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AP11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AQ11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:46">
-      <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V12" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y12" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z12" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA12" s="1" t="s">
+      <c r="AM12" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="AB12" s="1" t="s">
+      <c r="AN12" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="AC12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD12" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AE12" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF12" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AH12" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI12" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="AJ12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AK12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL12" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="AM12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AO12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AP12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AQ12" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="AO12" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="AP12" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ12" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="AR12" s="21"/>
+      <c r="AS12" s="21"/>
+      <c r="AT12" s="21"/>
     </row>
     <row r="13" spans="1:46">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="K13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="R13" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="S13" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="W13" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="X13" s="1" t="s">
-        <v>80</v>
+        <v>135</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AA13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AB13" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG13" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AH13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI13" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK13" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AL13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN13" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="AC13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD13" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AE13" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF13" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG13" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AH13" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI13" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="AJ13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AK13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL13" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="AM13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN13" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="AO13" s="1" t="s">
         <v>11</v>
@@ -2325,40 +2389,40 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="M14" s="1" t="s">
-        <v>11</v>
+        <v>171</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>11</v>
@@ -2369,77 +2433,77 @@
       <c r="P14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q14" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="R14" s="1" t="s">
+      <c r="Q14" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="R14" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="S14" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z14" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="U14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="W14" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="X14" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y14" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="Z14" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="AA14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AB14" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AC14" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="AC14" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="AD14" s="1" t="s">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="AE14" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="AF14" s="1" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="AG14" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AH14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI14" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AJ14" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK14" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="AH14" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="AI14" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="AJ14" s="1" t="s">
+      <c r="AL14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AK14" s="4" t="s">
+      <c r="AM14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AL14" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="AM14" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="AN14" s="1" t="s">
-        <v>11</v>
+        <v>173</v>
       </c>
       <c r="AO14" s="1" t="s">
         <v>11</v>
@@ -2456,121 +2520,121 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="M15" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q15" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="R15" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="S15" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="W15" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="R15" s="1" t="s">
+      <c r="X15" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z15" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="U15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="W15" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="X15" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y15" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="Z15" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="AA15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AB15" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AC15" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="AC15" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="AD15" s="1" t="s">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="AE15" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="AF15" s="1" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="AG15" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AH15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI15" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AJ15" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK15" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="AH15" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="AI15" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="AJ15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AK15" s="4" t="s">
-        <v>3</v>
       </c>
       <c r="AL15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AM15" s="1" t="s">
-        <v>11</v>
+      <c r="AM15" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="AN15" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="AO15" s="1" t="s">
         <v>11</v>
@@ -2587,41 +2651,41 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="N16" s="1" t="s">
         <v>11</v>
       </c>
@@ -2631,35 +2695,35 @@
       <c r="P16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q16" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="R16" s="1" t="s">
+      <c r="Q16" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="R16" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="S16" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z16" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="T16" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="U16" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="V16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="W16" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="X16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y16" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="Z16" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="AA16" s="1" t="s">
         <v>3</v>
@@ -2668,40 +2732,40 @@
         <v>11</v>
       </c>
       <c r="AC16" s="1" t="s">
-        <v>11</v>
+        <v>190</v>
       </c>
       <c r="AD16" s="1" t="s">
-        <v>103</v>
+        <v>19</v>
       </c>
       <c r="AE16" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="AF16" s="1" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="AG16" s="1" t="s">
-        <v>195</v>
+        <v>102</v>
       </c>
       <c r="AH16" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AI16" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AJ16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK16" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AL16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AK16" s="4" t="s">
+      <c r="AM16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AL16" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AM16" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="AN16" s="1" t="s">
-        <v>11</v>
+        <v>140</v>
       </c>
       <c r="AO16" s="1" t="s">
         <v>11</v>
@@ -2713,200 +2777,359 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
-      <c r="AG17" s="1"/>
-      <c r="AK17" s="4"/>
-    </row>
-    <row r="18" spans="1:37">
-      <c r="AG18" s="1"/>
-      <c r="AK18" s="4"/>
-    </row>
-    <row r="19" spans="1:37" ht="11.25" customHeight="1">
+    <row r="17" spans="1:41">
+      <c r="AI17" s="1"/>
+      <c r="AM17" s="4"/>
+    </row>
+    <row r="18" spans="1:41">
+      <c r="AI18" s="1"/>
+      <c r="AM18" s="4"/>
+    </row>
+    <row r="19" spans="1:41" ht="11.25" customHeight="1">
       <c r="B19" s="13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="20" spans="1:37" ht="11.25" customHeight="1">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" ht="11.25" customHeight="1">
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
-    </row>
-    <row r="21" spans="1:37" ht="11.25" customHeight="1">
+      <c r="AO20" s="12" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="21" spans="1:41" ht="11.25" customHeight="1">
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
-    </row>
-    <row r="22" spans="1:37" ht="11.25" customHeight="1">
-      <c r="A22" s="15" t="s">
+      <c r="AC21" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="AG21" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AO21" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" ht="11.25" customHeight="1">
+      <c r="A22" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="D22" s="17" t="s">
+      <c r="B22" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="G22" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="H22" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="I22" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="K22" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="L22" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="M22" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="N22" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="O22" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="P22" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="J22" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="K22" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="L22" s="17" t="s">
+      <c r="Q22" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="R22" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="S22" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="T22" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="M22" s="17" t="s">
+      <c r="U22" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="N22" s="20" t="s">
+      <c r="V22" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="W22" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="X22" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y22" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z22" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA22" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB22" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC22" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="AD22" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="AE22" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="AF22" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="AG22" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="AO22" s="16"/>
+    </row>
+    <row r="23" spans="1:41">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="16"/>
+      <c r="X23" s="16"/>
+      <c r="Y23" s="16"/>
+      <c r="Z23" s="16"/>
+      <c r="AA23" s="16"/>
+      <c r="AB23" s="16"/>
+      <c r="AC23" s="16"/>
+      <c r="AD23" s="16"/>
+      <c r="AE23" s="16"/>
+      <c r="AF23" s="16"/>
+      <c r="AG23" s="16"/>
+      <c r="AO23" s="16"/>
+    </row>
+    <row r="24" spans="1:41">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="16"/>
+      <c r="V24" s="16"/>
+      <c r="W24" s="16"/>
+      <c r="X24" s="16"/>
+      <c r="Y24" s="16"/>
+      <c r="Z24" s="16"/>
+      <c r="AA24" s="16"/>
+      <c r="AB24" s="16"/>
+      <c r="AC24" s="16"/>
+      <c r="AD24" s="16"/>
+      <c r="AE24" s="16"/>
+      <c r="AF24" s="16"/>
+      <c r="AG24" s="16"/>
+      <c r="AO24" s="16"/>
+    </row>
+    <row r="25" spans="1:41">
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
+      <c r="V25" s="16"/>
+      <c r="W25" s="16"/>
+      <c r="X25" s="16"/>
+      <c r="Y25" s="16"/>
+      <c r="Z25" s="16"/>
+      <c r="AA25" s="16"/>
+      <c r="AB25" s="16"/>
+      <c r="AC25" s="16"/>
+      <c r="AD25" s="16"/>
+      <c r="AE25" s="16"/>
+      <c r="AF25" s="16"/>
+      <c r="AG25" s="16"/>
+      <c r="AO25" s="16"/>
+    </row>
+    <row r="26" spans="1:41">
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+      <c r="V26" s="16"/>
+      <c r="W26" s="16"/>
+      <c r="X26" s="16"/>
+      <c r="Y26" s="16"/>
+      <c r="Z26" s="16"/>
+      <c r="AA26" s="16"/>
+      <c r="AB26" s="16"/>
+      <c r="AC26" s="16"/>
+      <c r="AD26" s="16"/>
+      <c r="AE26" s="16"/>
+      <c r="AF26" s="16"/>
+      <c r="AG26" s="16"/>
+      <c r="AO26" s="16"/>
+    </row>
+    <row r="27" spans="1:41">
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="16"/>
+      <c r="V27" s="16"/>
+      <c r="W27" s="16"/>
+      <c r="X27" s="16"/>
+      <c r="Y27" s="16"/>
+      <c r="Z27" s="16"/>
+      <c r="AA27" s="16"/>
+      <c r="AB27" s="16"/>
+      <c r="AC27" s="16"/>
+      <c r="AD27" s="16"/>
+      <c r="AE27" s="16"/>
+      <c r="AF27" s="16"/>
+      <c r="AG27" s="16"/>
+    </row>
+    <row r="29" spans="1:41">
+      <c r="K29" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="O22" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="P22" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q22" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="R22" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="S22" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="23" spans="1:37">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="18"/>
-    </row>
-    <row r="24" spans="1:37">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="18"/>
-    </row>
-    <row r="25" spans="1:37">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="20"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="17"/>
-      <c r="S25" s="18"/>
-    </row>
-    <row r="26" spans="1:37">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="20"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="17"/>
-      <c r="R26" s="17"/>
-      <c r="S26" s="18"/>
-    </row>
-    <row r="27" spans="1:37">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="17"/>
-      <c r="S27" s="18"/>
+    </row>
+    <row r="30" spans="1:41" ht="56.25">
+      <c r="K30" s="20" t="s">
+        <v>218</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="36">
+    <mergeCell ref="AO21:AO26"/>
+    <mergeCell ref="AA22:AA27"/>
+    <mergeCell ref="AB22:AB27"/>
+    <mergeCell ref="AF22:AF27"/>
+    <mergeCell ref="AD22:AD27"/>
+    <mergeCell ref="AG22:AG27"/>
+    <mergeCell ref="AC22:AC27"/>
+    <mergeCell ref="W22:W27"/>
+    <mergeCell ref="K22:K27"/>
+    <mergeCell ref="I22:I27"/>
+    <mergeCell ref="Y22:Y27"/>
+    <mergeCell ref="Z22:Z27"/>
+    <mergeCell ref="Q22:Q27"/>
     <mergeCell ref="R22:R27"/>
     <mergeCell ref="S22:S27"/>
-    <mergeCell ref="N22:N27"/>
+    <mergeCell ref="O22:O27"/>
+    <mergeCell ref="T22:T27"/>
+    <mergeCell ref="U22:U27"/>
+    <mergeCell ref="V22:V27"/>
+    <mergeCell ref="J22:J27"/>
+    <mergeCell ref="X22:X27"/>
+    <mergeCell ref="AE22:AE27"/>
+    <mergeCell ref="P22:P27"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="B22:B27"/>
@@ -2916,15 +3139,10 @@
     <mergeCell ref="F22:F27"/>
     <mergeCell ref="G22:G27"/>
     <mergeCell ref="H22:H27"/>
-    <mergeCell ref="J22:J27"/>
-    <mergeCell ref="K22:K27"/>
-    <mergeCell ref="C22:C27"/>
     <mergeCell ref="L22:L27"/>
     <mergeCell ref="M22:M27"/>
-    <mergeCell ref="O22:O27"/>
-    <mergeCell ref="P22:P27"/>
-    <mergeCell ref="Q22:Q27"/>
-    <mergeCell ref="I22:I27"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="N22:N27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2935,69 +3153,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F43"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="3:6">
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F3" t="str">
         <f>CONCATENATE(C3,",")</f>
-        <v>CD_FILIAL,</v>
+        <v>CD_CIA,</v>
       </c>
     </row>
     <row r="4" spans="3:6">
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" ref="F4:F48" si="0">CONCATENATE(C4,",")</f>
-        <v>NR_NF_RASCUNHO,</v>
+        <v>CD_UNIDADE_EMPRESARIAL,</v>
       </c>
     </row>
     <row r="5" spans="3:6">
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>NR_NF_REFERENCIA,</v>
+        <v>CD_FILIAL,</v>
       </c>
     </row>
     <row r="6" spans="3:6">
       <c r="C6" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>NR_SERIE_NFR_REFERENCIA,</v>
+        <v>NR_NF_RASCUNHO,</v>
       </c>
     </row>
     <row r="7" spans="3:6">
       <c r="C7" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>NR_PEDIDO_COMPRA,</v>
+        <v>NR_NF_REFERENCIA,</v>
       </c>
     </row>
     <row r="8" spans="3:6">
       <c r="C8" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>CD_FORNECEDOR,</v>
+        <v>NR_SERIE_NFR_REFERENCIA,</v>
       </c>
     </row>
     <row r="9" spans="3:6">
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
@@ -3006,7 +3224,7 @@
     </row>
     <row r="10" spans="3:6">
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
@@ -3015,313 +3233,317 @@
     </row>
     <row r="11" spans="3:6">
       <c r="C11" s="3" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>VL_PRODUTO,</v>
+        <v>ESPECIE_NOTA_FISCAL_RECEBIDA,</v>
       </c>
     </row>
     <row r="12" spans="3:6">
       <c r="C12" s="3" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>VL_DESPESA,</v>
+        <v>CD_SITUACAO_RASCUNHO,</v>
       </c>
     </row>
     <row r="13" spans="3:6">
       <c r="C13" s="3" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>VL_DESCONTO,</v>
+        <v>VL_PRODUTO,</v>
       </c>
     </row>
     <row r="14" spans="3:6">
       <c r="C14" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>VL_FRETE,</v>
+        <v>VL_TOTAL,</v>
       </c>
     </row>
     <row r="15" spans="3:6">
       <c r="C15" s="3" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v>VL_SEGURO,</v>
+        <v>VL_DESPESA,</v>
       </c>
     </row>
     <row r="16" spans="3:6">
       <c r="C16" s="3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v>VL_DESCONTO_INCONDICIONAL,</v>
+        <v>VL_DESCONTO,</v>
       </c>
     </row>
     <row r="17" spans="3:6">
       <c r="C17" s="3" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
-        <v>VL_TOTAL,</v>
+        <v>VL_DESCONTO_INCONDICIONAL,</v>
       </c>
     </row>
     <row r="18" spans="3:6">
       <c r="C18" s="3" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v>DT_ANALISE,</v>
+        <v>VL_FRETE,</v>
       </c>
     </row>
     <row r="19" spans="3:6">
       <c r="C19" s="3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v>CD_SITUACAO_RASCUNHO,</v>
+        <v>VL_SEGURO,</v>
       </c>
     </row>
     <row r="20" spans="3:6">
       <c r="C20" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>ESPECIE_NOTA_FISCAL_RECEBIDA,</v>
+        <v>DS_OBSERVACAO,</v>
       </c>
     </row>
     <row r="21" spans="3:6">
       <c r="C21" s="3" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v>NR_NOTA_RECEBIMENTO,</v>
+        <v>DT_ANALISE,</v>
       </c>
     </row>
     <row r="22" spans="3:6">
       <c r="C22" s="3" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>CD_DEPOSITO,</v>
+        <v>NR_PEDIDO_COMPRA,</v>
       </c>
     </row>
     <row r="23" spans="3:6">
       <c r="C23" s="3" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>CD_CONDICAO_PAGAMENTO,</v>
+        <v>CD_FORNECEDOR,</v>
       </c>
     </row>
     <row r="24" spans="3:6">
       <c r="C24" s="3" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>CD_NATUREZA_OPERACAO_COMPRA,</v>
+        <v>NR_NOTA_RECEBIMENTO,</v>
       </c>
     </row>
     <row r="25" spans="3:6">
       <c r="C25" s="3" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>VL_ICMS,</v>
+        <v>CD_DEPOSITO,</v>
       </c>
     </row>
     <row r="26" spans="3:6">
       <c r="C26" s="3" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>VL_ICMS_ST,</v>
+        <v>CD_CONDICAO_PAGAMENTO,</v>
       </c>
     </row>
     <row r="27" spans="3:6">
       <c r="C27" s="3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v>VL_IPI,</v>
+        <v>CD_NATUREZA_OPERACAO_COMPRA,</v>
       </c>
     </row>
     <row r="28" spans="3:6">
       <c r="C28" s="3" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v>VL_IMPOSTO_IMPORTACAO,</v>
+        <v>VL_ICMS,</v>
       </c>
     </row>
     <row r="29" spans="3:6">
       <c r="C29" s="3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>SQ_NATUREZA_OPERACAO_COMPRA,</v>
+        <v>VL_ICMS_ST,</v>
       </c>
     </row>
     <row r="30" spans="3:6">
       <c r="C30" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>DT_GERACAO_REGISTRO,</v>
+        <v>VL_IPI,</v>
       </c>
     </row>
     <row r="31" spans="3:6">
       <c r="C31" s="3" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>CD_USUARIO_INCLUSAO,</v>
+        <v>VL_IMPOSTO_IMPORTACAO,</v>
       </c>
     </row>
     <row r="32" spans="3:6">
       <c r="C32" s="3" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>DT_INCLUSAO,</v>
+        <v>SQ_NATUREZA_OPERACAO_COMPRA,</v>
       </c>
     </row>
     <row r="33" spans="3:6">
       <c r="C33" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v>CD_USUARIO_ALTERACAO,</v>
+        <v>DT_GERACAO_REGISTRO,</v>
       </c>
     </row>
     <row r="34" spans="3:6">
       <c r="C34" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v>DT_ALTERACAO,</v>
+        <v>CD_USUARIO_INCLUSAO,</v>
       </c>
     </row>
     <row r="35" spans="3:6">
       <c r="C35" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>CD_USUARIO_CANCELAMENTO,</v>
+        <v>DT_INCLUSAO,</v>
       </c>
     </row>
     <row r="36" spans="3:6">
-      <c r="C36" s="5" t="s">
-        <v>48</v>
+      <c r="C36" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v>DT_CANCELAMENTO,</v>
+        <v>CD_USUARIO_ALTERACAO,</v>
       </c>
     </row>
     <row r="37" spans="3:6">
       <c r="C37" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v>DS_SITUACAO_ANALISE,</v>
+        <v>DT_ALTERACAO,</v>
       </c>
     </row>
     <row r="38" spans="3:6">
       <c r="C38" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v>DS_OBSERVACAO,</v>
+        <v>CD_USUARIO_CANCELAMENTO,</v>
       </c>
     </row>
     <row r="39" spans="3:6">
-      <c r="C39" s="3" t="s">
-        <v>54</v>
+      <c r="C39" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
-        <v>VL_DESPESA_ADUANEIRA,</v>
+        <v>DT_CANCELAMENTO,</v>
       </c>
     </row>
     <row r="40" spans="3:6">
       <c r="C40" s="3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
-        <v>VL_ADICIONAL_IMPORTACAO,</v>
+        <v>DS_SITUACAO_ANALISE,</v>
       </c>
     </row>
     <row r="41" spans="3:6">
       <c r="C41" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
-        <v>VL_PIS_IMPORTACAO,</v>
+        <v>VL_DESPESA_ADUANEIRA,</v>
       </c>
     </row>
     <row r="42" spans="3:6">
       <c r="C42" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
-        <v>VL_COFINS_IMPORTACAO,</v>
+        <v>VL_ADICIONAL_IMPORTACAO,</v>
       </c>
     </row>
     <row r="43" spans="3:6">
       <c r="C43" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
+        <v>VL_PIS_IMPORTACAO,</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6">
+      <c r="C44" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>VL_COFINS_IMPORTACAO,</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6">
+      <c r="C45" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
         <v>VL_CIF_IMPORTACAO,</v>
-      </c>
-    </row>
-    <row r="44" spans="3:6">
-      <c r="C44" s="3"/>
-      <c r="F44" t="str">
-        <f t="shared" si="0"/>
-        <v>,</v>
-      </c>
-    </row>
-    <row r="45" spans="3:6">
-      <c r="C45" s="3"/>
-      <c r="F45" t="str">
-        <f t="shared" si="0"/>
-        <v>,</v>
       </c>
     </row>
     <row r="46" spans="3:6">

</xml_diff>

<commit_message>
Atualização Conferência LN - FAT e NFR
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_NFR.xlsx
+++ b/Documentação/Planilhas/Conferencia_NFR.xlsx
@@ -2818,9 +2818,6 @@
     <t>Na lupinha, informar o Cód Item limpando todos os campos primeiramente. Na aba "Transações", pegar a última informação da coluna Data Transação</t>
   </si>
   <si>
-    <t>Na lupinha, informar o Cód Item limpando todos os campos primeiramente. Na aba "Transações", pegar o valor da coluna da coluna MAUC [BRL] referente à última data da transação</t>
-  </si>
-  <si>
     <t>Sessão whina1512m000</t>
   </si>
   <si>
@@ -2843,6 +2840,9 @@
   </si>
   <si>
     <t>Aguardando a resposta do Fábio sobre o recebimento do mesmo item em dois armazéns distintos.</t>
+  </si>
+  <si>
+    <t>Na lupinha, informar o Cód Item limpando todos os campos primeiramente. Pedir o detalhamento da última data apresentada. Na aba inferior "Detalhes de Custos", pegar o valor da coluna da coluna MAUC [BRL]</t>
   </si>
 </sst>
 </file>
@@ -3266,13 +3266,61 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3308,58 +3356,10 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3375,6 +3375,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3404,19 +3419,7 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3425,20 +3428,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3449,11 +3446,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3481,9 +3484,6 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3845,19 +3845,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:43" ht="21">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="40"/>
+      <c r="B2" s="56"/>
       <c r="C2" s="17" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:43" ht="21">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="41"/>
+      <c r="B3" s="57"/>
       <c r="C3" s="17" t="s">
         <v>245</v>
       </c>
@@ -5312,551 +5312,535 @@
       <c r="AO18" s="4"/>
     </row>
     <row r="19" spans="1:43" ht="11.25" customHeight="1">
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="43"/>
-      <c r="O19" s="43"/>
-      <c r="P19" s="43"/>
-      <c r="Q19" s="43"/>
-      <c r="R19" s="43"/>
-      <c r="S19" s="43"/>
-      <c r="T19" s="43"/>
-      <c r="U19" s="43"/>
-      <c r="V19" s="43"/>
-      <c r="W19" s="43"/>
-      <c r="X19" s="43"/>
-      <c r="Y19" s="43"/>
-      <c r="Z19" s="43"/>
-      <c r="AA19" s="44"/>
-      <c r="AB19" s="51" t="s">
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="59"/>
+      <c r="P19" s="59"/>
+      <c r="Q19" s="59"/>
+      <c r="R19" s="59"/>
+      <c r="S19" s="59"/>
+      <c r="T19" s="59"/>
+      <c r="U19" s="59"/>
+      <c r="V19" s="59"/>
+      <c r="W19" s="59"/>
+      <c r="X19" s="59"/>
+      <c r="Y19" s="59"/>
+      <c r="Z19" s="59"/>
+      <c r="AA19" s="60"/>
+      <c r="AB19" s="47" t="s">
         <v>243</v>
       </c>
-      <c r="AC19" s="52"/>
-      <c r="AD19" s="52"/>
-      <c r="AE19" s="52"/>
-      <c r="AF19" s="52"/>
-      <c r="AG19" s="52"/>
-      <c r="AH19" s="53"/>
-      <c r="AI19" s="66" t="s">
+      <c r="AC19" s="48"/>
+      <c r="AD19" s="48"/>
+      <c r="AE19" s="48"/>
+      <c r="AF19" s="48"/>
+      <c r="AG19" s="48"/>
+      <c r="AH19" s="49"/>
+      <c r="AI19" s="44" t="s">
         <v>238</v>
       </c>
-      <c r="AJ19" s="51" t="s">
+      <c r="AJ19" s="47" t="s">
         <v>239</v>
       </c>
-      <c r="AK19" s="52"/>
-      <c r="AL19" s="52"/>
-      <c r="AM19" s="52"/>
-      <c r="AN19" s="52"/>
-      <c r="AO19" s="53"/>
-      <c r="AP19" s="63" t="s">
+      <c r="AK19" s="48"/>
+      <c r="AL19" s="48"/>
+      <c r="AM19" s="48"/>
+      <c r="AN19" s="48"/>
+      <c r="AO19" s="49"/>
+      <c r="AP19" s="41" t="s">
         <v>240</v>
       </c>
-      <c r="AQ19" s="66" t="s">
+      <c r="AQ19" s="44" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:43" ht="11.25" customHeight="1">
-      <c r="B20" s="45"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="46"/>
-      <c r="N20" s="46"/>
-      <c r="O20" s="46"/>
-      <c r="P20" s="46"/>
-      <c r="Q20" s="46"/>
-      <c r="R20" s="46"/>
-      <c r="S20" s="46"/>
-      <c r="T20" s="46"/>
-      <c r="U20" s="46"/>
-      <c r="V20" s="46"/>
-      <c r="W20" s="46"/>
-      <c r="X20" s="46"/>
-      <c r="Y20" s="46"/>
-      <c r="Z20" s="46"/>
-      <c r="AA20" s="47"/>
-      <c r="AB20" s="54"/>
-      <c r="AC20" s="55"/>
-      <c r="AD20" s="55"/>
-      <c r="AE20" s="55"/>
-      <c r="AF20" s="55"/>
-      <c r="AG20" s="55"/>
-      <c r="AH20" s="56"/>
-      <c r="AI20" s="67"/>
-      <c r="AJ20" s="54"/>
-      <c r="AK20" s="55"/>
-      <c r="AL20" s="55"/>
-      <c r="AM20" s="55"/>
-      <c r="AN20" s="55"/>
-      <c r="AO20" s="56"/>
-      <c r="AP20" s="64"/>
-      <c r="AQ20" s="67"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="62"/>
+      <c r="N20" s="62"/>
+      <c r="O20" s="62"/>
+      <c r="P20" s="62"/>
+      <c r="Q20" s="62"/>
+      <c r="R20" s="62"/>
+      <c r="S20" s="62"/>
+      <c r="T20" s="62"/>
+      <c r="U20" s="62"/>
+      <c r="V20" s="62"/>
+      <c r="W20" s="62"/>
+      <c r="X20" s="62"/>
+      <c r="Y20" s="62"/>
+      <c r="Z20" s="62"/>
+      <c r="AA20" s="63"/>
+      <c r="AB20" s="50"/>
+      <c r="AC20" s="51"/>
+      <c r="AD20" s="51"/>
+      <c r="AE20" s="51"/>
+      <c r="AF20" s="51"/>
+      <c r="AG20" s="51"/>
+      <c r="AH20" s="52"/>
+      <c r="AI20" s="45"/>
+      <c r="AJ20" s="50"/>
+      <c r="AK20" s="51"/>
+      <c r="AL20" s="51"/>
+      <c r="AM20" s="51"/>
+      <c r="AN20" s="51"/>
+      <c r="AO20" s="52"/>
+      <c r="AP20" s="42"/>
+      <c r="AQ20" s="45"/>
     </row>
     <row r="21" spans="1:43" ht="11.25" customHeight="1">
-      <c r="B21" s="48"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="49"/>
-      <c r="O21" s="49"/>
-      <c r="P21" s="49"/>
-      <c r="Q21" s="49"/>
-      <c r="R21" s="49"/>
-      <c r="S21" s="49"/>
-      <c r="T21" s="49"/>
-      <c r="U21" s="49"/>
-      <c r="V21" s="49"/>
-      <c r="W21" s="49"/>
-      <c r="X21" s="49"/>
-      <c r="Y21" s="49"/>
-      <c r="Z21" s="49"/>
-      <c r="AA21" s="50"/>
-      <c r="AB21" s="57"/>
-      <c r="AC21" s="58"/>
-      <c r="AD21" s="58"/>
-      <c r="AE21" s="58"/>
-      <c r="AF21" s="58"/>
-      <c r="AG21" s="58"/>
-      <c r="AH21" s="59"/>
-      <c r="AI21" s="68"/>
-      <c r="AJ21" s="57"/>
-      <c r="AK21" s="58"/>
-      <c r="AL21" s="58"/>
-      <c r="AM21" s="58"/>
-      <c r="AN21" s="58"/>
-      <c r="AO21" s="59"/>
-      <c r="AP21" s="65"/>
-      <c r="AQ21" s="68"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="65"/>
+      <c r="K21" s="65"/>
+      <c r="L21" s="65"/>
+      <c r="M21" s="65"/>
+      <c r="N21" s="65"/>
+      <c r="O21" s="65"/>
+      <c r="P21" s="65"/>
+      <c r="Q21" s="65"/>
+      <c r="R21" s="65"/>
+      <c r="S21" s="65"/>
+      <c r="T21" s="65"/>
+      <c r="U21" s="65"/>
+      <c r="V21" s="65"/>
+      <c r="W21" s="65"/>
+      <c r="X21" s="65"/>
+      <c r="Y21" s="65"/>
+      <c r="Z21" s="65"/>
+      <c r="AA21" s="66"/>
+      <c r="AB21" s="53"/>
+      <c r="AC21" s="54"/>
+      <c r="AD21" s="54"/>
+      <c r="AE21" s="54"/>
+      <c r="AF21" s="54"/>
+      <c r="AG21" s="54"/>
+      <c r="AH21" s="55"/>
+      <c r="AI21" s="46"/>
+      <c r="AJ21" s="53"/>
+      <c r="AK21" s="54"/>
+      <c r="AL21" s="54"/>
+      <c r="AM21" s="54"/>
+      <c r="AN21" s="54"/>
+      <c r="AO21" s="55"/>
+      <c r="AP21" s="43"/>
+      <c r="AQ21" s="46"/>
     </row>
     <row r="22" spans="1:43" ht="11.25" customHeight="1">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="37" t="s">
         <v>198</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="D22" s="37" t="s">
         <v>199</v>
       </c>
-      <c r="E22" s="38" t="s">
+      <c r="E22" s="37" t="s">
         <v>200</v>
       </c>
-      <c r="F22" s="38" t="s">
+      <c r="F22" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="G22" s="38" t="s">
+      <c r="G22" s="37" t="s">
         <v>216</v>
       </c>
-      <c r="H22" s="38" t="s">
+      <c r="H22" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="I22" s="38" t="s">
+      <c r="I22" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="J22" s="38" t="s">
+      <c r="J22" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="K22" s="38" t="s">
+      <c r="K22" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="L22" s="38" t="s">
+      <c r="L22" s="37" t="s">
         <v>204</v>
       </c>
-      <c r="M22" s="38" t="s">
+      <c r="M22" s="37" t="s">
         <v>205</v>
       </c>
-      <c r="N22" s="37" t="s">
+      <c r="N22" s="67" t="s">
         <v>211</v>
       </c>
-      <c r="O22" s="38" t="s">
+      <c r="O22" s="37" t="s">
         <v>226</v>
       </c>
-      <c r="P22" s="38" t="s">
+      <c r="P22" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="Q22" s="38" t="s">
+      <c r="Q22" s="37" t="s">
         <v>228</v>
       </c>
-      <c r="R22" s="38" t="s">
+      <c r="R22" s="37" t="s">
         <v>206</v>
       </c>
-      <c r="S22" s="38" t="s">
+      <c r="S22" s="37" t="s">
         <v>207</v>
       </c>
-      <c r="T22" s="38" t="s">
+      <c r="T22" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="U22" s="38" t="s">
+      <c r="U22" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="V22" s="38" t="s">
+      <c r="V22" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="W22" s="38" t="s">
+      <c r="W22" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="X22" s="38" t="s">
+      <c r="X22" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="Y22" s="38" t="s">
+      <c r="Y22" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="Z22" s="38" t="s">
+      <c r="Z22" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="AA22" s="38" t="s">
+      <c r="AA22" s="37" t="s">
         <v>237</v>
       </c>
-      <c r="AB22" s="38" t="s">
+      <c r="AB22" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="AC22" s="38" t="s">
+      <c r="AC22" s="37" t="s">
         <v>221</v>
       </c>
-      <c r="AD22" s="38" t="s">
+      <c r="AD22" s="37" t="s">
         <v>222</v>
       </c>
-      <c r="AE22" s="38" t="s">
+      <c r="AE22" s="37" t="s">
         <v>223</v>
       </c>
-      <c r="AF22" s="38" t="s">
+      <c r="AF22" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="AG22" s="38" t="s">
+      <c r="AG22" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="AH22" s="38" t="s">
+      <c r="AH22" s="37" t="s">
         <v>244</v>
       </c>
-      <c r="AI22" s="38" t="s">
+      <c r="AI22" s="37" t="s">
         <v>224</v>
       </c>
-      <c r="AJ22" s="38" t="s">
+      <c r="AJ22" s="37" t="s">
         <v>230</v>
       </c>
-      <c r="AK22" s="38" t="s">
+      <c r="AK22" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="AL22" s="38" t="s">
+      <c r="AL22" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="AM22" s="38" t="s">
+      <c r="AM22" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="AN22" s="38" t="s">
+      <c r="AN22" s="37" t="s">
         <v>234</v>
       </c>
-      <c r="AO22" s="38" t="s">
+      <c r="AO22" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="AP22" s="38" t="s">
+      <c r="AP22" s="37" t="s">
         <v>236</v>
       </c>
-      <c r="AQ22" s="60" t="s">
+      <c r="AQ22" s="38" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:43">
-      <c r="A23" s="38"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="37"/>
-      <c r="O23" s="38"/>
-      <c r="P23" s="38"/>
-      <c r="Q23" s="38"/>
-      <c r="R23" s="38"/>
-      <c r="S23" s="38"/>
-      <c r="T23" s="38"/>
-      <c r="U23" s="38"/>
-      <c r="V23" s="38"/>
-      <c r="W23" s="38"/>
-      <c r="X23" s="38"/>
-      <c r="Y23" s="38"/>
-      <c r="Z23" s="38"/>
-      <c r="AA23" s="38"/>
-      <c r="AB23" s="38"/>
-      <c r="AC23" s="38"/>
-      <c r="AD23" s="38"/>
-      <c r="AE23" s="38"/>
-      <c r="AF23" s="38"/>
-      <c r="AG23" s="38"/>
-      <c r="AH23" s="38"/>
-      <c r="AI23" s="38"/>
-      <c r="AJ23" s="38"/>
-      <c r="AK23" s="38"/>
-      <c r="AL23" s="38"/>
-      <c r="AM23" s="38"/>
-      <c r="AN23" s="38"/>
-      <c r="AO23" s="38"/>
-      <c r="AP23" s="38"/>
-      <c r="AQ23" s="61"/>
+      <c r="A23" s="37"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="67"/>
+      <c r="O23" s="37"/>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="37"/>
+      <c r="R23" s="37"/>
+      <c r="S23" s="37"/>
+      <c r="T23" s="37"/>
+      <c r="U23" s="37"/>
+      <c r="V23" s="37"/>
+      <c r="W23" s="37"/>
+      <c r="X23" s="37"/>
+      <c r="Y23" s="37"/>
+      <c r="Z23" s="37"/>
+      <c r="AA23" s="37"/>
+      <c r="AB23" s="37"/>
+      <c r="AC23" s="37"/>
+      <c r="AD23" s="37"/>
+      <c r="AE23" s="37"/>
+      <c r="AF23" s="37"/>
+      <c r="AG23" s="37"/>
+      <c r="AH23" s="37"/>
+      <c r="AI23" s="37"/>
+      <c r="AJ23" s="37"/>
+      <c r="AK23" s="37"/>
+      <c r="AL23" s="37"/>
+      <c r="AM23" s="37"/>
+      <c r="AN23" s="37"/>
+      <c r="AO23" s="37"/>
+      <c r="AP23" s="37"/>
+      <c r="AQ23" s="39"/>
     </row>
     <row r="24" spans="1:43">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="38"/>
-      <c r="R24" s="38"/>
-      <c r="S24" s="38"/>
-      <c r="T24" s="38"/>
-      <c r="U24" s="38"/>
-      <c r="V24" s="38"/>
-      <c r="W24" s="38"/>
-      <c r="X24" s="38"/>
-      <c r="Y24" s="38"/>
-      <c r="Z24" s="38"/>
-      <c r="AA24" s="38"/>
-      <c r="AB24" s="38"/>
-      <c r="AC24" s="38"/>
-      <c r="AD24" s="38"/>
-      <c r="AE24" s="38"/>
-      <c r="AF24" s="38"/>
-      <c r="AG24" s="38"/>
-      <c r="AH24" s="38"/>
-      <c r="AI24" s="38"/>
-      <c r="AJ24" s="38"/>
-      <c r="AK24" s="38"/>
-      <c r="AL24" s="38"/>
-      <c r="AM24" s="38"/>
-      <c r="AN24" s="38"/>
-      <c r="AO24" s="38"/>
-      <c r="AP24" s="38"/>
-      <c r="AQ24" s="61"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="67"/>
+      <c r="O24" s="37"/>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="37"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="37"/>
+      <c r="U24" s="37"/>
+      <c r="V24" s="37"/>
+      <c r="W24" s="37"/>
+      <c r="X24" s="37"/>
+      <c r="Y24" s="37"/>
+      <c r="Z24" s="37"/>
+      <c r="AA24" s="37"/>
+      <c r="AB24" s="37"/>
+      <c r="AC24" s="37"/>
+      <c r="AD24" s="37"/>
+      <c r="AE24" s="37"/>
+      <c r="AF24" s="37"/>
+      <c r="AG24" s="37"/>
+      <c r="AH24" s="37"/>
+      <c r="AI24" s="37"/>
+      <c r="AJ24" s="37"/>
+      <c r="AK24" s="37"/>
+      <c r="AL24" s="37"/>
+      <c r="AM24" s="37"/>
+      <c r="AN24" s="37"/>
+      <c r="AO24" s="37"/>
+      <c r="AP24" s="37"/>
+      <c r="AQ24" s="39"/>
     </row>
     <row r="25" spans="1:43">
-      <c r="A25" s="38"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="37"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="38"/>
-      <c r="U25" s="38"/>
-      <c r="V25" s="38"/>
-      <c r="W25" s="38"/>
-      <c r="X25" s="38"/>
-      <c r="Y25" s="38"/>
-      <c r="Z25" s="38"/>
-      <c r="AA25" s="38"/>
-      <c r="AB25" s="38"/>
-      <c r="AC25" s="38"/>
-      <c r="AD25" s="38"/>
-      <c r="AE25" s="38"/>
-      <c r="AF25" s="38"/>
-      <c r="AG25" s="38"/>
-      <c r="AH25" s="38"/>
-      <c r="AI25" s="38"/>
-      <c r="AJ25" s="38"/>
-      <c r="AK25" s="38"/>
-      <c r="AL25" s="38"/>
-      <c r="AM25" s="38"/>
-      <c r="AN25" s="38"/>
-      <c r="AO25" s="38"/>
-      <c r="AP25" s="38"/>
-      <c r="AQ25" s="61"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="67"/>
+      <c r="O25" s="37"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="37"/>
+      <c r="U25" s="37"/>
+      <c r="V25" s="37"/>
+      <c r="W25" s="37"/>
+      <c r="X25" s="37"/>
+      <c r="Y25" s="37"/>
+      <c r="Z25" s="37"/>
+      <c r="AA25" s="37"/>
+      <c r="AB25" s="37"/>
+      <c r="AC25" s="37"/>
+      <c r="AD25" s="37"/>
+      <c r="AE25" s="37"/>
+      <c r="AF25" s="37"/>
+      <c r="AG25" s="37"/>
+      <c r="AH25" s="37"/>
+      <c r="AI25" s="37"/>
+      <c r="AJ25" s="37"/>
+      <c r="AK25" s="37"/>
+      <c r="AL25" s="37"/>
+      <c r="AM25" s="37"/>
+      <c r="AN25" s="37"/>
+      <c r="AO25" s="37"/>
+      <c r="AP25" s="37"/>
+      <c r="AQ25" s="39"/>
     </row>
     <row r="26" spans="1:43">
-      <c r="A26" s="38"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="37"/>
-      <c r="O26" s="38"/>
-      <c r="P26" s="38"/>
-      <c r="Q26" s="38"/>
-      <c r="R26" s="38"/>
-      <c r="S26" s="38"/>
-      <c r="T26" s="38"/>
-      <c r="U26" s="38"/>
-      <c r="V26" s="38"/>
-      <c r="W26" s="38"/>
-      <c r="X26" s="38"/>
-      <c r="Y26" s="38"/>
-      <c r="Z26" s="38"/>
-      <c r="AA26" s="38"/>
-      <c r="AB26" s="38"/>
-      <c r="AC26" s="38"/>
-      <c r="AD26" s="38"/>
-      <c r="AE26" s="38"/>
-      <c r="AF26" s="38"/>
-      <c r="AG26" s="38"/>
-      <c r="AH26" s="38"/>
-      <c r="AI26" s="38"/>
-      <c r="AJ26" s="38"/>
-      <c r="AK26" s="38"/>
-      <c r="AL26" s="38"/>
-      <c r="AM26" s="38"/>
-      <c r="AN26" s="38"/>
-      <c r="AO26" s="38"/>
-      <c r="AP26" s="38"/>
-      <c r="AQ26" s="61"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="67"/>
+      <c r="O26" s="37"/>
+      <c r="P26" s="37"/>
+      <c r="Q26" s="37"/>
+      <c r="R26" s="37"/>
+      <c r="S26" s="37"/>
+      <c r="T26" s="37"/>
+      <c r="U26" s="37"/>
+      <c r="V26" s="37"/>
+      <c r="W26" s="37"/>
+      <c r="X26" s="37"/>
+      <c r="Y26" s="37"/>
+      <c r="Z26" s="37"/>
+      <c r="AA26" s="37"/>
+      <c r="AB26" s="37"/>
+      <c r="AC26" s="37"/>
+      <c r="AD26" s="37"/>
+      <c r="AE26" s="37"/>
+      <c r="AF26" s="37"/>
+      <c r="AG26" s="37"/>
+      <c r="AH26" s="37"/>
+      <c r="AI26" s="37"/>
+      <c r="AJ26" s="37"/>
+      <c r="AK26" s="37"/>
+      <c r="AL26" s="37"/>
+      <c r="AM26" s="37"/>
+      <c r="AN26" s="37"/>
+      <c r="AO26" s="37"/>
+      <c r="AP26" s="37"/>
+      <c r="AQ26" s="39"/>
     </row>
     <row r="27" spans="1:43">
-      <c r="A27" s="38"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="38"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="38"/>
-      <c r="P27" s="38"/>
-      <c r="Q27" s="38"/>
-      <c r="R27" s="38"/>
-      <c r="S27" s="38"/>
-      <c r="T27" s="38"/>
-      <c r="U27" s="38"/>
-      <c r="V27" s="38"/>
-      <c r="W27" s="38"/>
-      <c r="X27" s="38"/>
-      <c r="Y27" s="38"/>
-      <c r="Z27" s="38"/>
-      <c r="AA27" s="38"/>
-      <c r="AB27" s="38"/>
-      <c r="AC27" s="38"/>
-      <c r="AD27" s="38"/>
-      <c r="AE27" s="38"/>
-      <c r="AF27" s="38"/>
-      <c r="AG27" s="38"/>
-      <c r="AH27" s="38"/>
-      <c r="AI27" s="38"/>
-      <c r="AJ27" s="38"/>
-      <c r="AK27" s="38"/>
-      <c r="AL27" s="38"/>
-      <c r="AM27" s="38"/>
-      <c r="AN27" s="38"/>
-      <c r="AO27" s="38"/>
-      <c r="AP27" s="38"/>
-      <c r="AQ27" s="62"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+      <c r="N27" s="67"/>
+      <c r="O27" s="37"/>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="37"/>
+      <c r="R27" s="37"/>
+      <c r="S27" s="37"/>
+      <c r="T27" s="37"/>
+      <c r="U27" s="37"/>
+      <c r="V27" s="37"/>
+      <c r="W27" s="37"/>
+      <c r="X27" s="37"/>
+      <c r="Y27" s="37"/>
+      <c r="Z27" s="37"/>
+      <c r="AA27" s="37"/>
+      <c r="AB27" s="37"/>
+      <c r="AC27" s="37"/>
+      <c r="AD27" s="37"/>
+      <c r="AE27" s="37"/>
+      <c r="AF27" s="37"/>
+      <c r="AG27" s="37"/>
+      <c r="AH27" s="37"/>
+      <c r="AI27" s="37"/>
+      <c r="AJ27" s="37"/>
+      <c r="AK27" s="37"/>
+      <c r="AL27" s="37"/>
+      <c r="AM27" s="37"/>
+      <c r="AN27" s="37"/>
+      <c r="AO27" s="37"/>
+      <c r="AP27" s="37"/>
+      <c r="AQ27" s="40"/>
     </row>
     <row r="29" spans="1:43" ht="11.25" customHeight="1">
       <c r="I29" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="O29" s="39" t="s">
+      <c r="O29" s="68" t="s">
         <v>327</v>
       </c>
-      <c r="P29" s="39"/>
-      <c r="Q29" s="39"/>
+      <c r="P29" s="68"/>
+      <c r="Q29" s="68"/>
     </row>
     <row r="30" spans="1:43" ht="56.25">
       <c r="I30" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="O30" s="39"/>
-      <c r="P30" s="39"/>
-      <c r="Q30" s="39"/>
+      <c r="O30" s="68"/>
+      <c r="P30" s="68"/>
+      <c r="Q30" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="AO22:AO27"/>
-    <mergeCell ref="AQ22:AQ27"/>
-    <mergeCell ref="AP22:AP27"/>
-    <mergeCell ref="AP19:AP21"/>
-    <mergeCell ref="AI19:AI21"/>
-    <mergeCell ref="AJ19:AO21"/>
-    <mergeCell ref="AQ19:AQ21"/>
-    <mergeCell ref="AI22:AI27"/>
-    <mergeCell ref="AN22:AN27"/>
-    <mergeCell ref="AM22:AM27"/>
-    <mergeCell ref="AK22:AK27"/>
-    <mergeCell ref="AL22:AL27"/>
-    <mergeCell ref="AB19:AH21"/>
-    <mergeCell ref="U22:U27"/>
-    <mergeCell ref="W22:W27"/>
-    <mergeCell ref="X22:X27"/>
-    <mergeCell ref="V22:V27"/>
-    <mergeCell ref="Y22:Y27"/>
-    <mergeCell ref="Z22:Z27"/>
-    <mergeCell ref="AE22:AE27"/>
-    <mergeCell ref="AC22:AC27"/>
-    <mergeCell ref="AB22:AB27"/>
-    <mergeCell ref="AD22:AD27"/>
-    <mergeCell ref="AA22:AA27"/>
-    <mergeCell ref="AH22:AH27"/>
-    <mergeCell ref="AG22:AG27"/>
+    <mergeCell ref="N22:N27"/>
+    <mergeCell ref="K22:K27"/>
+    <mergeCell ref="O29:Q30"/>
+    <mergeCell ref="L22:L27"/>
+    <mergeCell ref="AJ22:AJ27"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="D22:D27"/>
+    <mergeCell ref="E22:E27"/>
+    <mergeCell ref="F22:F27"/>
+    <mergeCell ref="J22:J27"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="AF22:AF27"/>
@@ -5873,16 +5857,32 @@
     <mergeCell ref="S22:S27"/>
     <mergeCell ref="T22:T27"/>
     <mergeCell ref="H22:H27"/>
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="D22:D27"/>
-    <mergeCell ref="E22:E27"/>
-    <mergeCell ref="F22:F27"/>
-    <mergeCell ref="J22:J27"/>
-    <mergeCell ref="N22:N27"/>
-    <mergeCell ref="K22:K27"/>
-    <mergeCell ref="O29:Q30"/>
-    <mergeCell ref="L22:L27"/>
-    <mergeCell ref="AJ22:AJ27"/>
+    <mergeCell ref="AB19:AH21"/>
+    <mergeCell ref="U22:U27"/>
+    <mergeCell ref="W22:W27"/>
+    <mergeCell ref="X22:X27"/>
+    <mergeCell ref="V22:V27"/>
+    <mergeCell ref="Y22:Y27"/>
+    <mergeCell ref="Z22:Z27"/>
+    <mergeCell ref="AE22:AE27"/>
+    <mergeCell ref="AC22:AC27"/>
+    <mergeCell ref="AB22:AB27"/>
+    <mergeCell ref="AD22:AD27"/>
+    <mergeCell ref="AA22:AA27"/>
+    <mergeCell ref="AH22:AH27"/>
+    <mergeCell ref="AG22:AG27"/>
+    <mergeCell ref="AO22:AO27"/>
+    <mergeCell ref="AQ22:AQ27"/>
+    <mergeCell ref="AP22:AP27"/>
+    <mergeCell ref="AP19:AP21"/>
+    <mergeCell ref="AI19:AI21"/>
+    <mergeCell ref="AJ19:AO21"/>
+    <mergeCell ref="AQ19:AQ21"/>
+    <mergeCell ref="AI22:AI27"/>
+    <mergeCell ref="AN22:AN27"/>
+    <mergeCell ref="AM22:AM27"/>
+    <mergeCell ref="AK22:AK27"/>
+    <mergeCell ref="AL22:AL27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5948,19 +5948,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="21">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="41"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="2" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="21">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="41"/>
+      <c r="B3" s="57"/>
       <c r="C3" s="2" t="s">
         <v>333</v>
       </c>
@@ -6755,23 +6755,23 @@
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:23">
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="58" t="s">
         <v>331</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="43"/>
-      <c r="O19" s="43"/>
-      <c r="P19" s="44"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="59"/>
+      <c r="P19" s="60"/>
       <c r="Q19" s="70" t="s">
         <v>332</v>
       </c>
@@ -6780,117 +6780,117 @@
       <c r="T19" s="70"/>
       <c r="U19" s="70"/>
       <c r="V19" s="70"/>
-      <c r="W19" s="66" t="s">
+      <c r="W19" s="44" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:23">
-      <c r="B20" s="45"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="46"/>
-      <c r="N20" s="46"/>
-      <c r="O20" s="46"/>
-      <c r="P20" s="47"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="62"/>
+      <c r="N20" s="62"/>
+      <c r="O20" s="62"/>
+      <c r="P20" s="63"/>
       <c r="Q20" s="70"/>
       <c r="R20" s="70"/>
       <c r="S20" s="70"/>
       <c r="T20" s="70"/>
       <c r="U20" s="70"/>
       <c r="V20" s="70"/>
-      <c r="W20" s="67"/>
+      <c r="W20" s="45"/>
     </row>
     <row r="21" spans="1:23">
-      <c r="B21" s="48"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="49"/>
-      <c r="O21" s="49"/>
-      <c r="P21" s="50"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="65"/>
+      <c r="K21" s="65"/>
+      <c r="L21" s="65"/>
+      <c r="M21" s="65"/>
+      <c r="N21" s="65"/>
+      <c r="O21" s="65"/>
+      <c r="P21" s="66"/>
       <c r="Q21" s="70"/>
       <c r="R21" s="70"/>
       <c r="S21" s="70"/>
       <c r="T21" s="70"/>
       <c r="U21" s="70"/>
       <c r="V21" s="70"/>
-      <c r="W21" s="68"/>
+      <c r="W21" s="46"/>
     </row>
     <row r="22" spans="1:23" ht="11.25" customHeight="1">
       <c r="A22" s="6"/>
-      <c r="B22" s="62" t="s">
+      <c r="B22" s="40" t="s">
         <v>308</v>
       </c>
-      <c r="C22" s="62" t="s">
+      <c r="C22" s="40" t="s">
         <v>309</v>
       </c>
-      <c r="D22" s="62" t="s">
+      <c r="D22" s="40" t="s">
         <v>310</v>
       </c>
-      <c r="E22" s="62" t="s">
+      <c r="E22" s="40" t="s">
         <v>311</v>
       </c>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62" t="s">
+      <c r="F22" s="40"/>
+      <c r="G22" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="H22" s="62" t="s">
+      <c r="H22" s="40" t="s">
         <v>313</v>
       </c>
-      <c r="I22" s="62" t="s">
+      <c r="I22" s="40" t="s">
         <v>314</v>
       </c>
       <c r="J22" s="8"/>
-      <c r="K22" s="62" t="s">
+      <c r="K22" s="40" t="s">
         <v>315</v>
       </c>
-      <c r="L22" s="62" t="s">
+      <c r="L22" s="40" t="s">
         <v>316</v>
       </c>
-      <c r="M22" s="62" t="s">
+      <c r="M22" s="40" t="s">
         <v>317</v>
       </c>
-      <c r="N22" s="62" t="s">
+      <c r="N22" s="40" t="s">
         <v>318</v>
       </c>
-      <c r="O22" s="62" t="s">
+      <c r="O22" s="40" t="s">
         <v>324</v>
       </c>
-      <c r="P22" s="62" t="s">
+      <c r="P22" s="40" t="s">
         <v>325</v>
       </c>
-      <c r="Q22" s="38" t="s">
+      <c r="Q22" s="37" t="s">
         <v>319</v>
       </c>
-      <c r="R22" s="38" t="s">
+      <c r="R22" s="37" t="s">
         <v>320</v>
       </c>
-      <c r="S22" s="38" t="s">
+      <c r="S22" s="37" t="s">
         <v>321</v>
       </c>
-      <c r="T22" s="38" t="s">
+      <c r="T22" s="37" t="s">
         <v>322</v>
       </c>
-      <c r="U22" s="38" t="s">
+      <c r="U22" s="37" t="s">
         <v>323</v>
       </c>
-      <c r="V22" s="38" t="s">
+      <c r="V22" s="37" t="s">
         <v>328</v>
       </c>
       <c r="W22" s="71" t="s">
@@ -6898,123 +6898,123 @@
       </c>
     </row>
     <row r="23" spans="1:23">
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
       <c r="J23" s="8"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="38"/>
-      <c r="O23" s="38"/>
-      <c r="P23" s="38"/>
-      <c r="Q23" s="38"/>
-      <c r="R23" s="38"/>
-      <c r="S23" s="38"/>
-      <c r="T23" s="38"/>
-      <c r="U23" s="38"/>
-      <c r="V23" s="38"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="37"/>
+      <c r="O23" s="37"/>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="37"/>
+      <c r="R23" s="37"/>
+      <c r="S23" s="37"/>
+      <c r="T23" s="37"/>
+      <c r="U23" s="37"/>
+      <c r="V23" s="37"/>
       <c r="W23" s="72"/>
     </row>
     <row r="24" spans="1:23">
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
       <c r="J24" s="8"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="38"/>
-      <c r="R24" s="38"/>
-      <c r="S24" s="38"/>
-      <c r="T24" s="38"/>
-      <c r="U24" s="38"/>
-      <c r="V24" s="38"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="37"/>
+      <c r="O24" s="37"/>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="37"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="37"/>
+      <c r="U24" s="37"/>
+      <c r="V24" s="37"/>
       <c r="W24" s="72"/>
     </row>
     <row r="25" spans="1:23">
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
       <c r="J25" s="8"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="38"/>
-      <c r="U25" s="38"/>
-      <c r="V25" s="38"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="37"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="37"/>
+      <c r="U25" s="37"/>
+      <c r="V25" s="37"/>
       <c r="W25" s="72"/>
     </row>
     <row r="26" spans="1:23">
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
       <c r="J26" s="8"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
-      <c r="O26" s="38"/>
-      <c r="P26" s="38"/>
-      <c r="Q26" s="38"/>
-      <c r="R26" s="38"/>
-      <c r="S26" s="38"/>
-      <c r="T26" s="38"/>
-      <c r="U26" s="38"/>
-      <c r="V26" s="38"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="37"/>
+      <c r="P26" s="37"/>
+      <c r="Q26" s="37"/>
+      <c r="R26" s="37"/>
+      <c r="S26" s="37"/>
+      <c r="T26" s="37"/>
+      <c r="U26" s="37"/>
+      <c r="V26" s="37"/>
       <c r="W26" s="72"/>
     </row>
     <row r="27" spans="1:23">
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
       <c r="J27" s="8"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="38"/>
-      <c r="N27" s="38"/>
-      <c r="O27" s="38"/>
-      <c r="P27" s="38"/>
-      <c r="Q27" s="38"/>
-      <c r="R27" s="38"/>
-      <c r="S27" s="38"/>
-      <c r="T27" s="38"/>
-      <c r="U27" s="38"/>
-      <c r="V27" s="38"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+      <c r="N27" s="37"/>
+      <c r="O27" s="37"/>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="37"/>
+      <c r="R27" s="37"/>
+      <c r="S27" s="37"/>
+      <c r="T27" s="37"/>
+      <c r="U27" s="37"/>
+      <c r="V27" s="37"/>
       <c r="W27" s="73"/>
     </row>
     <row r="28" spans="1:23">
@@ -7022,57 +7022,45 @@
     </row>
     <row r="29" spans="1:23" ht="11.25" customHeight="1">
       <c r="B29" s="6"/>
-      <c r="O29" s="39" t="s">
+      <c r="O29" s="68" t="s">
         <v>326</v>
       </c>
-      <c r="P29" s="39"/>
+      <c r="P29" s="68"/>
       <c r="W29" s="69" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="30" spans="1:23">
       <c r="B30" s="6"/>
-      <c r="O30" s="39"/>
-      <c r="P30" s="39"/>
+      <c r="O30" s="68"/>
+      <c r="P30" s="68"/>
       <c r="W30" s="69"/>
     </row>
     <row r="31" spans="1:23">
-      <c r="O31" s="39"/>
-      <c r="P31" s="39"/>
+      <c r="O31" s="68"/>
+      <c r="P31" s="68"/>
       <c r="W31" s="69"/>
     </row>
     <row r="32" spans="1:23">
-      <c r="O32" s="39"/>
-      <c r="P32" s="39"/>
+      <c r="O32" s="68"/>
+      <c r="P32" s="68"/>
       <c r="W32" s="69"/>
     </row>
     <row r="33" spans="15:23">
-      <c r="O33" s="39"/>
-      <c r="P33" s="39"/>
+      <c r="O33" s="68"/>
+      <c r="P33" s="68"/>
       <c r="W33" s="69"/>
     </row>
     <row r="34" spans="15:23">
-      <c r="O34" s="39"/>
-      <c r="P34" s="39"/>
+      <c r="O34" s="68"/>
+      <c r="P34" s="68"/>
     </row>
     <row r="35" spans="15:23">
-      <c r="O35" s="39"/>
-      <c r="P35" s="39"/>
+      <c r="O35" s="68"/>
+      <c r="P35" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="W19:W21"/>
-    <mergeCell ref="Q22:Q27"/>
-    <mergeCell ref="E22:E27"/>
-    <mergeCell ref="F22:F27"/>
-    <mergeCell ref="G22:G27"/>
-    <mergeCell ref="H22:H27"/>
-    <mergeCell ref="I22:I27"/>
-    <mergeCell ref="K22:K27"/>
-    <mergeCell ref="L22:L27"/>
-    <mergeCell ref="M22:M27"/>
-    <mergeCell ref="N22:N27"/>
-    <mergeCell ref="T22:T27"/>
     <mergeCell ref="B22:B27"/>
     <mergeCell ref="W29:W33"/>
     <mergeCell ref="B19:P21"/>
@@ -7089,6 +7077,18 @@
     <mergeCell ref="W22:W27"/>
     <mergeCell ref="R22:R27"/>
     <mergeCell ref="S22:S27"/>
+    <mergeCell ref="W19:W21"/>
+    <mergeCell ref="Q22:Q27"/>
+    <mergeCell ref="E22:E27"/>
+    <mergeCell ref="F22:F27"/>
+    <mergeCell ref="G22:G27"/>
+    <mergeCell ref="H22:H27"/>
+    <mergeCell ref="I22:I27"/>
+    <mergeCell ref="K22:K27"/>
+    <mergeCell ref="L22:L27"/>
+    <mergeCell ref="M22:M27"/>
+    <mergeCell ref="N22:N27"/>
+    <mergeCell ref="T22:T27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7170,19 +7170,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:56" ht="21">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="40"/>
+      <c r="B2" s="56"/>
       <c r="C2" s="17" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:56" ht="21">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="41"/>
+      <c r="B3" s="57"/>
       <c r="C3" s="17" t="s">
         <v>587</v>
       </c>
@@ -9144,57 +9144,57 @@
       <c r="BB19" s="1"/>
     </row>
     <row r="20" spans="1:56" ht="15" customHeight="1">
-      <c r="B20" s="74" t="s">
+      <c r="B20" s="79" t="s">
         <v>582</v>
       </c>
-      <c r="C20" s="75"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="75"/>
-      <c r="I20" s="75"/>
-      <c r="J20" s="75"/>
-      <c r="K20" s="75"/>
-      <c r="L20" s="75"/>
-      <c r="M20" s="75"/>
-      <c r="N20" s="75"/>
-      <c r="O20" s="75"/>
-      <c r="P20" s="75"/>
-      <c r="Q20" s="75"/>
-      <c r="R20" s="75"/>
-      <c r="S20" s="75"/>
-      <c r="T20" s="75"/>
-      <c r="U20" s="75"/>
-      <c r="V20" s="75"/>
-      <c r="W20" s="75"/>
-      <c r="X20" s="75"/>
-      <c r="Y20" s="75"/>
-      <c r="Z20" s="75"/>
-      <c r="AA20" s="75"/>
-      <c r="AB20" s="75"/>
-      <c r="AC20" s="75"/>
-      <c r="AD20" s="75"/>
-      <c r="AE20" s="75"/>
-      <c r="AF20" s="75"/>
-      <c r="AG20" s="75"/>
-      <c r="AH20" s="75"/>
-      <c r="AI20" s="75"/>
-      <c r="AJ20" s="75"/>
-      <c r="AK20" s="75"/>
-      <c r="AL20" s="75"/>
-      <c r="AM20" s="75"/>
-      <c r="AN20" s="75"/>
-      <c r="AO20" s="75"/>
-      <c r="AP20" s="75"/>
-      <c r="AQ20" s="75"/>
-      <c r="AR20" s="75"/>
-      <c r="AS20" s="75"/>
-      <c r="AT20" s="75"/>
-      <c r="AU20" s="75"/>
-      <c r="AV20" s="75"/>
-      <c r="AW20" s="75"/>
-      <c r="AX20" s="76"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="80"/>
+      <c r="K20" s="80"/>
+      <c r="L20" s="80"/>
+      <c r="M20" s="80"/>
+      <c r="N20" s="80"/>
+      <c r="O20" s="80"/>
+      <c r="P20" s="80"/>
+      <c r="Q20" s="80"/>
+      <c r="R20" s="80"/>
+      <c r="S20" s="80"/>
+      <c r="T20" s="80"/>
+      <c r="U20" s="80"/>
+      <c r="V20" s="80"/>
+      <c r="W20" s="80"/>
+      <c r="X20" s="80"/>
+      <c r="Y20" s="80"/>
+      <c r="Z20" s="80"/>
+      <c r="AA20" s="80"/>
+      <c r="AB20" s="80"/>
+      <c r="AC20" s="80"/>
+      <c r="AD20" s="80"/>
+      <c r="AE20" s="80"/>
+      <c r="AF20" s="80"/>
+      <c r="AG20" s="80"/>
+      <c r="AH20" s="80"/>
+      <c r="AI20" s="80"/>
+      <c r="AJ20" s="80"/>
+      <c r="AK20" s="80"/>
+      <c r="AL20" s="80"/>
+      <c r="AM20" s="80"/>
+      <c r="AN20" s="80"/>
+      <c r="AO20" s="80"/>
+      <c r="AP20" s="80"/>
+      <c r="AQ20" s="80"/>
+      <c r="AR20" s="80"/>
+      <c r="AS20" s="80"/>
+      <c r="AT20" s="80"/>
+      <c r="AU20" s="80"/>
+      <c r="AV20" s="80"/>
+      <c r="AW20" s="80"/>
+      <c r="AX20" s="81"/>
       <c r="AY20" s="70" t="s">
         <v>583</v>
       </c>
@@ -9211,55 +9211,55 @@
       </c>
     </row>
     <row r="21" spans="1:56" ht="11.25" customHeight="1">
-      <c r="B21" s="77"/>
-      <c r="C21" s="78"/>
-      <c r="D21" s="78"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="78"/>
-      <c r="J21" s="78"/>
-      <c r="K21" s="78"/>
-      <c r="L21" s="78"/>
-      <c r="M21" s="78"/>
-      <c r="N21" s="78"/>
-      <c r="O21" s="78"/>
-      <c r="P21" s="78"/>
-      <c r="Q21" s="78"/>
-      <c r="R21" s="78"/>
-      <c r="S21" s="78"/>
-      <c r="T21" s="78"/>
-      <c r="U21" s="78"/>
-      <c r="V21" s="78"/>
-      <c r="W21" s="78"/>
-      <c r="X21" s="78"/>
-      <c r="Y21" s="78"/>
-      <c r="Z21" s="78"/>
-      <c r="AA21" s="78"/>
-      <c r="AB21" s="78"/>
-      <c r="AC21" s="78"/>
-      <c r="AD21" s="78"/>
-      <c r="AE21" s="78"/>
-      <c r="AF21" s="78"/>
-      <c r="AG21" s="78"/>
-      <c r="AH21" s="78"/>
-      <c r="AI21" s="78"/>
-      <c r="AJ21" s="78"/>
-      <c r="AK21" s="78"/>
-      <c r="AL21" s="78"/>
-      <c r="AM21" s="78"/>
-      <c r="AN21" s="78"/>
-      <c r="AO21" s="78"/>
-      <c r="AP21" s="78"/>
-      <c r="AQ21" s="78"/>
-      <c r="AR21" s="78"/>
-      <c r="AS21" s="78"/>
-      <c r="AT21" s="78"/>
-      <c r="AU21" s="78"/>
-      <c r="AV21" s="78"/>
-      <c r="AW21" s="78"/>
-      <c r="AX21" s="79"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="83"/>
+      <c r="H21" s="83"/>
+      <c r="I21" s="83"/>
+      <c r="J21" s="83"/>
+      <c r="K21" s="83"/>
+      <c r="L21" s="83"/>
+      <c r="M21" s="83"/>
+      <c r="N21" s="83"/>
+      <c r="O21" s="83"/>
+      <c r="P21" s="83"/>
+      <c r="Q21" s="83"/>
+      <c r="R21" s="83"/>
+      <c r="S21" s="83"/>
+      <c r="T21" s="83"/>
+      <c r="U21" s="83"/>
+      <c r="V21" s="83"/>
+      <c r="W21" s="83"/>
+      <c r="X21" s="83"/>
+      <c r="Y21" s="83"/>
+      <c r="Z21" s="83"/>
+      <c r="AA21" s="83"/>
+      <c r="AB21" s="83"/>
+      <c r="AC21" s="83"/>
+      <c r="AD21" s="83"/>
+      <c r="AE21" s="83"/>
+      <c r="AF21" s="83"/>
+      <c r="AG21" s="83"/>
+      <c r="AH21" s="83"/>
+      <c r="AI21" s="83"/>
+      <c r="AJ21" s="83"/>
+      <c r="AK21" s="83"/>
+      <c r="AL21" s="83"/>
+      <c r="AM21" s="83"/>
+      <c r="AN21" s="83"/>
+      <c r="AO21" s="83"/>
+      <c r="AP21" s="83"/>
+      <c r="AQ21" s="83"/>
+      <c r="AR21" s="83"/>
+      <c r="AS21" s="83"/>
+      <c r="AT21" s="83"/>
+      <c r="AU21" s="83"/>
+      <c r="AV21" s="83"/>
+      <c r="AW21" s="83"/>
+      <c r="AX21" s="84"/>
       <c r="AY21" s="70"/>
       <c r="AZ21" s="70"/>
       <c r="BA21" s="12"/>
@@ -9268,55 +9268,55 @@
       <c r="BD21" s="70"/>
     </row>
     <row r="22" spans="1:56" ht="11.25" customHeight="1">
-      <c r="B22" s="80"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81"/>
-      <c r="E22" s="81"/>
-      <c r="F22" s="81"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="81"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="81"/>
-      <c r="O22" s="81"/>
-      <c r="P22" s="81"/>
-      <c r="Q22" s="81"/>
-      <c r="R22" s="81"/>
-      <c r="S22" s="81"/>
-      <c r="T22" s="81"/>
-      <c r="U22" s="81"/>
-      <c r="V22" s="81"/>
-      <c r="W22" s="81"/>
-      <c r="X22" s="81"/>
-      <c r="Y22" s="81"/>
-      <c r="Z22" s="81"/>
-      <c r="AA22" s="81"/>
-      <c r="AB22" s="81"/>
-      <c r="AC22" s="81"/>
-      <c r="AD22" s="81"/>
-      <c r="AE22" s="81"/>
-      <c r="AF22" s="81"/>
-      <c r="AG22" s="81"/>
-      <c r="AH22" s="81"/>
-      <c r="AI22" s="81"/>
-      <c r="AJ22" s="81"/>
-      <c r="AK22" s="81"/>
-      <c r="AL22" s="81"/>
-      <c r="AM22" s="81"/>
-      <c r="AN22" s="81"/>
-      <c r="AO22" s="81"/>
-      <c r="AP22" s="81"/>
-      <c r="AQ22" s="81"/>
-      <c r="AR22" s="81"/>
-      <c r="AS22" s="81"/>
-      <c r="AT22" s="81"/>
-      <c r="AU22" s="81"/>
-      <c r="AV22" s="81"/>
-      <c r="AW22" s="81"/>
-      <c r="AX22" s="82"/>
+      <c r="B22" s="85"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="86"/>
+      <c r="I22" s="86"/>
+      <c r="J22" s="86"/>
+      <c r="K22" s="86"/>
+      <c r="L22" s="86"/>
+      <c r="M22" s="86"/>
+      <c r="N22" s="86"/>
+      <c r="O22" s="86"/>
+      <c r="P22" s="86"/>
+      <c r="Q22" s="86"/>
+      <c r="R22" s="86"/>
+      <c r="S22" s="86"/>
+      <c r="T22" s="86"/>
+      <c r="U22" s="86"/>
+      <c r="V22" s="86"/>
+      <c r="W22" s="86"/>
+      <c r="X22" s="86"/>
+      <c r="Y22" s="86"/>
+      <c r="Z22" s="86"/>
+      <c r="AA22" s="86"/>
+      <c r="AB22" s="86"/>
+      <c r="AC22" s="86"/>
+      <c r="AD22" s="86"/>
+      <c r="AE22" s="86"/>
+      <c r="AF22" s="86"/>
+      <c r="AG22" s="86"/>
+      <c r="AH22" s="86"/>
+      <c r="AI22" s="86"/>
+      <c r="AJ22" s="86"/>
+      <c r="AK22" s="86"/>
+      <c r="AL22" s="86"/>
+      <c r="AM22" s="86"/>
+      <c r="AN22" s="86"/>
+      <c r="AO22" s="86"/>
+      <c r="AP22" s="86"/>
+      <c r="AQ22" s="86"/>
+      <c r="AR22" s="86"/>
+      <c r="AS22" s="86"/>
+      <c r="AT22" s="86"/>
+      <c r="AU22" s="86"/>
+      <c r="AV22" s="86"/>
+      <c r="AW22" s="86"/>
+      <c r="AX22" s="87"/>
       <c r="AY22" s="70"/>
       <c r="AZ22" s="70"/>
       <c r="BA22" s="6"/>
@@ -9325,80 +9325,80 @@
       <c r="BD22" s="70"/>
     </row>
     <row r="23" spans="1:56" ht="11.25" customHeight="1">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="62" t="s">
+      <c r="B23" s="40" t="s">
         <v>448</v>
       </c>
-      <c r="C23" s="62" t="s">
+      <c r="C23" s="40" t="s">
         <v>514</v>
       </c>
-      <c r="D23" s="62" t="s">
+      <c r="D23" s="40" t="s">
         <v>515</v>
       </c>
-      <c r="E23" s="62" t="s">
+      <c r="E23" s="40" t="s">
         <v>449</v>
       </c>
-      <c r="F23" s="62" t="s">
+      <c r="F23" s="40" t="s">
         <v>502</v>
       </c>
-      <c r="G23" s="62" t="s">
+      <c r="G23" s="40" t="s">
         <v>503</v>
       </c>
       <c r="H23" s="73" t="s">
         <v>517</v>
       </c>
       <c r="I23" s="73"/>
-      <c r="J23" s="62" t="s">
+      <c r="J23" s="40" t="s">
         <v>497</v>
       </c>
-      <c r="K23" s="62" t="s">
+      <c r="K23" s="40" t="s">
         <v>498</v>
       </c>
-      <c r="L23" s="62" t="s">
+      <c r="L23" s="40" t="s">
         <v>499</v>
       </c>
-      <c r="M23" s="62" t="s">
+      <c r="M23" s="40" t="s">
         <v>500</v>
       </c>
-      <c r="N23" s="62" t="s">
+      <c r="N23" s="40" t="s">
         <v>504</v>
       </c>
-      <c r="O23" s="62" t="s">
+      <c r="O23" s="40" t="s">
         <v>505</v>
       </c>
-      <c r="P23" s="62" t="s">
+      <c r="P23" s="40" t="s">
         <v>506</v>
       </c>
-      <c r="Q23" s="62" t="s">
+      <c r="Q23" s="40" t="s">
         <v>507</v>
       </c>
-      <c r="R23" s="62" t="s">
+      <c r="R23" s="40" t="s">
         <v>508</v>
       </c>
-      <c r="S23" s="62" t="s">
+      <c r="S23" s="40" t="s">
         <v>512</v>
       </c>
-      <c r="T23" s="62" t="s">
+      <c r="T23" s="40" t="s">
         <v>509</v>
       </c>
-      <c r="U23" s="62" t="s">
+      <c r="U23" s="40" t="s">
         <v>510</v>
       </c>
-      <c r="V23" s="62" t="s">
+      <c r="V23" s="40" t="s">
         <v>511</v>
       </c>
-      <c r="W23" s="62" t="s">
+      <c r="W23" s="40" t="s">
         <v>519</v>
       </c>
-      <c r="X23" s="62" t="s">
+      <c r="X23" s="40" t="s">
         <v>513</v>
       </c>
-      <c r="Y23" s="62" t="s">
+      <c r="Y23" s="40" t="s">
         <v>518</v>
       </c>
-      <c r="Z23" s="86" t="s">
+      <c r="Z23" s="75" t="s">
         <v>736</v>
       </c>
       <c r="AA23" s="73" t="s">
@@ -9428,7 +9428,7 @@
       <c r="AI23" s="73" t="s">
         <v>543</v>
       </c>
-      <c r="AJ23" s="85" t="s">
+      <c r="AJ23" s="77" t="s">
         <v>544</v>
       </c>
       <c r="AK23" s="73" t="s">
@@ -9476,253 +9476,253 @@
       <c r="AY23" s="73" t="s">
         <v>559</v>
       </c>
-      <c r="AZ23" s="83" t="s">
+      <c r="AZ23" s="74" t="s">
         <v>560</v>
       </c>
-      <c r="BA23" s="37" t="s">
+      <c r="BA23" s="67" t="s">
         <v>561</v>
       </c>
-      <c r="BB23" s="37" t="s">
+      <c r="BB23" s="67" t="s">
         <v>561</v>
       </c>
-      <c r="BC23" s="83" t="s">
+      <c r="BC23" s="74" t="s">
         <v>562</v>
       </c>
-      <c r="BD23" s="84" t="s">
+      <c r="BD23" s="78" t="s">
         <v>563</v>
       </c>
     </row>
     <row r="24" spans="1:56" ht="11.25" customHeight="1">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="83"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="38"/>
-      <c r="R24" s="38"/>
-      <c r="S24" s="38"/>
-      <c r="T24" s="38"/>
-      <c r="U24" s="38"/>
-      <c r="V24" s="38"/>
-      <c r="W24" s="38"/>
-      <c r="X24" s="38"/>
-      <c r="Y24" s="38"/>
-      <c r="Z24" s="87"/>
-      <c r="AA24" s="83"/>
-      <c r="AB24" s="83"/>
-      <c r="AC24" s="83"/>
-      <c r="AD24" s="83"/>
-      <c r="AE24" s="83"/>
-      <c r="AF24" s="83"/>
-      <c r="AG24" s="83"/>
-      <c r="AH24" s="83"/>
-      <c r="AI24" s="83"/>
-      <c r="AJ24" s="85"/>
-      <c r="AK24" s="83"/>
-      <c r="AL24" s="83"/>
-      <c r="AM24" s="83"/>
-      <c r="AN24" s="83"/>
-      <c r="AO24" s="83"/>
-      <c r="AP24" s="83"/>
-      <c r="AQ24" s="83"/>
-      <c r="AR24" s="83"/>
-      <c r="AS24" s="83"/>
-      <c r="AT24" s="83"/>
-      <c r="AU24" s="83"/>
-      <c r="AV24" s="83"/>
-      <c r="AW24" s="83"/>
-      <c r="AX24" s="83"/>
-      <c r="AY24" s="83"/>
-      <c r="AZ24" s="83"/>
-      <c r="BA24" s="37"/>
-      <c r="BB24" s="37"/>
-      <c r="BC24" s="83"/>
-      <c r="BD24" s="84"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="37"/>
+      <c r="O24" s="37"/>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="37"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="37"/>
+      <c r="U24" s="37"/>
+      <c r="V24" s="37"/>
+      <c r="W24" s="37"/>
+      <c r="X24" s="37"/>
+      <c r="Y24" s="37"/>
+      <c r="Z24" s="76"/>
+      <c r="AA24" s="74"/>
+      <c r="AB24" s="74"/>
+      <c r="AC24" s="74"/>
+      <c r="AD24" s="74"/>
+      <c r="AE24" s="74"/>
+      <c r="AF24" s="74"/>
+      <c r="AG24" s="74"/>
+      <c r="AH24" s="74"/>
+      <c r="AI24" s="74"/>
+      <c r="AJ24" s="77"/>
+      <c r="AK24" s="74"/>
+      <c r="AL24" s="74"/>
+      <c r="AM24" s="74"/>
+      <c r="AN24" s="74"/>
+      <c r="AO24" s="74"/>
+      <c r="AP24" s="74"/>
+      <c r="AQ24" s="74"/>
+      <c r="AR24" s="74"/>
+      <c r="AS24" s="74"/>
+      <c r="AT24" s="74"/>
+      <c r="AU24" s="74"/>
+      <c r="AV24" s="74"/>
+      <c r="AW24" s="74"/>
+      <c r="AX24" s="74"/>
+      <c r="AY24" s="74"/>
+      <c r="AZ24" s="74"/>
+      <c r="BA24" s="67"/>
+      <c r="BB24" s="67"/>
+      <c r="BC24" s="74"/>
+      <c r="BD24" s="78"/>
     </row>
     <row r="25" spans="1:56">
-      <c r="A25" s="38"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="83"/>
-      <c r="I25" s="83"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="38"/>
-      <c r="U25" s="38"/>
-      <c r="V25" s="38"/>
-      <c r="W25" s="38"/>
-      <c r="X25" s="38"/>
-      <c r="Y25" s="38"/>
-      <c r="Z25" s="87"/>
-      <c r="AA25" s="83"/>
-      <c r="AB25" s="83"/>
-      <c r="AC25" s="83"/>
-      <c r="AD25" s="83"/>
-      <c r="AE25" s="83"/>
-      <c r="AF25" s="83"/>
-      <c r="AG25" s="83"/>
-      <c r="AH25" s="83"/>
-      <c r="AI25" s="83"/>
-      <c r="AJ25" s="85"/>
-      <c r="AK25" s="83"/>
-      <c r="AL25" s="83"/>
-      <c r="AM25" s="83"/>
-      <c r="AN25" s="83"/>
-      <c r="AO25" s="83"/>
-      <c r="AP25" s="83"/>
-      <c r="AQ25" s="83"/>
-      <c r="AR25" s="83"/>
-      <c r="AS25" s="83"/>
-      <c r="AT25" s="83"/>
-      <c r="AU25" s="83"/>
-      <c r="AV25" s="83"/>
-      <c r="AW25" s="83"/>
-      <c r="AX25" s="83"/>
-      <c r="AY25" s="83"/>
-      <c r="AZ25" s="83"/>
-      <c r="BA25" s="37"/>
-      <c r="BB25" s="37"/>
-      <c r="BC25" s="83"/>
-      <c r="BD25" s="84"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="37"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="37"/>
+      <c r="U25" s="37"/>
+      <c r="V25" s="37"/>
+      <c r="W25" s="37"/>
+      <c r="X25" s="37"/>
+      <c r="Y25" s="37"/>
+      <c r="Z25" s="76"/>
+      <c r="AA25" s="74"/>
+      <c r="AB25" s="74"/>
+      <c r="AC25" s="74"/>
+      <c r="AD25" s="74"/>
+      <c r="AE25" s="74"/>
+      <c r="AF25" s="74"/>
+      <c r="AG25" s="74"/>
+      <c r="AH25" s="74"/>
+      <c r="AI25" s="74"/>
+      <c r="AJ25" s="77"/>
+      <c r="AK25" s="74"/>
+      <c r="AL25" s="74"/>
+      <c r="AM25" s="74"/>
+      <c r="AN25" s="74"/>
+      <c r="AO25" s="74"/>
+      <c r="AP25" s="74"/>
+      <c r="AQ25" s="74"/>
+      <c r="AR25" s="74"/>
+      <c r="AS25" s="74"/>
+      <c r="AT25" s="74"/>
+      <c r="AU25" s="74"/>
+      <c r="AV25" s="74"/>
+      <c r="AW25" s="74"/>
+      <c r="AX25" s="74"/>
+      <c r="AY25" s="74"/>
+      <c r="AZ25" s="74"/>
+      <c r="BA25" s="67"/>
+      <c r="BB25" s="67"/>
+      <c r="BC25" s="74"/>
+      <c r="BD25" s="78"/>
     </row>
     <row r="26" spans="1:56">
-      <c r="A26" s="38"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="83"/>
-      <c r="I26" s="83"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
-      <c r="O26" s="38"/>
-      <c r="P26" s="38"/>
-      <c r="Q26" s="38"/>
-      <c r="R26" s="38"/>
-      <c r="S26" s="38"/>
-      <c r="T26" s="38"/>
-      <c r="U26" s="38"/>
-      <c r="V26" s="38"/>
-      <c r="W26" s="38"/>
-      <c r="X26" s="38"/>
-      <c r="Y26" s="38"/>
-      <c r="Z26" s="87"/>
-      <c r="AA26" s="83"/>
-      <c r="AB26" s="83"/>
-      <c r="AC26" s="83"/>
-      <c r="AD26" s="83"/>
-      <c r="AE26" s="83"/>
-      <c r="AF26" s="83"/>
-      <c r="AG26" s="83"/>
-      <c r="AH26" s="83"/>
-      <c r="AI26" s="83"/>
-      <c r="AJ26" s="85"/>
-      <c r="AK26" s="83"/>
-      <c r="AL26" s="83"/>
-      <c r="AM26" s="83"/>
-      <c r="AN26" s="83"/>
-      <c r="AO26" s="83"/>
-      <c r="AP26" s="83"/>
-      <c r="AQ26" s="83"/>
-      <c r="AR26" s="83"/>
-      <c r="AS26" s="83"/>
-      <c r="AT26" s="83"/>
-      <c r="AU26" s="83"/>
-      <c r="AV26" s="83"/>
-      <c r="AW26" s="83"/>
-      <c r="AX26" s="83"/>
-      <c r="AY26" s="83"/>
-      <c r="AZ26" s="83"/>
-      <c r="BA26" s="37"/>
-      <c r="BB26" s="37"/>
-      <c r="BC26" s="83"/>
-      <c r="BD26" s="84"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="37"/>
+      <c r="P26" s="37"/>
+      <c r="Q26" s="37"/>
+      <c r="R26" s="37"/>
+      <c r="S26" s="37"/>
+      <c r="T26" s="37"/>
+      <c r="U26" s="37"/>
+      <c r="V26" s="37"/>
+      <c r="W26" s="37"/>
+      <c r="X26" s="37"/>
+      <c r="Y26" s="37"/>
+      <c r="Z26" s="76"/>
+      <c r="AA26" s="74"/>
+      <c r="AB26" s="74"/>
+      <c r="AC26" s="74"/>
+      <c r="AD26" s="74"/>
+      <c r="AE26" s="74"/>
+      <c r="AF26" s="74"/>
+      <c r="AG26" s="74"/>
+      <c r="AH26" s="74"/>
+      <c r="AI26" s="74"/>
+      <c r="AJ26" s="77"/>
+      <c r="AK26" s="74"/>
+      <c r="AL26" s="74"/>
+      <c r="AM26" s="74"/>
+      <c r="AN26" s="74"/>
+      <c r="AO26" s="74"/>
+      <c r="AP26" s="74"/>
+      <c r="AQ26" s="74"/>
+      <c r="AR26" s="74"/>
+      <c r="AS26" s="74"/>
+      <c r="AT26" s="74"/>
+      <c r="AU26" s="74"/>
+      <c r="AV26" s="74"/>
+      <c r="AW26" s="74"/>
+      <c r="AX26" s="74"/>
+      <c r="AY26" s="74"/>
+      <c r="AZ26" s="74"/>
+      <c r="BA26" s="67"/>
+      <c r="BB26" s="67"/>
+      <c r="BC26" s="74"/>
+      <c r="BD26" s="78"/>
     </row>
     <row r="27" spans="1:56">
-      <c r="A27" s="38"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="83"/>
-      <c r="I27" s="83"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="38"/>
-      <c r="N27" s="38"/>
-      <c r="O27" s="38"/>
-      <c r="P27" s="38"/>
-      <c r="Q27" s="38"/>
-      <c r="R27" s="38"/>
-      <c r="S27" s="38"/>
-      <c r="T27" s="38"/>
-      <c r="U27" s="38"/>
-      <c r="V27" s="38"/>
-      <c r="W27" s="38"/>
-      <c r="X27" s="38"/>
-      <c r="Y27" s="38"/>
-      <c r="Z27" s="87"/>
-      <c r="AA27" s="83"/>
-      <c r="AB27" s="83"/>
-      <c r="AC27" s="83"/>
-      <c r="AD27" s="83"/>
-      <c r="AE27" s="83"/>
-      <c r="AF27" s="83"/>
-      <c r="AG27" s="83"/>
-      <c r="AH27" s="83"/>
-      <c r="AI27" s="83"/>
-      <c r="AJ27" s="85"/>
-      <c r="AK27" s="83"/>
-      <c r="AL27" s="83"/>
-      <c r="AM27" s="83"/>
-      <c r="AN27" s="83"/>
-      <c r="AO27" s="83"/>
-      <c r="AP27" s="83"/>
-      <c r="AQ27" s="83"/>
-      <c r="AR27" s="83"/>
-      <c r="AS27" s="83"/>
-      <c r="AT27" s="83"/>
-      <c r="AU27" s="83"/>
-      <c r="AV27" s="83"/>
-      <c r="AW27" s="83"/>
-      <c r="AX27" s="83"/>
-      <c r="AY27" s="83"/>
-      <c r="AZ27" s="83"/>
-      <c r="BA27" s="37"/>
-      <c r="BB27" s="37"/>
-      <c r="BC27" s="83"/>
-      <c r="BD27" s="84"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+      <c r="N27" s="37"/>
+      <c r="O27" s="37"/>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="37"/>
+      <c r="R27" s="37"/>
+      <c r="S27" s="37"/>
+      <c r="T27" s="37"/>
+      <c r="U27" s="37"/>
+      <c r="V27" s="37"/>
+      <c r="W27" s="37"/>
+      <c r="X27" s="37"/>
+      <c r="Y27" s="37"/>
+      <c r="Z27" s="76"/>
+      <c r="AA27" s="74"/>
+      <c r="AB27" s="74"/>
+      <c r="AC27" s="74"/>
+      <c r="AD27" s="74"/>
+      <c r="AE27" s="74"/>
+      <c r="AF27" s="74"/>
+      <c r="AG27" s="74"/>
+      <c r="AH27" s="74"/>
+      <c r="AI27" s="74"/>
+      <c r="AJ27" s="77"/>
+      <c r="AK27" s="74"/>
+      <c r="AL27" s="74"/>
+      <c r="AM27" s="74"/>
+      <c r="AN27" s="74"/>
+      <c r="AO27" s="74"/>
+      <c r="AP27" s="74"/>
+      <c r="AQ27" s="74"/>
+      <c r="AR27" s="74"/>
+      <c r="AS27" s="74"/>
+      <c r="AT27" s="74"/>
+      <c r="AU27" s="74"/>
+      <c r="AV27" s="74"/>
+      <c r="AW27" s="74"/>
+      <c r="AX27" s="74"/>
+      <c r="AY27" s="74"/>
+      <c r="AZ27" s="74"/>
+      <c r="BA27" s="67"/>
+      <c r="BB27" s="67"/>
+      <c r="BC27" s="74"/>
+      <c r="BD27" s="78"/>
     </row>
     <row r="28" spans="1:56">
       <c r="H28" s="4"/>
@@ -9730,35 +9730,35 @@
       <c r="W28" s="12"/>
       <c r="X28" s="1"/>
       <c r="Z28" s="1"/>
-      <c r="AA28" s="83"/>
-      <c r="AB28" s="83"/>
-      <c r="AC28" s="83"/>
-      <c r="AD28" s="83"/>
-      <c r="AE28" s="83"/>
-      <c r="AF28" s="83"/>
-      <c r="AG28" s="83"/>
-      <c r="AH28" s="83"/>
-      <c r="AI28" s="83"/>
-      <c r="AJ28" s="85"/>
-      <c r="AK28" s="83"/>
-      <c r="AL28" s="83"/>
-      <c r="AM28" s="83"/>
-      <c r="AN28" s="83"/>
-      <c r="AO28" s="83"/>
-      <c r="AP28" s="83"/>
-      <c r="AQ28" s="83"/>
-      <c r="AR28" s="83"/>
-      <c r="AS28" s="83"/>
-      <c r="AT28" s="83"/>
-      <c r="AU28" s="83"/>
-      <c r="AV28" s="83"/>
-      <c r="AW28" s="83"/>
-      <c r="AX28" s="83"/>
-      <c r="AY28" s="83"/>
-      <c r="AZ28" s="83"/>
-      <c r="BA28" s="37"/>
-      <c r="BB28" s="37"/>
-      <c r="BC28" s="83"/>
+      <c r="AA28" s="74"/>
+      <c r="AB28" s="74"/>
+      <c r="AC28" s="74"/>
+      <c r="AD28" s="74"/>
+      <c r="AE28" s="74"/>
+      <c r="AF28" s="74"/>
+      <c r="AG28" s="74"/>
+      <c r="AH28" s="74"/>
+      <c r="AI28" s="74"/>
+      <c r="AJ28" s="77"/>
+      <c r="AK28" s="74"/>
+      <c r="AL28" s="74"/>
+      <c r="AM28" s="74"/>
+      <c r="AN28" s="74"/>
+      <c r="AO28" s="74"/>
+      <c r="AP28" s="74"/>
+      <c r="AQ28" s="74"/>
+      <c r="AR28" s="74"/>
+      <c r="AS28" s="74"/>
+      <c r="AT28" s="74"/>
+      <c r="AU28" s="74"/>
+      <c r="AV28" s="74"/>
+      <c r="AW28" s="74"/>
+      <c r="AX28" s="74"/>
+      <c r="AY28" s="74"/>
+      <c r="AZ28" s="74"/>
+      <c r="BA28" s="67"/>
+      <c r="BB28" s="67"/>
+      <c r="BC28" s="74"/>
     </row>
     <row r="29" spans="1:56">
       <c r="C29" s="21" t="s">
@@ -9777,35 +9777,35 @@
       <c r="Z29" s="25" t="s">
         <v>735</v>
       </c>
-      <c r="AA29" s="83"/>
-      <c r="AB29" s="83"/>
-      <c r="AC29" s="83"/>
-      <c r="AD29" s="83"/>
-      <c r="AE29" s="83"/>
-      <c r="AF29" s="83"/>
-      <c r="AG29" s="83"/>
-      <c r="AH29" s="83"/>
-      <c r="AI29" s="83"/>
-      <c r="AJ29" s="85"/>
-      <c r="AK29" s="83"/>
-      <c r="AL29" s="83"/>
-      <c r="AM29" s="83"/>
-      <c r="AN29" s="83"/>
-      <c r="AO29" s="83"/>
-      <c r="AP29" s="83"/>
-      <c r="AQ29" s="83"/>
-      <c r="AR29" s="83"/>
-      <c r="AS29" s="83"/>
-      <c r="AT29" s="83"/>
-      <c r="AU29" s="83"/>
-      <c r="AV29" s="83"/>
-      <c r="AW29" s="83"/>
-      <c r="AX29" s="83"/>
-      <c r="AY29" s="83"/>
-      <c r="AZ29" s="83"/>
-      <c r="BA29" s="37"/>
-      <c r="BB29" s="37"/>
-      <c r="BC29" s="83"/>
+      <c r="AA29" s="74"/>
+      <c r="AB29" s="74"/>
+      <c r="AC29" s="74"/>
+      <c r="AD29" s="74"/>
+      <c r="AE29" s="74"/>
+      <c r="AF29" s="74"/>
+      <c r="AG29" s="74"/>
+      <c r="AH29" s="74"/>
+      <c r="AI29" s="74"/>
+      <c r="AJ29" s="77"/>
+      <c r="AK29" s="74"/>
+      <c r="AL29" s="74"/>
+      <c r="AM29" s="74"/>
+      <c r="AN29" s="74"/>
+      <c r="AO29" s="74"/>
+      <c r="AP29" s="74"/>
+      <c r="AQ29" s="74"/>
+      <c r="AR29" s="74"/>
+      <c r="AS29" s="74"/>
+      <c r="AT29" s="74"/>
+      <c r="AU29" s="74"/>
+      <c r="AV29" s="74"/>
+      <c r="AW29" s="74"/>
+      <c r="AX29" s="74"/>
+      <c r="AY29" s="74"/>
+      <c r="AZ29" s="74"/>
+      <c r="BA29" s="67"/>
+      <c r="BB29" s="67"/>
+      <c r="BC29" s="74"/>
     </row>
     <row r="30" spans="1:56" ht="123.75">
       <c r="C30" s="14" t="s">
@@ -13141,24 +13141,42 @@
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="AC23:AC29"/>
-    <mergeCell ref="AB23:AB29"/>
-    <mergeCell ref="AD23:AD29"/>
-    <mergeCell ref="AE23:AE29"/>
-    <mergeCell ref="Y23:Y27"/>
-    <mergeCell ref="Q23:Q27"/>
-    <mergeCell ref="R23:R27"/>
-    <mergeCell ref="T23:T27"/>
-    <mergeCell ref="N23:N27"/>
-    <mergeCell ref="O23:O27"/>
-    <mergeCell ref="P23:P27"/>
-    <mergeCell ref="W23:W27"/>
-    <mergeCell ref="Z23:Z27"/>
-    <mergeCell ref="AA23:AA29"/>
-    <mergeCell ref="S23:S27"/>
-    <mergeCell ref="X23:X27"/>
-    <mergeCell ref="U23:U27"/>
-    <mergeCell ref="V23:V27"/>
+    <mergeCell ref="AY20:AY22"/>
+    <mergeCell ref="B20:AX22"/>
+    <mergeCell ref="AZ20:AZ22"/>
+    <mergeCell ref="BC20:BC22"/>
+    <mergeCell ref="BD20:BD22"/>
+    <mergeCell ref="AZ23:AZ29"/>
+    <mergeCell ref="BA23:BA29"/>
+    <mergeCell ref="BB23:BB29"/>
+    <mergeCell ref="BC23:BC29"/>
+    <mergeCell ref="BD23:BD27"/>
+    <mergeCell ref="AU23:AU29"/>
+    <mergeCell ref="AV23:AV29"/>
+    <mergeCell ref="AW23:AW29"/>
+    <mergeCell ref="AX23:AX29"/>
+    <mergeCell ref="AY23:AY29"/>
+    <mergeCell ref="AP23:AP29"/>
+    <mergeCell ref="AQ23:AQ29"/>
+    <mergeCell ref="AR23:AR29"/>
+    <mergeCell ref="AS23:AS29"/>
+    <mergeCell ref="AT23:AT29"/>
+    <mergeCell ref="AK23:AK29"/>
+    <mergeCell ref="AL23:AL29"/>
+    <mergeCell ref="AM23:AM29"/>
+    <mergeCell ref="AN23:AN29"/>
+    <mergeCell ref="AO23:AO29"/>
+    <mergeCell ref="AF23:AF29"/>
+    <mergeCell ref="AG23:AG29"/>
+    <mergeCell ref="AH23:AH29"/>
+    <mergeCell ref="AI23:AI29"/>
+    <mergeCell ref="AJ23:AJ29"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E23:E27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="D23:D27"/>
     <mergeCell ref="J23:J27"/>
     <mergeCell ref="K23:K27"/>
     <mergeCell ref="L23:L27"/>
@@ -13167,42 +13185,24 @@
     <mergeCell ref="F23:F27"/>
     <mergeCell ref="G23:G27"/>
     <mergeCell ref="H23:I27"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="E23:E27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="AF23:AF29"/>
-    <mergeCell ref="AG23:AG29"/>
-    <mergeCell ref="AH23:AH29"/>
-    <mergeCell ref="AI23:AI29"/>
-    <mergeCell ref="AJ23:AJ29"/>
-    <mergeCell ref="AK23:AK29"/>
-    <mergeCell ref="AL23:AL29"/>
-    <mergeCell ref="AM23:AM29"/>
-    <mergeCell ref="AN23:AN29"/>
-    <mergeCell ref="AO23:AO29"/>
-    <mergeCell ref="AP23:AP29"/>
-    <mergeCell ref="AQ23:AQ29"/>
-    <mergeCell ref="AR23:AR29"/>
-    <mergeCell ref="AS23:AS29"/>
-    <mergeCell ref="AT23:AT29"/>
-    <mergeCell ref="AU23:AU29"/>
-    <mergeCell ref="AV23:AV29"/>
-    <mergeCell ref="AW23:AW29"/>
-    <mergeCell ref="AX23:AX29"/>
-    <mergeCell ref="AY23:AY29"/>
-    <mergeCell ref="AZ23:AZ29"/>
-    <mergeCell ref="BA23:BA29"/>
-    <mergeCell ref="BB23:BB29"/>
-    <mergeCell ref="BC23:BC29"/>
-    <mergeCell ref="BD23:BD27"/>
-    <mergeCell ref="AY20:AY22"/>
-    <mergeCell ref="B20:AX22"/>
-    <mergeCell ref="AZ20:AZ22"/>
-    <mergeCell ref="BC20:BC22"/>
-    <mergeCell ref="BD20:BD22"/>
+    <mergeCell ref="W23:W27"/>
+    <mergeCell ref="Z23:Z27"/>
+    <mergeCell ref="AA23:AA29"/>
+    <mergeCell ref="S23:S27"/>
+    <mergeCell ref="X23:X27"/>
+    <mergeCell ref="U23:U27"/>
+    <mergeCell ref="V23:V27"/>
+    <mergeCell ref="Q23:Q27"/>
+    <mergeCell ref="R23:R27"/>
+    <mergeCell ref="T23:T27"/>
+    <mergeCell ref="N23:N27"/>
+    <mergeCell ref="O23:O27"/>
+    <mergeCell ref="P23:P27"/>
+    <mergeCell ref="AC23:AC29"/>
+    <mergeCell ref="AB23:AB29"/>
+    <mergeCell ref="AD23:AD29"/>
+    <mergeCell ref="AE23:AE29"/>
+    <mergeCell ref="Y23:Y27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -13216,9 +13216,7 @@
   </sheetPr>
   <dimension ref="A1:BW53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
@@ -13303,10 +13301,10 @@
       <c r="BW1" s="1"/>
     </row>
     <row r="2" spans="1:75" ht="21">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="40"/>
+      <c r="B2" s="56"/>
       <c r="C2" s="17" t="s">
         <v>588</v>
       </c>
@@ -13315,10 +13313,10 @@
       <c r="BW2" s="1"/>
     </row>
     <row r="3" spans="1:75" ht="21">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="41"/>
+      <c r="B3" s="57"/>
       <c r="C3" s="17" t="s">
         <v>848</v>
       </c>
@@ -15854,72 +15852,72 @@
       <c r="BS17" s="12"/>
     </row>
     <row r="18" spans="1:73" ht="11.25" customHeight="1">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="58" t="s">
         <v>582</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="43"/>
-      <c r="O18" s="43"/>
-      <c r="P18" s="43"/>
-      <c r="Q18" s="43"/>
-      <c r="R18" s="43"/>
-      <c r="S18" s="43"/>
-      <c r="T18" s="43"/>
-      <c r="U18" s="43"/>
-      <c r="V18" s="43"/>
-      <c r="W18" s="43"/>
-      <c r="X18" s="43"/>
-      <c r="Y18" s="43"/>
-      <c r="Z18" s="43"/>
-      <c r="AA18" s="43"/>
-      <c r="AB18" s="43"/>
-      <c r="AC18" s="43"/>
-      <c r="AD18" s="43"/>
-      <c r="AE18" s="43"/>
-      <c r="AF18" s="43"/>
-      <c r="AG18" s="43"/>
-      <c r="AH18" s="43"/>
-      <c r="AI18" s="43"/>
-      <c r="AJ18" s="43"/>
-      <c r="AK18" s="43"/>
-      <c r="AL18" s="43"/>
-      <c r="AM18" s="43"/>
-      <c r="AN18" s="43"/>
-      <c r="AO18" s="43"/>
-      <c r="AP18" s="43"/>
-      <c r="AQ18" s="43"/>
-      <c r="AR18" s="43"/>
-      <c r="AS18" s="43"/>
-      <c r="AT18" s="43"/>
-      <c r="AU18" s="43"/>
-      <c r="AV18" s="43"/>
-      <c r="AW18" s="43"/>
-      <c r="AX18" s="43"/>
-      <c r="AY18" s="43"/>
-      <c r="AZ18" s="43"/>
-      <c r="BA18" s="43"/>
-      <c r="BB18" s="43"/>
-      <c r="BC18" s="43"/>
-      <c r="BD18" s="43"/>
-      <c r="BE18" s="43"/>
-      <c r="BF18" s="43"/>
-      <c r="BG18" s="43"/>
-      <c r="BH18" s="43"/>
-      <c r="BI18" s="43"/>
-      <c r="BJ18" s="43"/>
-      <c r="BK18" s="43"/>
-      <c r="BL18" s="43"/>
-      <c r="BM18" s="44"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="59"/>
+      <c r="O18" s="59"/>
+      <c r="P18" s="59"/>
+      <c r="Q18" s="59"/>
+      <c r="R18" s="59"/>
+      <c r="S18" s="59"/>
+      <c r="T18" s="59"/>
+      <c r="U18" s="59"/>
+      <c r="V18" s="59"/>
+      <c r="W18" s="59"/>
+      <c r="X18" s="59"/>
+      <c r="Y18" s="59"/>
+      <c r="Z18" s="59"/>
+      <c r="AA18" s="59"/>
+      <c r="AB18" s="59"/>
+      <c r="AC18" s="59"/>
+      <c r="AD18" s="59"/>
+      <c r="AE18" s="59"/>
+      <c r="AF18" s="59"/>
+      <c r="AG18" s="59"/>
+      <c r="AH18" s="59"/>
+      <c r="AI18" s="59"/>
+      <c r="AJ18" s="59"/>
+      <c r="AK18" s="59"/>
+      <c r="AL18" s="59"/>
+      <c r="AM18" s="59"/>
+      <c r="AN18" s="59"/>
+      <c r="AO18" s="59"/>
+      <c r="AP18" s="59"/>
+      <c r="AQ18" s="59"/>
+      <c r="AR18" s="59"/>
+      <c r="AS18" s="59"/>
+      <c r="AT18" s="59"/>
+      <c r="AU18" s="59"/>
+      <c r="AV18" s="59"/>
+      <c r="AW18" s="59"/>
+      <c r="AX18" s="59"/>
+      <c r="AY18" s="59"/>
+      <c r="AZ18" s="59"/>
+      <c r="BA18" s="59"/>
+      <c r="BB18" s="59"/>
+      <c r="BC18" s="59"/>
+      <c r="BD18" s="59"/>
+      <c r="BE18" s="59"/>
+      <c r="BF18" s="59"/>
+      <c r="BG18" s="59"/>
+      <c r="BH18" s="59"/>
+      <c r="BI18" s="59"/>
+      <c r="BJ18" s="59"/>
+      <c r="BK18" s="59"/>
+      <c r="BL18" s="59"/>
+      <c r="BM18" s="60"/>
       <c r="BN18" s="70" t="s">
         <v>767</v>
       </c>
@@ -15936,161 +15934,161 @@
         <v>586</v>
       </c>
       <c r="BS18" s="30"/>
-      <c r="BT18" s="94" t="s">
+      <c r="BT18" s="97" t="s">
         <v>822</v>
       </c>
-      <c r="BU18" s="94"/>
+      <c r="BU18" s="97"/>
     </row>
     <row r="19" spans="1:73" ht="11.25" customHeight="1">
-      <c r="B19" s="45"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="46"/>
-      <c r="Q19" s="46"/>
-      <c r="R19" s="46"/>
-      <c r="S19" s="46"/>
-      <c r="T19" s="46"/>
-      <c r="U19" s="46"/>
-      <c r="V19" s="46"/>
-      <c r="W19" s="46"/>
-      <c r="X19" s="46"/>
-      <c r="Y19" s="46"/>
-      <c r="Z19" s="46"/>
-      <c r="AA19" s="46"/>
-      <c r="AB19" s="46"/>
-      <c r="AC19" s="46"/>
-      <c r="AD19" s="46"/>
-      <c r="AE19" s="46"/>
-      <c r="AF19" s="46"/>
-      <c r="AG19" s="46"/>
-      <c r="AH19" s="46"/>
-      <c r="AI19" s="46"/>
-      <c r="AJ19" s="46"/>
-      <c r="AK19" s="46"/>
-      <c r="AL19" s="46"/>
-      <c r="AM19" s="46"/>
-      <c r="AN19" s="46"/>
-      <c r="AO19" s="46"/>
-      <c r="AP19" s="46"/>
-      <c r="AQ19" s="46"/>
-      <c r="AR19" s="46"/>
-      <c r="AS19" s="46"/>
-      <c r="AT19" s="46"/>
-      <c r="AU19" s="46"/>
-      <c r="AV19" s="46"/>
-      <c r="AW19" s="46"/>
-      <c r="AX19" s="46"/>
-      <c r="AY19" s="46"/>
-      <c r="AZ19" s="46"/>
-      <c r="BA19" s="46"/>
-      <c r="BB19" s="46"/>
-      <c r="BC19" s="46"/>
-      <c r="BD19" s="46"/>
-      <c r="BE19" s="46"/>
-      <c r="BF19" s="46"/>
-      <c r="BG19" s="46"/>
-      <c r="BH19" s="46"/>
-      <c r="BI19" s="46"/>
-      <c r="BJ19" s="46"/>
-      <c r="BK19" s="46"/>
-      <c r="BL19" s="46"/>
-      <c r="BM19" s="47"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="62"/>
+      <c r="N19" s="62"/>
+      <c r="O19" s="62"/>
+      <c r="P19" s="62"/>
+      <c r="Q19" s="62"/>
+      <c r="R19" s="62"/>
+      <c r="S19" s="62"/>
+      <c r="T19" s="62"/>
+      <c r="U19" s="62"/>
+      <c r="V19" s="62"/>
+      <c r="W19" s="62"/>
+      <c r="X19" s="62"/>
+      <c r="Y19" s="62"/>
+      <c r="Z19" s="62"/>
+      <c r="AA19" s="62"/>
+      <c r="AB19" s="62"/>
+      <c r="AC19" s="62"/>
+      <c r="AD19" s="62"/>
+      <c r="AE19" s="62"/>
+      <c r="AF19" s="62"/>
+      <c r="AG19" s="62"/>
+      <c r="AH19" s="62"/>
+      <c r="AI19" s="62"/>
+      <c r="AJ19" s="62"/>
+      <c r="AK19" s="62"/>
+      <c r="AL19" s="62"/>
+      <c r="AM19" s="62"/>
+      <c r="AN19" s="62"/>
+      <c r="AO19" s="62"/>
+      <c r="AP19" s="62"/>
+      <c r="AQ19" s="62"/>
+      <c r="AR19" s="62"/>
+      <c r="AS19" s="62"/>
+      <c r="AT19" s="62"/>
+      <c r="AU19" s="62"/>
+      <c r="AV19" s="62"/>
+      <c r="AW19" s="62"/>
+      <c r="AX19" s="62"/>
+      <c r="AY19" s="62"/>
+      <c r="AZ19" s="62"/>
+      <c r="BA19" s="62"/>
+      <c r="BB19" s="62"/>
+      <c r="BC19" s="62"/>
+      <c r="BD19" s="62"/>
+      <c r="BE19" s="62"/>
+      <c r="BF19" s="62"/>
+      <c r="BG19" s="62"/>
+      <c r="BH19" s="62"/>
+      <c r="BI19" s="62"/>
+      <c r="BJ19" s="62"/>
+      <c r="BK19" s="62"/>
+      <c r="BL19" s="62"/>
+      <c r="BM19" s="63"/>
       <c r="BN19" s="70"/>
       <c r="BO19" s="70"/>
       <c r="BP19" s="70"/>
       <c r="BQ19" s="70"/>
       <c r="BR19" s="70"/>
       <c r="BS19" s="31"/>
-      <c r="BT19" s="94"/>
-      <c r="BU19" s="94"/>
+      <c r="BT19" s="97"/>
+      <c r="BU19" s="97"/>
     </row>
     <row r="20" spans="1:73" ht="11.25" customHeight="1">
-      <c r="B20" s="48"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="49"/>
-      <c r="O20" s="49"/>
-      <c r="P20" s="49"/>
-      <c r="Q20" s="49"/>
-      <c r="R20" s="49"/>
-      <c r="S20" s="49"/>
-      <c r="T20" s="49"/>
-      <c r="U20" s="49"/>
-      <c r="V20" s="49"/>
-      <c r="W20" s="49"/>
-      <c r="X20" s="49"/>
-      <c r="Y20" s="49"/>
-      <c r="Z20" s="49"/>
-      <c r="AA20" s="49"/>
-      <c r="AB20" s="49"/>
-      <c r="AC20" s="49"/>
-      <c r="AD20" s="49"/>
-      <c r="AE20" s="49"/>
-      <c r="AF20" s="49"/>
-      <c r="AG20" s="49"/>
-      <c r="AH20" s="49"/>
-      <c r="AI20" s="49"/>
-      <c r="AJ20" s="49"/>
-      <c r="AK20" s="49"/>
-      <c r="AL20" s="49"/>
-      <c r="AM20" s="49"/>
-      <c r="AN20" s="49"/>
-      <c r="AO20" s="49"/>
-      <c r="AP20" s="49"/>
-      <c r="AQ20" s="49"/>
-      <c r="AR20" s="49"/>
-      <c r="AS20" s="49"/>
-      <c r="AT20" s="49"/>
-      <c r="AU20" s="49"/>
-      <c r="AV20" s="49"/>
-      <c r="AW20" s="49"/>
-      <c r="AX20" s="49"/>
-      <c r="AY20" s="49"/>
-      <c r="AZ20" s="49"/>
-      <c r="BA20" s="49"/>
-      <c r="BB20" s="49"/>
-      <c r="BC20" s="49"/>
-      <c r="BD20" s="49"/>
-      <c r="BE20" s="49"/>
-      <c r="BF20" s="49"/>
-      <c r="BG20" s="49"/>
-      <c r="BH20" s="49"/>
-      <c r="BI20" s="49"/>
-      <c r="BJ20" s="49"/>
-      <c r="BK20" s="49"/>
-      <c r="BL20" s="49"/>
-      <c r="BM20" s="50"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="65"/>
+      <c r="L20" s="65"/>
+      <c r="M20" s="65"/>
+      <c r="N20" s="65"/>
+      <c r="O20" s="65"/>
+      <c r="P20" s="65"/>
+      <c r="Q20" s="65"/>
+      <c r="R20" s="65"/>
+      <c r="S20" s="65"/>
+      <c r="T20" s="65"/>
+      <c r="U20" s="65"/>
+      <c r="V20" s="65"/>
+      <c r="W20" s="65"/>
+      <c r="X20" s="65"/>
+      <c r="Y20" s="65"/>
+      <c r="Z20" s="65"/>
+      <c r="AA20" s="65"/>
+      <c r="AB20" s="65"/>
+      <c r="AC20" s="65"/>
+      <c r="AD20" s="65"/>
+      <c r="AE20" s="65"/>
+      <c r="AF20" s="65"/>
+      <c r="AG20" s="65"/>
+      <c r="AH20" s="65"/>
+      <c r="AI20" s="65"/>
+      <c r="AJ20" s="65"/>
+      <c r="AK20" s="65"/>
+      <c r="AL20" s="65"/>
+      <c r="AM20" s="65"/>
+      <c r="AN20" s="65"/>
+      <c r="AO20" s="65"/>
+      <c r="AP20" s="65"/>
+      <c r="AQ20" s="65"/>
+      <c r="AR20" s="65"/>
+      <c r="AS20" s="65"/>
+      <c r="AT20" s="65"/>
+      <c r="AU20" s="65"/>
+      <c r="AV20" s="65"/>
+      <c r="AW20" s="65"/>
+      <c r="AX20" s="65"/>
+      <c r="AY20" s="65"/>
+      <c r="AZ20" s="65"/>
+      <c r="BA20" s="65"/>
+      <c r="BB20" s="65"/>
+      <c r="BC20" s="65"/>
+      <c r="BD20" s="65"/>
+      <c r="BE20" s="65"/>
+      <c r="BF20" s="65"/>
+      <c r="BG20" s="65"/>
+      <c r="BH20" s="65"/>
+      <c r="BI20" s="65"/>
+      <c r="BJ20" s="65"/>
+      <c r="BK20" s="65"/>
+      <c r="BL20" s="65"/>
+      <c r="BM20" s="66"/>
       <c r="BN20" s="70"/>
       <c r="BO20" s="70"/>
       <c r="BP20" s="70"/>
       <c r="BQ20" s="70"/>
       <c r="BR20" s="70"/>
       <c r="BS20" s="32"/>
-      <c r="BT20" s="94"/>
-      <c r="BU20" s="94"/>
+      <c r="BT20" s="97"/>
+      <c r="BU20" s="97"/>
     </row>
     <row r="21" spans="1:73" s="29" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A21" s="83" t="s">
+      <c r="A21" s="74" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="73" t="s">
@@ -16153,25 +16151,25 @@
       <c r="U21" s="73" t="s">
         <v>692</v>
       </c>
-      <c r="V21" s="88" t="s">
+      <c r="V21" s="89" t="s">
         <v>719</v>
       </c>
-      <c r="W21" s="88" t="s">
+      <c r="W21" s="89" t="s">
         <v>748</v>
       </c>
       <c r="X21" s="73" t="s">
         <v>757</v>
       </c>
-      <c r="Y21" s="88" t="s">
+      <c r="Y21" s="89" t="s">
         <v>749</v>
       </c>
-      <c r="Z21" s="88" t="s">
+      <c r="Z21" s="89" t="s">
         <v>750</v>
       </c>
       <c r="AA21" s="73" t="s">
         <v>747</v>
       </c>
-      <c r="AB21" s="98" t="s">
+      <c r="AB21" s="91" t="s">
         <v>724</v>
       </c>
       <c r="AC21" s="73" t="s">
@@ -16207,10 +16205,10 @@
       <c r="AM21" s="73" t="s">
         <v>760</v>
       </c>
-      <c r="AN21" s="88" t="s">
+      <c r="AN21" s="89" t="s">
         <v>827</v>
       </c>
-      <c r="AO21" s="88" t="s">
+      <c r="AO21" s="89" t="s">
         <v>828</v>
       </c>
       <c r="AP21" s="73" t="s">
@@ -16225,10 +16223,10 @@
       <c r="AS21" s="73" t="s">
         <v>761</v>
       </c>
-      <c r="AT21" s="88" t="s">
+      <c r="AT21" s="89" t="s">
         <v>825</v>
       </c>
-      <c r="AU21" s="88" t="s">
+      <c r="AU21" s="89" t="s">
         <v>826</v>
       </c>
       <c r="AV21" s="73" t="s">
@@ -16240,10 +16238,10 @@
       <c r="AX21" s="73" t="s">
         <v>756</v>
       </c>
-      <c r="AY21" s="88" t="s">
+      <c r="AY21" s="89" t="s">
         <v>758</v>
       </c>
-      <c r="AZ21" s="88" t="s">
+      <c r="AZ21" s="89" t="s">
         <v>759</v>
       </c>
       <c r="BA21" s="73" t="s">
@@ -16276,333 +16274,333 @@
       <c r="BJ21" s="93" t="s">
         <v>787</v>
       </c>
-      <c r="BK21" s="96" t="s">
+      <c r="BK21" s="95" t="s">
         <v>787</v>
       </c>
-      <c r="BL21" s="92" t="s">
+      <c r="BL21" s="88" t="s">
         <v>819</v>
       </c>
       <c r="BM21" s="34"/>
-      <c r="BN21" s="83" t="s">
+      <c r="BN21" s="74" t="s">
         <v>766</v>
       </c>
-      <c r="BO21" s="83" t="s">
+      <c r="BO21" s="74" t="s">
         <v>765</v>
       </c>
-      <c r="BP21" s="83" t="s">
+      <c r="BP21" s="74" t="s">
         <v>764</v>
       </c>
-      <c r="BQ21" s="83" t="s">
+      <c r="BQ21" s="74" t="s">
         <v>562</v>
       </c>
-      <c r="BR21" s="84" t="s">
+      <c r="BR21" s="78" t="s">
         <v>563</v>
       </c>
       <c r="BS21" s="73" t="s">
         <v>786</v>
       </c>
-      <c r="BT21" s="94"/>
-      <c r="BU21" s="94"/>
+      <c r="BT21" s="97"/>
+      <c r="BU21" s="97"/>
     </row>
     <row r="22" spans="1:73" s="29" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A22" s="83"/>
-      <c r="B22" s="83"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="83"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="83"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="83"/>
-      <c r="I22" s="83"/>
-      <c r="J22" s="83"/>
-      <c r="K22" s="83"/>
-      <c r="L22" s="83"/>
-      <c r="M22" s="83"/>
-      <c r="N22" s="83"/>
-      <c r="O22" s="83"/>
-      <c r="P22" s="83"/>
-      <c r="Q22" s="83"/>
-      <c r="R22" s="83"/>
-      <c r="S22" s="83"/>
-      <c r="T22" s="83"/>
-      <c r="U22" s="83"/>
-      <c r="V22" s="89"/>
-      <c r="W22" s="89"/>
-      <c r="X22" s="83"/>
-      <c r="Y22" s="89"/>
-      <c r="Z22" s="89"/>
-      <c r="AA22" s="83"/>
-      <c r="AB22" s="99"/>
-      <c r="AC22" s="83"/>
-      <c r="AD22" s="83"/>
-      <c r="AE22" s="83"/>
-      <c r="AF22" s="83"/>
-      <c r="AG22" s="83"/>
-      <c r="AH22" s="83"/>
-      <c r="AI22" s="83"/>
-      <c r="AJ22" s="83"/>
-      <c r="AK22" s="83"/>
-      <c r="AL22" s="83"/>
-      <c r="AM22" s="83"/>
-      <c r="AN22" s="89"/>
-      <c r="AO22" s="89"/>
-      <c r="AP22" s="83"/>
-      <c r="AQ22" s="83"/>
-      <c r="AR22" s="83"/>
-      <c r="AS22" s="83"/>
-      <c r="AT22" s="89"/>
-      <c r="AU22" s="89"/>
-      <c r="AV22" s="83"/>
-      <c r="AW22" s="83"/>
-      <c r="AX22" s="83"/>
-      <c r="AY22" s="89"/>
-      <c r="AZ22" s="89"/>
-      <c r="BA22" s="83"/>
-      <c r="BB22" s="83"/>
-      <c r="BC22" s="83"/>
-      <c r="BD22" s="83"/>
-      <c r="BE22" s="83"/>
-      <c r="BF22" s="83"/>
-      <c r="BG22" s="83"/>
-      <c r="BH22" s="83"/>
-      <c r="BI22" s="83"/>
-      <c r="BJ22" s="95"/>
-      <c r="BK22" s="97"/>
-      <c r="BL22" s="92"/>
+      <c r="A22" s="74"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="74"/>
+      <c r="K22" s="74"/>
+      <c r="L22" s="74"/>
+      <c r="M22" s="74"/>
+      <c r="N22" s="74"/>
+      <c r="O22" s="74"/>
+      <c r="P22" s="74"/>
+      <c r="Q22" s="74"/>
+      <c r="R22" s="74"/>
+      <c r="S22" s="74"/>
+      <c r="T22" s="74"/>
+      <c r="U22" s="74"/>
+      <c r="V22" s="90"/>
+      <c r="W22" s="90"/>
+      <c r="X22" s="74"/>
+      <c r="Y22" s="90"/>
+      <c r="Z22" s="90"/>
+      <c r="AA22" s="74"/>
+      <c r="AB22" s="92"/>
+      <c r="AC22" s="74"/>
+      <c r="AD22" s="74"/>
+      <c r="AE22" s="74"/>
+      <c r="AF22" s="74"/>
+      <c r="AG22" s="74"/>
+      <c r="AH22" s="74"/>
+      <c r="AI22" s="74"/>
+      <c r="AJ22" s="74"/>
+      <c r="AK22" s="74"/>
+      <c r="AL22" s="74"/>
+      <c r="AM22" s="74"/>
+      <c r="AN22" s="90"/>
+      <c r="AO22" s="90"/>
+      <c r="AP22" s="74"/>
+      <c r="AQ22" s="74"/>
+      <c r="AR22" s="74"/>
+      <c r="AS22" s="74"/>
+      <c r="AT22" s="90"/>
+      <c r="AU22" s="90"/>
+      <c r="AV22" s="74"/>
+      <c r="AW22" s="74"/>
+      <c r="AX22" s="74"/>
+      <c r="AY22" s="90"/>
+      <c r="AZ22" s="90"/>
+      <c r="BA22" s="74"/>
+      <c r="BB22" s="74"/>
+      <c r="BC22" s="74"/>
+      <c r="BD22" s="74"/>
+      <c r="BE22" s="74"/>
+      <c r="BF22" s="74"/>
+      <c r="BG22" s="74"/>
+      <c r="BH22" s="74"/>
+      <c r="BI22" s="74"/>
+      <c r="BJ22" s="94"/>
+      <c r="BK22" s="96"/>
+      <c r="BL22" s="88"/>
       <c r="BM22" s="34"/>
-      <c r="BN22" s="83"/>
-      <c r="BO22" s="83"/>
-      <c r="BP22" s="83"/>
-      <c r="BQ22" s="83"/>
-      <c r="BR22" s="84"/>
-      <c r="BS22" s="83"/>
-      <c r="BT22" s="94"/>
-      <c r="BU22" s="94"/>
+      <c r="BN22" s="74"/>
+      <c r="BO22" s="74"/>
+      <c r="BP22" s="74"/>
+      <c r="BQ22" s="74"/>
+      <c r="BR22" s="78"/>
+      <c r="BS22" s="74"/>
+      <c r="BT22" s="97"/>
+      <c r="BU22" s="97"/>
     </row>
     <row r="23" spans="1:73" s="29" customFormat="1">
-      <c r="A23" s="83"/>
-      <c r="B23" s="83"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="83"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="83"/>
-      <c r="G23" s="83"/>
-      <c r="H23" s="83"/>
-      <c r="I23" s="83"/>
-      <c r="J23" s="83"/>
-      <c r="K23" s="83"/>
-      <c r="L23" s="83"/>
-      <c r="M23" s="83"/>
-      <c r="N23" s="83"/>
-      <c r="O23" s="83"/>
-      <c r="P23" s="83"/>
-      <c r="Q23" s="83"/>
-      <c r="R23" s="83"/>
-      <c r="S23" s="83"/>
-      <c r="T23" s="83"/>
-      <c r="U23" s="83"/>
-      <c r="V23" s="89"/>
-      <c r="W23" s="89"/>
-      <c r="X23" s="83"/>
-      <c r="Y23" s="89"/>
-      <c r="Z23" s="89"/>
-      <c r="AA23" s="83"/>
-      <c r="AB23" s="99"/>
-      <c r="AC23" s="83"/>
-      <c r="AD23" s="83"/>
-      <c r="AE23" s="83"/>
-      <c r="AF23" s="83"/>
-      <c r="AG23" s="83"/>
-      <c r="AH23" s="83"/>
-      <c r="AI23" s="83"/>
-      <c r="AJ23" s="83"/>
-      <c r="AK23" s="83"/>
-      <c r="AL23" s="83"/>
-      <c r="AM23" s="83"/>
-      <c r="AN23" s="89"/>
-      <c r="AO23" s="89"/>
-      <c r="AP23" s="83"/>
-      <c r="AQ23" s="83"/>
-      <c r="AR23" s="83"/>
-      <c r="AS23" s="83"/>
-      <c r="AT23" s="89"/>
-      <c r="AU23" s="89"/>
-      <c r="AV23" s="83"/>
-      <c r="AW23" s="83"/>
-      <c r="AX23" s="83"/>
-      <c r="AY23" s="89"/>
-      <c r="AZ23" s="89"/>
-      <c r="BA23" s="83"/>
-      <c r="BB23" s="83"/>
-      <c r="BC23" s="83"/>
-      <c r="BD23" s="83"/>
-      <c r="BE23" s="83"/>
-      <c r="BF23" s="83"/>
-      <c r="BG23" s="83"/>
-      <c r="BH23" s="83"/>
-      <c r="BI23" s="83"/>
-      <c r="BJ23" s="95"/>
-      <c r="BK23" s="97"/>
-      <c r="BL23" s="92"/>
+      <c r="A23" s="74"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="74"/>
+      <c r="L23" s="74"/>
+      <c r="M23" s="74"/>
+      <c r="N23" s="74"/>
+      <c r="O23" s="74"/>
+      <c r="P23" s="74"/>
+      <c r="Q23" s="74"/>
+      <c r="R23" s="74"/>
+      <c r="S23" s="74"/>
+      <c r="T23" s="74"/>
+      <c r="U23" s="74"/>
+      <c r="V23" s="90"/>
+      <c r="W23" s="90"/>
+      <c r="X23" s="74"/>
+      <c r="Y23" s="90"/>
+      <c r="Z23" s="90"/>
+      <c r="AA23" s="74"/>
+      <c r="AB23" s="92"/>
+      <c r="AC23" s="74"/>
+      <c r="AD23" s="74"/>
+      <c r="AE23" s="74"/>
+      <c r="AF23" s="74"/>
+      <c r="AG23" s="74"/>
+      <c r="AH23" s="74"/>
+      <c r="AI23" s="74"/>
+      <c r="AJ23" s="74"/>
+      <c r="AK23" s="74"/>
+      <c r="AL23" s="74"/>
+      <c r="AM23" s="74"/>
+      <c r="AN23" s="90"/>
+      <c r="AO23" s="90"/>
+      <c r="AP23" s="74"/>
+      <c r="AQ23" s="74"/>
+      <c r="AR23" s="74"/>
+      <c r="AS23" s="74"/>
+      <c r="AT23" s="90"/>
+      <c r="AU23" s="90"/>
+      <c r="AV23" s="74"/>
+      <c r="AW23" s="74"/>
+      <c r="AX23" s="74"/>
+      <c r="AY23" s="90"/>
+      <c r="AZ23" s="90"/>
+      <c r="BA23" s="74"/>
+      <c r="BB23" s="74"/>
+      <c r="BC23" s="74"/>
+      <c r="BD23" s="74"/>
+      <c r="BE23" s="74"/>
+      <c r="BF23" s="74"/>
+      <c r="BG23" s="74"/>
+      <c r="BH23" s="74"/>
+      <c r="BI23" s="74"/>
+      <c r="BJ23" s="94"/>
+      <c r="BK23" s="96"/>
+      <c r="BL23" s="88"/>
       <c r="BM23" s="34"/>
-      <c r="BN23" s="83"/>
-      <c r="BO23" s="83"/>
-      <c r="BP23" s="83"/>
-      <c r="BQ23" s="83"/>
-      <c r="BR23" s="84"/>
-      <c r="BS23" s="83"/>
-      <c r="BT23" s="94"/>
-      <c r="BU23" s="94"/>
+      <c r="BN23" s="74"/>
+      <c r="BO23" s="74"/>
+      <c r="BP23" s="74"/>
+      <c r="BQ23" s="74"/>
+      <c r="BR23" s="78"/>
+      <c r="BS23" s="74"/>
+      <c r="BT23" s="97"/>
+      <c r="BU23" s="97"/>
     </row>
     <row r="24" spans="1:73" s="29" customFormat="1">
-      <c r="A24" s="83"/>
-      <c r="B24" s="83"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
-      <c r="G24" s="83"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="83"/>
-      <c r="J24" s="83"/>
-      <c r="K24" s="83"/>
-      <c r="L24" s="83"/>
-      <c r="M24" s="83"/>
-      <c r="N24" s="83"/>
-      <c r="O24" s="83"/>
-      <c r="P24" s="83"/>
-      <c r="Q24" s="83"/>
-      <c r="R24" s="83"/>
-      <c r="S24" s="83"/>
-      <c r="T24" s="83"/>
-      <c r="U24" s="83"/>
-      <c r="V24" s="89"/>
-      <c r="W24" s="89"/>
-      <c r="X24" s="83"/>
-      <c r="Y24" s="89"/>
-      <c r="Z24" s="89"/>
-      <c r="AA24" s="83"/>
-      <c r="AB24" s="99"/>
-      <c r="AC24" s="83"/>
-      <c r="AD24" s="83"/>
-      <c r="AE24" s="83"/>
-      <c r="AF24" s="83"/>
-      <c r="AG24" s="83"/>
-      <c r="AH24" s="83"/>
-      <c r="AI24" s="83"/>
-      <c r="AJ24" s="83"/>
-      <c r="AK24" s="83"/>
-      <c r="AL24" s="83"/>
-      <c r="AM24" s="83"/>
-      <c r="AN24" s="89"/>
-      <c r="AO24" s="89"/>
-      <c r="AP24" s="83"/>
-      <c r="AQ24" s="83"/>
-      <c r="AR24" s="83"/>
-      <c r="AS24" s="83"/>
-      <c r="AT24" s="89"/>
-      <c r="AU24" s="89"/>
-      <c r="AV24" s="83"/>
-      <c r="AW24" s="83"/>
-      <c r="AX24" s="83"/>
-      <c r="AY24" s="89"/>
-      <c r="AZ24" s="89"/>
-      <c r="BA24" s="83"/>
-      <c r="BB24" s="83"/>
-      <c r="BC24" s="83"/>
-      <c r="BD24" s="83"/>
-      <c r="BE24" s="83"/>
-      <c r="BF24" s="83"/>
-      <c r="BG24" s="83"/>
-      <c r="BH24" s="83"/>
-      <c r="BI24" s="83"/>
-      <c r="BJ24" s="95"/>
-      <c r="BK24" s="97"/>
-      <c r="BL24" s="92"/>
+      <c r="A24" s="74"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="74"/>
+      <c r="L24" s="74"/>
+      <c r="M24" s="74"/>
+      <c r="N24" s="74"/>
+      <c r="O24" s="74"/>
+      <c r="P24" s="74"/>
+      <c r="Q24" s="74"/>
+      <c r="R24" s="74"/>
+      <c r="S24" s="74"/>
+      <c r="T24" s="74"/>
+      <c r="U24" s="74"/>
+      <c r="V24" s="90"/>
+      <c r="W24" s="90"/>
+      <c r="X24" s="74"/>
+      <c r="Y24" s="90"/>
+      <c r="Z24" s="90"/>
+      <c r="AA24" s="74"/>
+      <c r="AB24" s="92"/>
+      <c r="AC24" s="74"/>
+      <c r="AD24" s="74"/>
+      <c r="AE24" s="74"/>
+      <c r="AF24" s="74"/>
+      <c r="AG24" s="74"/>
+      <c r="AH24" s="74"/>
+      <c r="AI24" s="74"/>
+      <c r="AJ24" s="74"/>
+      <c r="AK24" s="74"/>
+      <c r="AL24" s="74"/>
+      <c r="AM24" s="74"/>
+      <c r="AN24" s="90"/>
+      <c r="AO24" s="90"/>
+      <c r="AP24" s="74"/>
+      <c r="AQ24" s="74"/>
+      <c r="AR24" s="74"/>
+      <c r="AS24" s="74"/>
+      <c r="AT24" s="90"/>
+      <c r="AU24" s="90"/>
+      <c r="AV24" s="74"/>
+      <c r="AW24" s="74"/>
+      <c r="AX24" s="74"/>
+      <c r="AY24" s="90"/>
+      <c r="AZ24" s="90"/>
+      <c r="BA24" s="74"/>
+      <c r="BB24" s="74"/>
+      <c r="BC24" s="74"/>
+      <c r="BD24" s="74"/>
+      <c r="BE24" s="74"/>
+      <c r="BF24" s="74"/>
+      <c r="BG24" s="74"/>
+      <c r="BH24" s="74"/>
+      <c r="BI24" s="74"/>
+      <c r="BJ24" s="94"/>
+      <c r="BK24" s="96"/>
+      <c r="BL24" s="88"/>
       <c r="BM24" s="34"/>
-      <c r="BN24" s="83"/>
-      <c r="BO24" s="83"/>
-      <c r="BP24" s="83"/>
-      <c r="BQ24" s="83"/>
-      <c r="BR24" s="84"/>
-      <c r="BS24" s="83"/>
-      <c r="BT24" s="94"/>
-      <c r="BU24" s="94"/>
+      <c r="BN24" s="74"/>
+      <c r="BO24" s="74"/>
+      <c r="BP24" s="74"/>
+      <c r="BQ24" s="74"/>
+      <c r="BR24" s="78"/>
+      <c r="BS24" s="74"/>
+      <c r="BT24" s="97"/>
+      <c r="BU24" s="97"/>
     </row>
     <row r="25" spans="1:73" s="29" customFormat="1">
-      <c r="A25" s="83"/>
-      <c r="B25" s="83"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="83"/>
-      <c r="H25" s="83"/>
-      <c r="I25" s="83"/>
-      <c r="J25" s="83"/>
-      <c r="K25" s="83"/>
-      <c r="L25" s="83"/>
-      <c r="M25" s="83"/>
-      <c r="N25" s="83"/>
-      <c r="O25" s="83"/>
-      <c r="P25" s="83"/>
-      <c r="Q25" s="83"/>
-      <c r="R25" s="83"/>
-      <c r="S25" s="83"/>
-      <c r="T25" s="83"/>
-      <c r="U25" s="83"/>
-      <c r="V25" s="89"/>
-      <c r="W25" s="89"/>
-      <c r="X25" s="83"/>
-      <c r="Y25" s="89"/>
-      <c r="Z25" s="89"/>
-      <c r="AA25" s="83"/>
-      <c r="AB25" s="99"/>
-      <c r="AC25" s="83"/>
-      <c r="AD25" s="83"/>
-      <c r="AE25" s="83"/>
-      <c r="AF25" s="83"/>
-      <c r="AG25" s="83"/>
-      <c r="AH25" s="83"/>
-      <c r="AI25" s="83"/>
-      <c r="AJ25" s="83"/>
-      <c r="AK25" s="83"/>
-      <c r="AL25" s="83"/>
-      <c r="AM25" s="83"/>
-      <c r="AN25" s="89"/>
-      <c r="AO25" s="89"/>
-      <c r="AP25" s="83"/>
-      <c r="AQ25" s="83"/>
-      <c r="AR25" s="83"/>
-      <c r="AS25" s="83"/>
-      <c r="AT25" s="89"/>
-      <c r="AU25" s="89"/>
-      <c r="AV25" s="83"/>
-      <c r="AW25" s="83"/>
-      <c r="AX25" s="83"/>
-      <c r="AY25" s="89"/>
-      <c r="AZ25" s="89"/>
-      <c r="BA25" s="83"/>
-      <c r="BB25" s="83"/>
-      <c r="BC25" s="83"/>
-      <c r="BD25" s="83"/>
-      <c r="BE25" s="83"/>
-      <c r="BF25" s="83"/>
-      <c r="BG25" s="83"/>
-      <c r="BH25" s="83"/>
-      <c r="BI25" s="83"/>
-      <c r="BJ25" s="95"/>
-      <c r="BK25" s="97"/>
-      <c r="BL25" s="92"/>
+      <c r="A25" s="74"/>
+      <c r="B25" s="74"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="74"/>
+      <c r="K25" s="74"/>
+      <c r="L25" s="74"/>
+      <c r="M25" s="74"/>
+      <c r="N25" s="74"/>
+      <c r="O25" s="74"/>
+      <c r="P25" s="74"/>
+      <c r="Q25" s="74"/>
+      <c r="R25" s="74"/>
+      <c r="S25" s="74"/>
+      <c r="T25" s="74"/>
+      <c r="U25" s="74"/>
+      <c r="V25" s="90"/>
+      <c r="W25" s="90"/>
+      <c r="X25" s="74"/>
+      <c r="Y25" s="90"/>
+      <c r="Z25" s="90"/>
+      <c r="AA25" s="74"/>
+      <c r="AB25" s="92"/>
+      <c r="AC25" s="74"/>
+      <c r="AD25" s="74"/>
+      <c r="AE25" s="74"/>
+      <c r="AF25" s="74"/>
+      <c r="AG25" s="74"/>
+      <c r="AH25" s="74"/>
+      <c r="AI25" s="74"/>
+      <c r="AJ25" s="74"/>
+      <c r="AK25" s="74"/>
+      <c r="AL25" s="74"/>
+      <c r="AM25" s="74"/>
+      <c r="AN25" s="90"/>
+      <c r="AO25" s="90"/>
+      <c r="AP25" s="74"/>
+      <c r="AQ25" s="74"/>
+      <c r="AR25" s="74"/>
+      <c r="AS25" s="74"/>
+      <c r="AT25" s="90"/>
+      <c r="AU25" s="90"/>
+      <c r="AV25" s="74"/>
+      <c r="AW25" s="74"/>
+      <c r="AX25" s="74"/>
+      <c r="AY25" s="90"/>
+      <c r="AZ25" s="90"/>
+      <c r="BA25" s="74"/>
+      <c r="BB25" s="74"/>
+      <c r="BC25" s="74"/>
+      <c r="BD25" s="74"/>
+      <c r="BE25" s="74"/>
+      <c r="BF25" s="74"/>
+      <c r="BG25" s="74"/>
+      <c r="BH25" s="74"/>
+      <c r="BI25" s="74"/>
+      <c r="BJ25" s="94"/>
+      <c r="BK25" s="96"/>
+      <c r="BL25" s="88"/>
       <c r="BM25" s="34"/>
-      <c r="BN25" s="83"/>
-      <c r="BO25" s="83"/>
-      <c r="BP25" s="83"/>
-      <c r="BQ25" s="83"/>
-      <c r="BR25" s="84"/>
-      <c r="BS25" s="83"/>
-      <c r="BT25" s="94"/>
-      <c r="BU25" s="94"/>
+      <c r="BN25" s="74"/>
+      <c r="BO25" s="74"/>
+      <c r="BP25" s="74"/>
+      <c r="BQ25" s="74"/>
+      <c r="BR25" s="78"/>
+      <c r="BS25" s="74"/>
+      <c r="BT25" s="97"/>
+      <c r="BU25" s="97"/>
     </row>
     <row r="26" spans="1:73" ht="11.25" customHeight="1">
       <c r="E26" s="1"/>
@@ -16638,7 +16636,7 @@
       <c r="BF26" s="1"/>
       <c r="BI26" s="6"/>
       <c r="BJ26" s="12"/>
-      <c r="BL26" s="92" t="s">
+      <c r="BL26" s="88" t="s">
         <v>820</v>
       </c>
       <c r="BN26" s="1"/>
@@ -16662,10 +16660,10 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
       <c r="X27" s="6"/>
-      <c r="Y27" s="90" t="s">
+      <c r="Y27" s="37" t="s">
         <v>823</v>
       </c>
-      <c r="Z27" s="91" t="s">
+      <c r="Z27" s="74" t="s">
         <v>824</v>
       </c>
       <c r="AA27" s="1"/>
@@ -16675,27 +16673,27 @@
       <c r="AI27" s="12"/>
       <c r="AJ27" s="1"/>
       <c r="AM27" s="12"/>
-      <c r="AN27" s="90" t="s">
+      <c r="AN27" s="98" t="s">
         <v>823</v>
       </c>
-      <c r="AO27" s="91" t="s">
+      <c r="AO27" s="99" t="s">
         <v>824</v>
       </c>
       <c r="AR27" s="1"/>
       <c r="AS27" s="1"/>
-      <c r="AT27" s="90" t="s">
+      <c r="AT27" s="98" t="s">
         <v>823</v>
       </c>
-      <c r="AU27" s="91" t="s">
+      <c r="AU27" s="99" t="s">
         <v>824</v>
       </c>
       <c r="AV27" s="12"/>
       <c r="AW27" s="12"/>
       <c r="AX27" s="12"/>
-      <c r="AY27" s="90" t="s">
+      <c r="AY27" s="98" t="s">
         <v>823</v>
       </c>
-      <c r="AZ27" s="91" t="s">
+      <c r="AZ27" s="99" t="s">
         <v>824</v>
       </c>
       <c r="BA27" s="6"/>
@@ -16708,7 +16706,7 @@
       <c r="BJ27" s="12" t="s">
         <v>829</v>
       </c>
-      <c r="BL27" s="92"/>
+      <c r="BL27" s="88"/>
       <c r="BN27" s="1"/>
       <c r="BO27" s="4"/>
       <c r="BP27" s="6"/>
@@ -16730,8 +16728,8 @@
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
       <c r="X28" s="6"/>
-      <c r="Y28" s="90"/>
-      <c r="Z28" s="91"/>
+      <c r="Y28" s="37"/>
+      <c r="Z28" s="74"/>
       <c r="AD28" s="1"/>
       <c r="AG28" s="12"/>
       <c r="AH28" s="12"/>
@@ -16739,17 +16737,17 @@
       <c r="AJ28" s="1"/>
       <c r="AL28" s="1"/>
       <c r="AM28" s="6"/>
-      <c r="AN28" s="90"/>
-      <c r="AO28" s="91"/>
+      <c r="AN28" s="98"/>
+      <c r="AO28" s="99"/>
       <c r="AR28" s="1"/>
       <c r="AS28" s="6"/>
-      <c r="AT28" s="90"/>
-      <c r="AU28" s="91"/>
+      <c r="AT28" s="98"/>
+      <c r="AU28" s="99"/>
       <c r="AV28" s="12"/>
       <c r="AW28" s="12"/>
       <c r="AX28" s="12"/>
-      <c r="AY28" s="90"/>
-      <c r="AZ28" s="91"/>
+      <c r="AY28" s="98"/>
+      <c r="AZ28" s="99"/>
       <c r="BA28" s="6"/>
       <c r="BB28" s="6"/>
       <c r="BC28" s="24" t="s">
@@ -16758,7 +16756,7 @@
       <c r="BF28" s="1"/>
       <c r="BI28" s="6"/>
       <c r="BJ28" s="12"/>
-      <c r="BL28" s="92"/>
+      <c r="BL28" s="88"/>
       <c r="BN28" s="1"/>
       <c r="BO28" s="4"/>
       <c r="BP28" s="6"/>
@@ -16799,7 +16797,7 @@
       <c r="BF29" s="1"/>
       <c r="BI29" s="6"/>
       <c r="BJ29" s="12"/>
-      <c r="BL29" s="92" t="s">
+      <c r="BL29" s="88" t="s">
         <v>821</v>
       </c>
       <c r="BN29" s="1"/>
@@ -16842,7 +16840,7 @@
       <c r="BF30" s="1"/>
       <c r="BI30" s="6"/>
       <c r="BJ30" s="12"/>
-      <c r="BL30" s="92"/>
+      <c r="BL30" s="88"/>
       <c r="BN30" s="1"/>
       <c r="BO30" s="4"/>
       <c r="BP30" s="6"/>
@@ -16883,7 +16881,7 @@
       <c r="BF31" s="1"/>
       <c r="BI31" s="6"/>
       <c r="BJ31" s="12"/>
-      <c r="BL31" s="92"/>
+      <c r="BL31" s="88"/>
       <c r="BN31" s="1"/>
       <c r="BO31" s="4"/>
       <c r="BP31" s="6"/>
@@ -16924,7 +16922,7 @@
       <c r="BF32" s="1"/>
       <c r="BI32" s="6"/>
       <c r="BJ32" s="12"/>
-      <c r="BL32" s="92"/>
+      <c r="BL32" s="88"/>
       <c r="BN32" s="1"/>
       <c r="BO32" s="4"/>
       <c r="BP32" s="6"/>
@@ -17617,33 +17615,47 @@
     </row>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="BL21:BL25"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="BQ18:BQ20"/>
-    <mergeCell ref="BQ21:BQ25"/>
-    <mergeCell ref="BR18:BR20"/>
-    <mergeCell ref="BR21:BR25"/>
-    <mergeCell ref="BP21:BP25"/>
-    <mergeCell ref="BO21:BO25"/>
-    <mergeCell ref="BN21:BN25"/>
-    <mergeCell ref="BN18:BN20"/>
-    <mergeCell ref="BO18:BO20"/>
-    <mergeCell ref="BP18:BP20"/>
-    <mergeCell ref="X21:X25"/>
-    <mergeCell ref="AY21:AY25"/>
-    <mergeCell ref="AZ21:AZ25"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="W21:W25"/>
-    <mergeCell ref="AF21:AF25"/>
-    <mergeCell ref="AG21:AG25"/>
-    <mergeCell ref="AC21:AC25"/>
-    <mergeCell ref="AD21:AD25"/>
-    <mergeCell ref="AB21:AB25"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="L21:L25"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="F21:F25"/>
+    <mergeCell ref="AN21:AN25"/>
+    <mergeCell ref="AO21:AO25"/>
+    <mergeCell ref="AN27:AN28"/>
+    <mergeCell ref="AO27:AO28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="Z27:Z28"/>
+    <mergeCell ref="AY27:AY28"/>
+    <mergeCell ref="AZ27:AZ28"/>
+    <mergeCell ref="AT21:AT25"/>
+    <mergeCell ref="AH21:AH25"/>
+    <mergeCell ref="AI21:AI25"/>
+    <mergeCell ref="AM21:AM25"/>
+    <mergeCell ref="AS21:AS25"/>
+    <mergeCell ref="AE21:AE25"/>
+    <mergeCell ref="AR21:AR25"/>
+    <mergeCell ref="AL21:AL25"/>
+    <mergeCell ref="AX21:AX25"/>
+    <mergeCell ref="AU21:AU25"/>
+    <mergeCell ref="AT27:AT28"/>
+    <mergeCell ref="AU27:AU28"/>
+    <mergeCell ref="BL26:BL28"/>
+    <mergeCell ref="BL29:BL33"/>
+    <mergeCell ref="BT18:BU25"/>
+    <mergeCell ref="B18:BM20"/>
+    <mergeCell ref="S21:S25"/>
+    <mergeCell ref="T21:T25"/>
+    <mergeCell ref="U21:U25"/>
+    <mergeCell ref="BC21:BC25"/>
+    <mergeCell ref="BD21:BD25"/>
+    <mergeCell ref="Y21:Y25"/>
+    <mergeCell ref="AJ21:AJ25"/>
+    <mergeCell ref="AK21:AK25"/>
+    <mergeCell ref="AP21:AP25"/>
+    <mergeCell ref="AQ21:AQ25"/>
+    <mergeCell ref="AV21:AV25"/>
+    <mergeCell ref="AW21:AW25"/>
+    <mergeCell ref="O21:O25"/>
+    <mergeCell ref="P21:P25"/>
+    <mergeCell ref="N21:N25"/>
+    <mergeCell ref="Q21:Q25"/>
+    <mergeCell ref="R21:R25"/>
     <mergeCell ref="BS21:BS25"/>
     <mergeCell ref="C21:C25"/>
     <mergeCell ref="D21:D25"/>
@@ -17660,52 +17672,38 @@
     <mergeCell ref="BH21:BH25"/>
     <mergeCell ref="M21:M25"/>
     <mergeCell ref="E21:E25"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="W21:W25"/>
+    <mergeCell ref="AF21:AF25"/>
+    <mergeCell ref="AG21:AG25"/>
+    <mergeCell ref="AC21:AC25"/>
+    <mergeCell ref="AD21:AD25"/>
+    <mergeCell ref="AB21:AB25"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="L21:L25"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="F21:F25"/>
     <mergeCell ref="G21:G25"/>
     <mergeCell ref="H21:H25"/>
     <mergeCell ref="I21:I25"/>
     <mergeCell ref="J21:J25"/>
+    <mergeCell ref="BL21:BL25"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="BQ18:BQ20"/>
+    <mergeCell ref="BQ21:BQ25"/>
+    <mergeCell ref="BR18:BR20"/>
+    <mergeCell ref="BR21:BR25"/>
+    <mergeCell ref="BP21:BP25"/>
+    <mergeCell ref="BO21:BO25"/>
+    <mergeCell ref="BN21:BN25"/>
+    <mergeCell ref="BN18:BN20"/>
+    <mergeCell ref="BO18:BO20"/>
+    <mergeCell ref="BP18:BP20"/>
+    <mergeCell ref="X21:X25"/>
+    <mergeCell ref="AY21:AY25"/>
+    <mergeCell ref="AZ21:AZ25"/>
     <mergeCell ref="K21:K25"/>
-    <mergeCell ref="O21:O25"/>
-    <mergeCell ref="P21:P25"/>
-    <mergeCell ref="N21:N25"/>
-    <mergeCell ref="Q21:Q25"/>
-    <mergeCell ref="R21:R25"/>
-    <mergeCell ref="BL26:BL28"/>
-    <mergeCell ref="BL29:BL33"/>
-    <mergeCell ref="BT18:BU25"/>
-    <mergeCell ref="B18:BM20"/>
-    <mergeCell ref="S21:S25"/>
-    <mergeCell ref="T21:T25"/>
-    <mergeCell ref="U21:U25"/>
-    <mergeCell ref="BC21:BC25"/>
-    <mergeCell ref="BD21:BD25"/>
-    <mergeCell ref="Y21:Y25"/>
-    <mergeCell ref="AJ21:AJ25"/>
-    <mergeCell ref="AK21:AK25"/>
-    <mergeCell ref="AP21:AP25"/>
-    <mergeCell ref="AQ21:AQ25"/>
-    <mergeCell ref="AV21:AV25"/>
-    <mergeCell ref="AW21:AW25"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="Z27:Z28"/>
-    <mergeCell ref="AY27:AY28"/>
-    <mergeCell ref="AZ27:AZ28"/>
-    <mergeCell ref="AT21:AT25"/>
-    <mergeCell ref="AH21:AH25"/>
-    <mergeCell ref="AI21:AI25"/>
-    <mergeCell ref="AM21:AM25"/>
-    <mergeCell ref="AS21:AS25"/>
-    <mergeCell ref="AE21:AE25"/>
-    <mergeCell ref="AR21:AR25"/>
-    <mergeCell ref="AL21:AL25"/>
-    <mergeCell ref="AX21:AX25"/>
-    <mergeCell ref="AU21:AU25"/>
-    <mergeCell ref="AT27:AT28"/>
-    <mergeCell ref="AU27:AU28"/>
-    <mergeCell ref="AN21:AN25"/>
-    <mergeCell ref="AO21:AO25"/>
-    <mergeCell ref="AN27:AN28"/>
-    <mergeCell ref="AO27:AO28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -17720,14 +17718,14 @@
   <dimension ref="A1:BW31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:D24"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="28.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="29.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="36.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="43.85546875" style="6" customWidth="1"/>
     <col min="6" max="6" width="41.5703125" style="1" customWidth="1"/>
@@ -17806,10 +17804,10 @@
       <c r="BW1" s="1"/>
     </row>
     <row r="2" spans="1:75" ht="21">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="40"/>
+      <c r="B2" s="56"/>
       <c r="C2" s="17" t="s">
         <v>830</v>
       </c>
@@ -17818,12 +17816,12 @@
       <c r="BW2" s="1"/>
     </row>
     <row r="3" spans="1:75" ht="21">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="41"/>
+      <c r="B3" s="57"/>
       <c r="C3" s="17" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="BV3" s="1"/>
       <c r="BW3" s="1"/>
@@ -17931,7 +17929,7 @@
       <c r="BF6" s="1"/>
       <c r="BI6" s="6"/>
       <c r="BJ6" s="12"/>
-      <c r="BL6" s="92" t="s">
+      <c r="BL6" s="88" t="s">
         <v>821</v>
       </c>
       <c r="BN6" s="1"/>
@@ -17991,7 +17989,7 @@
       <c r="BF7" s="1"/>
       <c r="BI7" s="6"/>
       <c r="BJ7" s="12"/>
-      <c r="BL7" s="92"/>
+      <c r="BL7" s="88"/>
       <c r="BN7" s="1"/>
       <c r="BO7" s="4"/>
       <c r="BP7" s="6"/>
@@ -18049,7 +18047,7 @@
       <c r="BF8" s="1"/>
       <c r="BI8" s="6"/>
       <c r="BJ8" s="12"/>
-      <c r="BL8" s="92"/>
+      <c r="BL8" s="88"/>
       <c r="BN8" s="1"/>
       <c r="BO8" s="4"/>
       <c r="BP8" s="6"/>
@@ -18107,7 +18105,7 @@
       <c r="BF9" s="1"/>
       <c r="BI9" s="6"/>
       <c r="BJ9" s="12"/>
-      <c r="BL9" s="92"/>
+      <c r="BL9" s="88"/>
       <c r="BN9" s="1"/>
       <c r="BO9" s="4"/>
       <c r="BP9" s="6"/>
@@ -18369,19 +18367,19 @@
       <c r="BW14" s="6"/>
     </row>
     <row r="15" spans="1:75" s="1" customFormat="1">
-      <c r="A15" s="100" t="s">
-        <v>859</v>
-      </c>
-      <c r="B15" s="101"/>
-      <c r="C15" s="102"/>
+      <c r="A15" s="101" t="s">
+        <v>858</v>
+      </c>
+      <c r="B15" s="102"/>
+      <c r="C15" s="103"/>
       <c r="D15" s="70" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="E15" s="70" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F15" s="70" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
@@ -18420,9 +18418,9 @@
       <c r="BW15" s="6"/>
     </row>
     <row r="16" spans="1:75" s="1" customFormat="1">
-      <c r="A16" s="103"/>
-      <c r="B16" s="104"/>
-      <c r="C16" s="105"/>
+      <c r="A16" s="104"/>
+      <c r="B16" s="105"/>
+      <c r="C16" s="106"/>
       <c r="D16" s="70"/>
       <c r="E16" s="70"/>
       <c r="F16" s="70"/>
@@ -18463,9 +18461,9 @@
       <c r="BW16" s="6"/>
     </row>
     <row r="17" spans="1:75" s="1" customFormat="1">
-      <c r="A17" s="106"/>
-      <c r="B17" s="107"/>
-      <c r="C17" s="108"/>
+      <c r="A17" s="107"/>
+      <c r="B17" s="108"/>
+      <c r="C17" s="109"/>
       <c r="D17" s="70"/>
       <c r="E17" s="70"/>
       <c r="F17" s="70"/>
@@ -18504,23 +18502,23 @@
       <c r="BW17" s="6"/>
     </row>
     <row r="18" spans="1:75" s="1" customFormat="1">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="37" t="s">
         <v>850</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="37" t="s">
         <v>857</v>
       </c>
-      <c r="C18" s="38" t="s">
-        <v>858</v>
-      </c>
-      <c r="D18" s="38" t="s">
-        <v>860</v>
-      </c>
-      <c r="E18" s="38" t="s">
-        <v>862</v>
-      </c>
-      <c r="F18" s="38" t="s">
-        <v>864</v>
+      <c r="C18" s="37" t="s">
+        <v>866</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>859</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>861</v>
+      </c>
+      <c r="F18" s="37" t="s">
+        <v>863</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -18557,12 +18555,12 @@
       <c r="BW18" s="6"/>
     </row>
     <row r="19" spans="1:75" s="1" customFormat="1">
-      <c r="A19" s="38"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -18598,12 +18596,12 @@
       <c r="BW19" s="6"/>
     </row>
     <row r="20" spans="1:75" s="1" customFormat="1">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -18639,12 +18637,12 @@
       <c r="BW20" s="6"/>
     </row>
     <row r="21" spans="1:75" s="1" customFormat="1">
-      <c r="A21" s="38"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -18752,12 +18750,12 @@
       <c r="BW23" s="6"/>
     </row>
     <row r="24" spans="1:75" s="1" customFormat="1">
-      <c r="A24" s="109" t="s">
-        <v>866</v>
-      </c>
-      <c r="B24" s="109"/>
-      <c r="C24" s="109"/>
-      <c r="D24" s="109"/>
+      <c r="A24" s="100" t="s">
+        <v>865</v>
+      </c>
+      <c r="B24" s="100"/>
+      <c r="C24" s="100"/>
+      <c r="D24" s="100"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>

</xml_diff>

<commit_message>
Mapeamento Conferência LN - NFR
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_NFR.xlsx
+++ b/Documentação/Planilhas/Conferencia_NFR.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2586" uniqueCount="868">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2586" uniqueCount="867">
   <si>
     <t>1</t>
   </si>
@@ -2831,9 +2831,6 @@
   </si>
   <si>
     <t>Na lupinha, informar o Cód Item limpando todos os campos primeiramente. Pedir o detalhamento da última data apresentada. Na aba inferior "Detalhes de Custos", pegar o valor da coluna da coluna MAUC [BRL]</t>
-  </si>
-  <si>
-    <t>86.9800</t>
   </si>
   <si>
     <t>66.6600</t>
@@ -3165,7 +3162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3259,9 +3256,6 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3269,61 +3263,13 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3359,10 +3305,58 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3378,21 +3372,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3422,7 +3401,25 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3431,10 +3428,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3443,10 +3437,10 @@
     <xf numFmtId="49" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3839,19 +3833,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:43" ht="21">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="56"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="17" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:43" ht="21">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="57"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="17" t="s">
         <v>245</v>
       </c>
@@ -5306,148 +5300,148 @@
       <c r="AO18" s="4"/>
     </row>
     <row r="19" spans="1:43" ht="11.25" customHeight="1">
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="41" t="s">
         <v>196</v>
       </c>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="N19" s="59"/>
-      <c r="O19" s="59"/>
-      <c r="P19" s="59"/>
-      <c r="Q19" s="59"/>
-      <c r="R19" s="59"/>
-      <c r="S19" s="59"/>
-      <c r="T19" s="59"/>
-      <c r="U19" s="59"/>
-      <c r="V19" s="59"/>
-      <c r="W19" s="59"/>
-      <c r="X19" s="59"/>
-      <c r="Y19" s="59"/>
-      <c r="Z19" s="59"/>
-      <c r="AA19" s="60"/>
-      <c r="AB19" s="47" t="s">
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="42"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="42"/>
+      <c r="S19" s="42"/>
+      <c r="T19" s="42"/>
+      <c r="U19" s="42"/>
+      <c r="V19" s="42"/>
+      <c r="W19" s="42"/>
+      <c r="X19" s="42"/>
+      <c r="Y19" s="42"/>
+      <c r="Z19" s="42"/>
+      <c r="AA19" s="43"/>
+      <c r="AB19" s="50" t="s">
         <v>243</v>
       </c>
-      <c r="AC19" s="48"/>
-      <c r="AD19" s="48"/>
-      <c r="AE19" s="48"/>
-      <c r="AF19" s="48"/>
-      <c r="AG19" s="48"/>
-      <c r="AH19" s="49"/>
-      <c r="AI19" s="44" t="s">
+      <c r="AC19" s="51"/>
+      <c r="AD19" s="51"/>
+      <c r="AE19" s="51"/>
+      <c r="AF19" s="51"/>
+      <c r="AG19" s="51"/>
+      <c r="AH19" s="52"/>
+      <c r="AI19" s="65" t="s">
         <v>238</v>
       </c>
-      <c r="AJ19" s="47" t="s">
+      <c r="AJ19" s="50" t="s">
         <v>239</v>
       </c>
-      <c r="AK19" s="48"/>
-      <c r="AL19" s="48"/>
-      <c r="AM19" s="48"/>
-      <c r="AN19" s="48"/>
-      <c r="AO19" s="49"/>
-      <c r="AP19" s="41" t="s">
+      <c r="AK19" s="51"/>
+      <c r="AL19" s="51"/>
+      <c r="AM19" s="51"/>
+      <c r="AN19" s="51"/>
+      <c r="AO19" s="52"/>
+      <c r="AP19" s="62" t="s">
         <v>240</v>
       </c>
-      <c r="AQ19" s="44" t="s">
+      <c r="AQ19" s="65" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:43" ht="11.25" customHeight="1">
-      <c r="B20" s="61"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="62"/>
-      <c r="M20" s="62"/>
-      <c r="N20" s="62"/>
-      <c r="O20" s="62"/>
-      <c r="P20" s="62"/>
-      <c r="Q20" s="62"/>
-      <c r="R20" s="62"/>
-      <c r="S20" s="62"/>
-      <c r="T20" s="62"/>
-      <c r="U20" s="62"/>
-      <c r="V20" s="62"/>
-      <c r="W20" s="62"/>
-      <c r="X20" s="62"/>
-      <c r="Y20" s="62"/>
-      <c r="Z20" s="62"/>
-      <c r="AA20" s="63"/>
-      <c r="AB20" s="50"/>
-      <c r="AC20" s="51"/>
-      <c r="AD20" s="51"/>
-      <c r="AE20" s="51"/>
-      <c r="AF20" s="51"/>
-      <c r="AG20" s="51"/>
-      <c r="AH20" s="52"/>
-      <c r="AI20" s="45"/>
-      <c r="AJ20" s="50"/>
-      <c r="AK20" s="51"/>
-      <c r="AL20" s="51"/>
-      <c r="AM20" s="51"/>
-      <c r="AN20" s="51"/>
-      <c r="AO20" s="52"/>
-      <c r="AP20" s="42"/>
-      <c r="AQ20" s="45"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="45"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="45"/>
+      <c r="P20" s="45"/>
+      <c r="Q20" s="45"/>
+      <c r="R20" s="45"/>
+      <c r="S20" s="45"/>
+      <c r="T20" s="45"/>
+      <c r="U20" s="45"/>
+      <c r="V20" s="45"/>
+      <c r="W20" s="45"/>
+      <c r="X20" s="45"/>
+      <c r="Y20" s="45"/>
+      <c r="Z20" s="45"/>
+      <c r="AA20" s="46"/>
+      <c r="AB20" s="53"/>
+      <c r="AC20" s="54"/>
+      <c r="AD20" s="54"/>
+      <c r="AE20" s="54"/>
+      <c r="AF20" s="54"/>
+      <c r="AG20" s="54"/>
+      <c r="AH20" s="55"/>
+      <c r="AI20" s="66"/>
+      <c r="AJ20" s="53"/>
+      <c r="AK20" s="54"/>
+      <c r="AL20" s="54"/>
+      <c r="AM20" s="54"/>
+      <c r="AN20" s="54"/>
+      <c r="AO20" s="55"/>
+      <c r="AP20" s="63"/>
+      <c r="AQ20" s="66"/>
     </row>
     <row r="21" spans="1:43" ht="11.25" customHeight="1">
-      <c r="B21" s="64"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="65"/>
-      <c r="K21" s="65"/>
-      <c r="L21" s="65"/>
-      <c r="M21" s="65"/>
-      <c r="N21" s="65"/>
-      <c r="O21" s="65"/>
-      <c r="P21" s="65"/>
-      <c r="Q21" s="65"/>
-      <c r="R21" s="65"/>
-      <c r="S21" s="65"/>
-      <c r="T21" s="65"/>
-      <c r="U21" s="65"/>
-      <c r="V21" s="65"/>
-      <c r="W21" s="65"/>
-      <c r="X21" s="65"/>
-      <c r="Y21" s="65"/>
-      <c r="Z21" s="65"/>
-      <c r="AA21" s="66"/>
-      <c r="AB21" s="53"/>
-      <c r="AC21" s="54"/>
-      <c r="AD21" s="54"/>
-      <c r="AE21" s="54"/>
-      <c r="AF21" s="54"/>
-      <c r="AG21" s="54"/>
-      <c r="AH21" s="55"/>
-      <c r="AI21" s="46"/>
-      <c r="AJ21" s="53"/>
-      <c r="AK21" s="54"/>
-      <c r="AL21" s="54"/>
-      <c r="AM21" s="54"/>
-      <c r="AN21" s="54"/>
-      <c r="AO21" s="55"/>
-      <c r="AP21" s="43"/>
-      <c r="AQ21" s="46"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
+      <c r="P21" s="48"/>
+      <c r="Q21" s="48"/>
+      <c r="R21" s="48"/>
+      <c r="S21" s="48"/>
+      <c r="T21" s="48"/>
+      <c r="U21" s="48"/>
+      <c r="V21" s="48"/>
+      <c r="W21" s="48"/>
+      <c r="X21" s="48"/>
+      <c r="Y21" s="48"/>
+      <c r="Z21" s="48"/>
+      <c r="AA21" s="49"/>
+      <c r="AB21" s="56"/>
+      <c r="AC21" s="57"/>
+      <c r="AD21" s="57"/>
+      <c r="AE21" s="57"/>
+      <c r="AF21" s="57"/>
+      <c r="AG21" s="57"/>
+      <c r="AH21" s="58"/>
+      <c r="AI21" s="67"/>
+      <c r="AJ21" s="56"/>
+      <c r="AK21" s="57"/>
+      <c r="AL21" s="57"/>
+      <c r="AM21" s="57"/>
+      <c r="AN21" s="57"/>
+      <c r="AO21" s="58"/>
+      <c r="AP21" s="64"/>
+      <c r="AQ21" s="67"/>
     </row>
     <row r="22" spans="1:43" ht="11.25" customHeight="1">
       <c r="A22" s="37" t="s">
@@ -5489,7 +5483,7 @@
       <c r="M22" s="37" t="s">
         <v>205</v>
       </c>
-      <c r="N22" s="67" t="s">
+      <c r="N22" s="36" t="s">
         <v>211</v>
       </c>
       <c r="O22" s="37" t="s">
@@ -5576,7 +5570,7 @@
       <c r="AP22" s="37" t="s">
         <v>236</v>
       </c>
-      <c r="AQ22" s="38" t="s">
+      <c r="AQ22" s="59" t="s">
         <v>229</v>
       </c>
     </row>
@@ -5594,7 +5588,7 @@
       <c r="K23" s="37"/>
       <c r="L23" s="37"/>
       <c r="M23" s="37"/>
-      <c r="N23" s="67"/>
+      <c r="N23" s="36"/>
       <c r="O23" s="37"/>
       <c r="P23" s="37"/>
       <c r="Q23" s="37"/>
@@ -5623,7 +5617,7 @@
       <c r="AN23" s="37"/>
       <c r="AO23" s="37"/>
       <c r="AP23" s="37"/>
-      <c r="AQ23" s="39"/>
+      <c r="AQ23" s="60"/>
     </row>
     <row r="24" spans="1:43">
       <c r="A24" s="37"/>
@@ -5639,7 +5633,7 @@
       <c r="K24" s="37"/>
       <c r="L24" s="37"/>
       <c r="M24" s="37"/>
-      <c r="N24" s="67"/>
+      <c r="N24" s="36"/>
       <c r="O24" s="37"/>
       <c r="P24" s="37"/>
       <c r="Q24" s="37"/>
@@ -5668,7 +5662,7 @@
       <c r="AN24" s="37"/>
       <c r="AO24" s="37"/>
       <c r="AP24" s="37"/>
-      <c r="AQ24" s="39"/>
+      <c r="AQ24" s="60"/>
     </row>
     <row r="25" spans="1:43">
       <c r="A25" s="37"/>
@@ -5684,7 +5678,7 @@
       <c r="K25" s="37"/>
       <c r="L25" s="37"/>
       <c r="M25" s="37"/>
-      <c r="N25" s="67"/>
+      <c r="N25" s="36"/>
       <c r="O25" s="37"/>
       <c r="P25" s="37"/>
       <c r="Q25" s="37"/>
@@ -5713,7 +5707,7 @@
       <c r="AN25" s="37"/>
       <c r="AO25" s="37"/>
       <c r="AP25" s="37"/>
-      <c r="AQ25" s="39"/>
+      <c r="AQ25" s="60"/>
     </row>
     <row r="26" spans="1:43">
       <c r="A26" s="37"/>
@@ -5729,7 +5723,7 @@
       <c r="K26" s="37"/>
       <c r="L26" s="37"/>
       <c r="M26" s="37"/>
-      <c r="N26" s="67"/>
+      <c r="N26" s="36"/>
       <c r="O26" s="37"/>
       <c r="P26" s="37"/>
       <c r="Q26" s="37"/>
@@ -5758,7 +5752,7 @@
       <c r="AN26" s="37"/>
       <c r="AO26" s="37"/>
       <c r="AP26" s="37"/>
-      <c r="AQ26" s="39"/>
+      <c r="AQ26" s="60"/>
     </row>
     <row r="27" spans="1:43">
       <c r="A27" s="37"/>
@@ -5774,7 +5768,7 @@
       <c r="K27" s="37"/>
       <c r="L27" s="37"/>
       <c r="M27" s="37"/>
-      <c r="N27" s="67"/>
+      <c r="N27" s="36"/>
       <c r="O27" s="37"/>
       <c r="P27" s="37"/>
       <c r="Q27" s="37"/>
@@ -5803,38 +5797,54 @@
       <c r="AN27" s="37"/>
       <c r="AO27" s="37"/>
       <c r="AP27" s="37"/>
-      <c r="AQ27" s="40"/>
+      <c r="AQ27" s="61"/>
     </row>
     <row r="29" spans="1:43" ht="11.25" customHeight="1">
       <c r="I29" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="O29" s="68" t="s">
+      <c r="O29" s="38" t="s">
         <v>327</v>
       </c>
-      <c r="P29" s="68"/>
-      <c r="Q29" s="68"/>
+      <c r="P29" s="38"/>
+      <c r="Q29" s="38"/>
     </row>
     <row r="30" spans="1:43" ht="56.25">
       <c r="I30" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="O30" s="68"/>
-      <c r="P30" s="68"/>
-      <c r="Q30" s="68"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="N22:N27"/>
-    <mergeCell ref="K22:K27"/>
-    <mergeCell ref="O29:Q30"/>
-    <mergeCell ref="L22:L27"/>
-    <mergeCell ref="AJ22:AJ27"/>
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="D22:D27"/>
-    <mergeCell ref="E22:E27"/>
-    <mergeCell ref="F22:F27"/>
-    <mergeCell ref="J22:J27"/>
+    <mergeCell ref="AO22:AO27"/>
+    <mergeCell ref="AQ22:AQ27"/>
+    <mergeCell ref="AP22:AP27"/>
+    <mergeCell ref="AP19:AP21"/>
+    <mergeCell ref="AI19:AI21"/>
+    <mergeCell ref="AJ19:AO21"/>
+    <mergeCell ref="AQ19:AQ21"/>
+    <mergeCell ref="AI22:AI27"/>
+    <mergeCell ref="AN22:AN27"/>
+    <mergeCell ref="AM22:AM27"/>
+    <mergeCell ref="AK22:AK27"/>
+    <mergeCell ref="AL22:AL27"/>
+    <mergeCell ref="AB19:AH21"/>
+    <mergeCell ref="U22:U27"/>
+    <mergeCell ref="W22:W27"/>
+    <mergeCell ref="X22:X27"/>
+    <mergeCell ref="V22:V27"/>
+    <mergeCell ref="Y22:Y27"/>
+    <mergeCell ref="Z22:Z27"/>
+    <mergeCell ref="AE22:AE27"/>
+    <mergeCell ref="AC22:AC27"/>
+    <mergeCell ref="AB22:AB27"/>
+    <mergeCell ref="AD22:AD27"/>
+    <mergeCell ref="AA22:AA27"/>
+    <mergeCell ref="AH22:AH27"/>
+    <mergeCell ref="AG22:AG27"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="AF22:AF27"/>
@@ -5851,32 +5861,16 @@
     <mergeCell ref="S22:S27"/>
     <mergeCell ref="T22:T27"/>
     <mergeCell ref="H22:H27"/>
-    <mergeCell ref="AB19:AH21"/>
-    <mergeCell ref="U22:U27"/>
-    <mergeCell ref="W22:W27"/>
-    <mergeCell ref="X22:X27"/>
-    <mergeCell ref="V22:V27"/>
-    <mergeCell ref="Y22:Y27"/>
-    <mergeCell ref="Z22:Z27"/>
-    <mergeCell ref="AE22:AE27"/>
-    <mergeCell ref="AC22:AC27"/>
-    <mergeCell ref="AB22:AB27"/>
-    <mergeCell ref="AD22:AD27"/>
-    <mergeCell ref="AA22:AA27"/>
-    <mergeCell ref="AH22:AH27"/>
-    <mergeCell ref="AG22:AG27"/>
-    <mergeCell ref="AO22:AO27"/>
-    <mergeCell ref="AQ22:AQ27"/>
-    <mergeCell ref="AP22:AP27"/>
-    <mergeCell ref="AP19:AP21"/>
-    <mergeCell ref="AI19:AI21"/>
-    <mergeCell ref="AJ19:AO21"/>
-    <mergeCell ref="AQ19:AQ21"/>
-    <mergeCell ref="AI22:AI27"/>
-    <mergeCell ref="AN22:AN27"/>
-    <mergeCell ref="AM22:AM27"/>
-    <mergeCell ref="AK22:AK27"/>
-    <mergeCell ref="AL22:AL27"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="D22:D27"/>
+    <mergeCell ref="E22:E27"/>
+    <mergeCell ref="F22:F27"/>
+    <mergeCell ref="J22:J27"/>
+    <mergeCell ref="N22:N27"/>
+    <mergeCell ref="K22:K27"/>
+    <mergeCell ref="O29:Q30"/>
+    <mergeCell ref="L22:L27"/>
+    <mergeCell ref="AJ22:AJ27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5942,19 +5936,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="21">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="57"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="2" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="21">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="57"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="2" t="s">
         <v>333</v>
       </c>
@@ -6749,124 +6743,124 @@
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:23">
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="41" t="s">
         <v>331</v>
       </c>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="N19" s="59"/>
-      <c r="O19" s="59"/>
-      <c r="P19" s="60"/>
-      <c r="Q19" s="70" t="s">
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="42"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="69" t="s">
         <v>332</v>
       </c>
-      <c r="R19" s="70"/>
-      <c r="S19" s="70"/>
-      <c r="T19" s="70"/>
-      <c r="U19" s="70"/>
-      <c r="V19" s="70"/>
-      <c r="W19" s="44" t="s">
+      <c r="R19" s="69"/>
+      <c r="S19" s="69"/>
+      <c r="T19" s="69"/>
+      <c r="U19" s="69"/>
+      <c r="V19" s="69"/>
+      <c r="W19" s="65" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:23">
-      <c r="B20" s="61"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="62"/>
-      <c r="M20" s="62"/>
-      <c r="N20" s="62"/>
-      <c r="O20" s="62"/>
-      <c r="P20" s="63"/>
-      <c r="Q20" s="70"/>
-      <c r="R20" s="70"/>
-      <c r="S20" s="70"/>
-      <c r="T20" s="70"/>
-      <c r="U20" s="70"/>
-      <c r="V20" s="70"/>
-      <c r="W20" s="45"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="45"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="45"/>
+      <c r="P20" s="46"/>
+      <c r="Q20" s="69"/>
+      <c r="R20" s="69"/>
+      <c r="S20" s="69"/>
+      <c r="T20" s="69"/>
+      <c r="U20" s="69"/>
+      <c r="V20" s="69"/>
+      <c r="W20" s="66"/>
     </row>
     <row r="21" spans="1:23">
-      <c r="B21" s="64"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="65"/>
-      <c r="K21" s="65"/>
-      <c r="L21" s="65"/>
-      <c r="M21" s="65"/>
-      <c r="N21" s="65"/>
-      <c r="O21" s="65"/>
-      <c r="P21" s="66"/>
-      <c r="Q21" s="70"/>
-      <c r="R21" s="70"/>
-      <c r="S21" s="70"/>
-      <c r="T21" s="70"/>
-      <c r="U21" s="70"/>
-      <c r="V21" s="70"/>
-      <c r="W21" s="46"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
+      <c r="P21" s="49"/>
+      <c r="Q21" s="69"/>
+      <c r="R21" s="69"/>
+      <c r="S21" s="69"/>
+      <c r="T21" s="69"/>
+      <c r="U21" s="69"/>
+      <c r="V21" s="69"/>
+      <c r="W21" s="67"/>
     </row>
     <row r="22" spans="1:23" ht="11.25" customHeight="1">
       <c r="A22" s="6"/>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="61" t="s">
         <v>308</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="61" t="s">
         <v>309</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="61" t="s">
         <v>310</v>
       </c>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="61" t="s">
         <v>311</v>
       </c>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40" t="s">
+      <c r="F22" s="61"/>
+      <c r="G22" s="61" t="s">
         <v>312</v>
       </c>
-      <c r="H22" s="40" t="s">
+      <c r="H22" s="61" t="s">
         <v>313</v>
       </c>
-      <c r="I22" s="40" t="s">
+      <c r="I22" s="61" t="s">
         <v>314</v>
       </c>
       <c r="J22" s="8"/>
-      <c r="K22" s="40" t="s">
+      <c r="K22" s="61" t="s">
         <v>315</v>
       </c>
-      <c r="L22" s="40" t="s">
+      <c r="L22" s="61" t="s">
         <v>316</v>
       </c>
-      <c r="M22" s="40" t="s">
+      <c r="M22" s="61" t="s">
         <v>317</v>
       </c>
-      <c r="N22" s="40" t="s">
+      <c r="N22" s="61" t="s">
         <v>318</v>
       </c>
-      <c r="O22" s="40" t="s">
+      <c r="O22" s="61" t="s">
         <v>324</v>
       </c>
-      <c r="P22" s="40" t="s">
+      <c r="P22" s="61" t="s">
         <v>325</v>
       </c>
       <c r="Q22" s="37" t="s">
@@ -6887,7 +6881,7 @@
       <c r="V22" s="37" t="s">
         <v>328</v>
       </c>
-      <c r="W22" s="71" t="s">
+      <c r="W22" s="70" t="s">
         <v>329</v>
       </c>
     </row>
@@ -6913,7 +6907,7 @@
       <c r="T23" s="37"/>
       <c r="U23" s="37"/>
       <c r="V23" s="37"/>
-      <c r="W23" s="72"/>
+      <c r="W23" s="71"/>
     </row>
     <row r="24" spans="1:23">
       <c r="B24" s="37"/>
@@ -6937,7 +6931,7 @@
       <c r="T24" s="37"/>
       <c r="U24" s="37"/>
       <c r="V24" s="37"/>
-      <c r="W24" s="72"/>
+      <c r="W24" s="71"/>
     </row>
     <row r="25" spans="1:23">
       <c r="B25" s="37"/>
@@ -6961,7 +6955,7 @@
       <c r="T25" s="37"/>
       <c r="U25" s="37"/>
       <c r="V25" s="37"/>
-      <c r="W25" s="72"/>
+      <c r="W25" s="71"/>
     </row>
     <row r="26" spans="1:23">
       <c r="B26" s="37"/>
@@ -6985,7 +6979,7 @@
       <c r="T26" s="37"/>
       <c r="U26" s="37"/>
       <c r="V26" s="37"/>
-      <c r="W26" s="72"/>
+      <c r="W26" s="71"/>
     </row>
     <row r="27" spans="1:23">
       <c r="B27" s="37"/>
@@ -7009,52 +7003,64 @@
       <c r="T27" s="37"/>
       <c r="U27" s="37"/>
       <c r="V27" s="37"/>
-      <c r="W27" s="73"/>
+      <c r="W27" s="72"/>
     </row>
     <row r="28" spans="1:23">
       <c r="B28" s="6"/>
     </row>
     <row r="29" spans="1:23" ht="11.25" customHeight="1">
       <c r="B29" s="6"/>
-      <c r="O29" s="68" t="s">
+      <c r="O29" s="38" t="s">
         <v>326</v>
       </c>
-      <c r="P29" s="68"/>
-      <c r="W29" s="69" t="s">
+      <c r="P29" s="38"/>
+      <c r="W29" s="68" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="30" spans="1:23">
       <c r="B30" s="6"/>
-      <c r="O30" s="68"/>
-      <c r="P30" s="68"/>
-      <c r="W30" s="69"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
+      <c r="W30" s="68"/>
     </row>
     <row r="31" spans="1:23">
-      <c r="O31" s="68"/>
-      <c r="P31" s="68"/>
-      <c r="W31" s="69"/>
+      <c r="O31" s="38"/>
+      <c r="P31" s="38"/>
+      <c r="W31" s="68"/>
     </row>
     <row r="32" spans="1:23">
-      <c r="O32" s="68"/>
-      <c r="P32" s="68"/>
-      <c r="W32" s="69"/>
+      <c r="O32" s="38"/>
+      <c r="P32" s="38"/>
+      <c r="W32" s="68"/>
     </row>
     <row r="33" spans="15:23">
-      <c r="O33" s="68"/>
-      <c r="P33" s="68"/>
-      <c r="W33" s="69"/>
+      <c r="O33" s="38"/>
+      <c r="P33" s="38"/>
+      <c r="W33" s="68"/>
     </row>
     <row r="34" spans="15:23">
-      <c r="O34" s="68"/>
-      <c r="P34" s="68"/>
+      <c r="O34" s="38"/>
+      <c r="P34" s="38"/>
     </row>
     <row r="35" spans="15:23">
-      <c r="O35" s="68"/>
-      <c r="P35" s="68"/>
+      <c r="O35" s="38"/>
+      <c r="P35" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="W19:W21"/>
+    <mergeCell ref="Q22:Q27"/>
+    <mergeCell ref="E22:E27"/>
+    <mergeCell ref="F22:F27"/>
+    <mergeCell ref="G22:G27"/>
+    <mergeCell ref="H22:H27"/>
+    <mergeCell ref="I22:I27"/>
+    <mergeCell ref="K22:K27"/>
+    <mergeCell ref="L22:L27"/>
+    <mergeCell ref="M22:M27"/>
+    <mergeCell ref="N22:N27"/>
+    <mergeCell ref="T22:T27"/>
     <mergeCell ref="B22:B27"/>
     <mergeCell ref="W29:W33"/>
     <mergeCell ref="B19:P21"/>
@@ -7071,18 +7077,6 @@
     <mergeCell ref="W22:W27"/>
     <mergeCell ref="R22:R27"/>
     <mergeCell ref="S22:S27"/>
-    <mergeCell ref="W19:W21"/>
-    <mergeCell ref="Q22:Q27"/>
-    <mergeCell ref="E22:E27"/>
-    <mergeCell ref="F22:F27"/>
-    <mergeCell ref="G22:G27"/>
-    <mergeCell ref="H22:H27"/>
-    <mergeCell ref="I22:I27"/>
-    <mergeCell ref="K22:K27"/>
-    <mergeCell ref="L22:L27"/>
-    <mergeCell ref="M22:M27"/>
-    <mergeCell ref="N22:N27"/>
-    <mergeCell ref="T22:T27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7164,19 +7158,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:56" ht="21">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="56"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="17" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:56" ht="21">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="57"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="17" t="s">
         <v>587</v>
       </c>
@@ -9138,351 +9132,351 @@
       <c r="BB19" s="1"/>
     </row>
     <row r="20" spans="1:56" ht="15" customHeight="1">
-      <c r="B20" s="79" t="s">
+      <c r="B20" s="73" t="s">
         <v>582</v>
       </c>
-      <c r="C20" s="80"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="80"/>
-      <c r="H20" s="80"/>
-      <c r="I20" s="80"/>
-      <c r="J20" s="80"/>
-      <c r="K20" s="80"/>
-      <c r="L20" s="80"/>
-      <c r="M20" s="80"/>
-      <c r="N20" s="80"/>
-      <c r="O20" s="80"/>
-      <c r="P20" s="80"/>
-      <c r="Q20" s="80"/>
-      <c r="R20" s="80"/>
-      <c r="S20" s="80"/>
-      <c r="T20" s="80"/>
-      <c r="U20" s="80"/>
-      <c r="V20" s="80"/>
-      <c r="W20" s="80"/>
-      <c r="X20" s="80"/>
-      <c r="Y20" s="80"/>
-      <c r="Z20" s="80"/>
-      <c r="AA20" s="80"/>
-      <c r="AB20" s="80"/>
-      <c r="AC20" s="80"/>
-      <c r="AD20" s="80"/>
-      <c r="AE20" s="80"/>
-      <c r="AF20" s="80"/>
-      <c r="AG20" s="80"/>
-      <c r="AH20" s="80"/>
-      <c r="AI20" s="80"/>
-      <c r="AJ20" s="80"/>
-      <c r="AK20" s="80"/>
-      <c r="AL20" s="80"/>
-      <c r="AM20" s="80"/>
-      <c r="AN20" s="80"/>
-      <c r="AO20" s="80"/>
-      <c r="AP20" s="80"/>
-      <c r="AQ20" s="80"/>
-      <c r="AR20" s="80"/>
-      <c r="AS20" s="80"/>
-      <c r="AT20" s="80"/>
-      <c r="AU20" s="80"/>
-      <c r="AV20" s="80"/>
-      <c r="AW20" s="80"/>
-      <c r="AX20" s="81"/>
-      <c r="AY20" s="70" t="s">
+      <c r="C20" s="74"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="74"/>
+      <c r="J20" s="74"/>
+      <c r="K20" s="74"/>
+      <c r="L20" s="74"/>
+      <c r="M20" s="74"/>
+      <c r="N20" s="74"/>
+      <c r="O20" s="74"/>
+      <c r="P20" s="74"/>
+      <c r="Q20" s="74"/>
+      <c r="R20" s="74"/>
+      <c r="S20" s="74"/>
+      <c r="T20" s="74"/>
+      <c r="U20" s="74"/>
+      <c r="V20" s="74"/>
+      <c r="W20" s="74"/>
+      <c r="X20" s="74"/>
+      <c r="Y20" s="74"/>
+      <c r="Z20" s="74"/>
+      <c r="AA20" s="74"/>
+      <c r="AB20" s="74"/>
+      <c r="AC20" s="74"/>
+      <c r="AD20" s="74"/>
+      <c r="AE20" s="74"/>
+      <c r="AF20" s="74"/>
+      <c r="AG20" s="74"/>
+      <c r="AH20" s="74"/>
+      <c r="AI20" s="74"/>
+      <c r="AJ20" s="74"/>
+      <c r="AK20" s="74"/>
+      <c r="AL20" s="74"/>
+      <c r="AM20" s="74"/>
+      <c r="AN20" s="74"/>
+      <c r="AO20" s="74"/>
+      <c r="AP20" s="74"/>
+      <c r="AQ20" s="74"/>
+      <c r="AR20" s="74"/>
+      <c r="AS20" s="74"/>
+      <c r="AT20" s="74"/>
+      <c r="AU20" s="74"/>
+      <c r="AV20" s="74"/>
+      <c r="AW20" s="74"/>
+      <c r="AX20" s="75"/>
+      <c r="AY20" s="69" t="s">
         <v>583</v>
       </c>
-      <c r="AZ20" s="70" t="s">
+      <c r="AZ20" s="69" t="s">
         <v>584</v>
       </c>
       <c r="BA20" s="12"/>
       <c r="BB20" s="1"/>
-      <c r="BC20" s="70" t="s">
+      <c r="BC20" s="69" t="s">
         <v>585</v>
       </c>
-      <c r="BD20" s="70" t="s">
+      <c r="BD20" s="69" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="21" spans="1:56" ht="11.25" customHeight="1">
-      <c r="B21" s="82"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83"/>
-      <c r="G21" s="83"/>
-      <c r="H21" s="83"/>
-      <c r="I21" s="83"/>
-      <c r="J21" s="83"/>
-      <c r="K21" s="83"/>
-      <c r="L21" s="83"/>
-      <c r="M21" s="83"/>
-      <c r="N21" s="83"/>
-      <c r="O21" s="83"/>
-      <c r="P21" s="83"/>
-      <c r="Q21" s="83"/>
-      <c r="R21" s="83"/>
-      <c r="S21" s="83"/>
-      <c r="T21" s="83"/>
-      <c r="U21" s="83"/>
-      <c r="V21" s="83"/>
-      <c r="W21" s="83"/>
-      <c r="X21" s="83"/>
-      <c r="Y21" s="83"/>
-      <c r="Z21" s="83"/>
-      <c r="AA21" s="83"/>
-      <c r="AB21" s="83"/>
-      <c r="AC21" s="83"/>
-      <c r="AD21" s="83"/>
-      <c r="AE21" s="83"/>
-      <c r="AF21" s="83"/>
-      <c r="AG21" s="83"/>
-      <c r="AH21" s="83"/>
-      <c r="AI21" s="83"/>
-      <c r="AJ21" s="83"/>
-      <c r="AK21" s="83"/>
-      <c r="AL21" s="83"/>
-      <c r="AM21" s="83"/>
-      <c r="AN21" s="83"/>
-      <c r="AO21" s="83"/>
-      <c r="AP21" s="83"/>
-      <c r="AQ21" s="83"/>
-      <c r="AR21" s="83"/>
-      <c r="AS21" s="83"/>
-      <c r="AT21" s="83"/>
-      <c r="AU21" s="83"/>
-      <c r="AV21" s="83"/>
-      <c r="AW21" s="83"/>
-      <c r="AX21" s="84"/>
-      <c r="AY21" s="70"/>
-      <c r="AZ21" s="70"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="77"/>
+      <c r="I21" s="77"/>
+      <c r="J21" s="77"/>
+      <c r="K21" s="77"/>
+      <c r="L21" s="77"/>
+      <c r="M21" s="77"/>
+      <c r="N21" s="77"/>
+      <c r="O21" s="77"/>
+      <c r="P21" s="77"/>
+      <c r="Q21" s="77"/>
+      <c r="R21" s="77"/>
+      <c r="S21" s="77"/>
+      <c r="T21" s="77"/>
+      <c r="U21" s="77"/>
+      <c r="V21" s="77"/>
+      <c r="W21" s="77"/>
+      <c r="X21" s="77"/>
+      <c r="Y21" s="77"/>
+      <c r="Z21" s="77"/>
+      <c r="AA21" s="77"/>
+      <c r="AB21" s="77"/>
+      <c r="AC21" s="77"/>
+      <c r="AD21" s="77"/>
+      <c r="AE21" s="77"/>
+      <c r="AF21" s="77"/>
+      <c r="AG21" s="77"/>
+      <c r="AH21" s="77"/>
+      <c r="AI21" s="77"/>
+      <c r="AJ21" s="77"/>
+      <c r="AK21" s="77"/>
+      <c r="AL21" s="77"/>
+      <c r="AM21" s="77"/>
+      <c r="AN21" s="77"/>
+      <c r="AO21" s="77"/>
+      <c r="AP21" s="77"/>
+      <c r="AQ21" s="77"/>
+      <c r="AR21" s="77"/>
+      <c r="AS21" s="77"/>
+      <c r="AT21" s="77"/>
+      <c r="AU21" s="77"/>
+      <c r="AV21" s="77"/>
+      <c r="AW21" s="77"/>
+      <c r="AX21" s="78"/>
+      <c r="AY21" s="69"/>
+      <c r="AZ21" s="69"/>
       <c r="BA21" s="12"/>
       <c r="BB21" s="1"/>
-      <c r="BC21" s="70"/>
-      <c r="BD21" s="70"/>
+      <c r="BC21" s="69"/>
+      <c r="BD21" s="69"/>
     </row>
     <row r="22" spans="1:56" ht="11.25" customHeight="1">
-      <c r="B22" s="85"/>
-      <c r="C22" s="86"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
-      <c r="H22" s="86"/>
-      <c r="I22" s="86"/>
-      <c r="J22" s="86"/>
-      <c r="K22" s="86"/>
-      <c r="L22" s="86"/>
-      <c r="M22" s="86"/>
-      <c r="N22" s="86"/>
-      <c r="O22" s="86"/>
-      <c r="P22" s="86"/>
-      <c r="Q22" s="86"/>
-      <c r="R22" s="86"/>
-      <c r="S22" s="86"/>
-      <c r="T22" s="86"/>
-      <c r="U22" s="86"/>
-      <c r="V22" s="86"/>
-      <c r="W22" s="86"/>
-      <c r="X22" s="86"/>
-      <c r="Y22" s="86"/>
-      <c r="Z22" s="86"/>
-      <c r="AA22" s="86"/>
-      <c r="AB22" s="86"/>
-      <c r="AC22" s="86"/>
-      <c r="AD22" s="86"/>
-      <c r="AE22" s="86"/>
-      <c r="AF22" s="86"/>
-      <c r="AG22" s="86"/>
-      <c r="AH22" s="86"/>
-      <c r="AI22" s="86"/>
-      <c r="AJ22" s="86"/>
-      <c r="AK22" s="86"/>
-      <c r="AL22" s="86"/>
-      <c r="AM22" s="86"/>
-      <c r="AN22" s="86"/>
-      <c r="AO22" s="86"/>
-      <c r="AP22" s="86"/>
-      <c r="AQ22" s="86"/>
-      <c r="AR22" s="86"/>
-      <c r="AS22" s="86"/>
-      <c r="AT22" s="86"/>
-      <c r="AU22" s="86"/>
-      <c r="AV22" s="86"/>
-      <c r="AW22" s="86"/>
-      <c r="AX22" s="87"/>
-      <c r="AY22" s="70"/>
-      <c r="AZ22" s="70"/>
+      <c r="B22" s="79"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="80"/>
+      <c r="M22" s="80"/>
+      <c r="N22" s="80"/>
+      <c r="O22" s="80"/>
+      <c r="P22" s="80"/>
+      <c r="Q22" s="80"/>
+      <c r="R22" s="80"/>
+      <c r="S22" s="80"/>
+      <c r="T22" s="80"/>
+      <c r="U22" s="80"/>
+      <c r="V22" s="80"/>
+      <c r="W22" s="80"/>
+      <c r="X22" s="80"/>
+      <c r="Y22" s="80"/>
+      <c r="Z22" s="80"/>
+      <c r="AA22" s="80"/>
+      <c r="AB22" s="80"/>
+      <c r="AC22" s="80"/>
+      <c r="AD22" s="80"/>
+      <c r="AE22" s="80"/>
+      <c r="AF22" s="80"/>
+      <c r="AG22" s="80"/>
+      <c r="AH22" s="80"/>
+      <c r="AI22" s="80"/>
+      <c r="AJ22" s="80"/>
+      <c r="AK22" s="80"/>
+      <c r="AL22" s="80"/>
+      <c r="AM22" s="80"/>
+      <c r="AN22" s="80"/>
+      <c r="AO22" s="80"/>
+      <c r="AP22" s="80"/>
+      <c r="AQ22" s="80"/>
+      <c r="AR22" s="80"/>
+      <c r="AS22" s="80"/>
+      <c r="AT22" s="80"/>
+      <c r="AU22" s="80"/>
+      <c r="AV22" s="80"/>
+      <c r="AW22" s="80"/>
+      <c r="AX22" s="81"/>
+      <c r="AY22" s="69"/>
+      <c r="AZ22" s="69"/>
       <c r="BA22" s="6"/>
       <c r="BB22" s="1"/>
-      <c r="BC22" s="70"/>
-      <c r="BD22" s="70"/>
+      <c r="BC22" s="69"/>
+      <c r="BD22" s="69"/>
     </row>
     <row r="23" spans="1:56" ht="11.25" customHeight="1">
       <c r="A23" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="61" t="s">
         <v>448</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="61" t="s">
         <v>514</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="61" t="s">
         <v>515</v>
       </c>
-      <c r="E23" s="40" t="s">
+      <c r="E23" s="61" t="s">
         <v>449</v>
       </c>
-      <c r="F23" s="40" t="s">
+      <c r="F23" s="61" t="s">
         <v>502</v>
       </c>
-      <c r="G23" s="40" t="s">
+      <c r="G23" s="61" t="s">
         <v>503</v>
       </c>
-      <c r="H23" s="73" t="s">
+      <c r="H23" s="72" t="s">
         <v>517</v>
       </c>
-      <c r="I23" s="73"/>
-      <c r="J23" s="40" t="s">
+      <c r="I23" s="72"/>
+      <c r="J23" s="61" t="s">
         <v>497</v>
       </c>
-      <c r="K23" s="40" t="s">
+      <c r="K23" s="61" t="s">
         <v>498</v>
       </c>
-      <c r="L23" s="40" t="s">
+      <c r="L23" s="61" t="s">
         <v>499</v>
       </c>
-      <c r="M23" s="40" t="s">
+      <c r="M23" s="61" t="s">
         <v>500</v>
       </c>
-      <c r="N23" s="40" t="s">
+      <c r="N23" s="61" t="s">
         <v>504</v>
       </c>
-      <c r="O23" s="40" t="s">
+      <c r="O23" s="61" t="s">
         <v>505</v>
       </c>
-      <c r="P23" s="40" t="s">
+      <c r="P23" s="61" t="s">
         <v>506</v>
       </c>
-      <c r="Q23" s="40" t="s">
+      <c r="Q23" s="61" t="s">
         <v>507</v>
       </c>
-      <c r="R23" s="40" t="s">
+      <c r="R23" s="61" t="s">
         <v>508</v>
       </c>
-      <c r="S23" s="40" t="s">
+      <c r="S23" s="61" t="s">
         <v>512</v>
       </c>
-      <c r="T23" s="40" t="s">
+      <c r="T23" s="61" t="s">
         <v>509</v>
       </c>
-      <c r="U23" s="40" t="s">
+      <c r="U23" s="61" t="s">
         <v>510</v>
       </c>
-      <c r="V23" s="40" t="s">
+      <c r="V23" s="61" t="s">
         <v>511</v>
       </c>
-      <c r="W23" s="40" t="s">
+      <c r="W23" s="61" t="s">
         <v>519</v>
       </c>
-      <c r="X23" s="40" t="s">
+      <c r="X23" s="61" t="s">
         <v>513</v>
       </c>
-      <c r="Y23" s="40" t="s">
+      <c r="Y23" s="61" t="s">
         <v>518</v>
       </c>
-      <c r="Z23" s="75" t="s">
+      <c r="Z23" s="85" t="s">
         <v>735</v>
       </c>
-      <c r="AA23" s="73" t="s">
+      <c r="AA23" s="72" t="s">
         <v>535</v>
       </c>
-      <c r="AB23" s="73" t="s">
+      <c r="AB23" s="72" t="s">
         <v>537</v>
       </c>
-      <c r="AC23" s="73" t="s">
+      <c r="AC23" s="72" t="s">
         <v>536</v>
       </c>
-      <c r="AD23" s="73" t="s">
+      <c r="AD23" s="72" t="s">
         <v>538</v>
       </c>
-      <c r="AE23" s="73" t="s">
+      <c r="AE23" s="72" t="s">
         <v>539</v>
       </c>
-      <c r="AF23" s="73" t="s">
+      <c r="AF23" s="72" t="s">
         <v>540</v>
       </c>
-      <c r="AG23" s="73" t="s">
+      <c r="AG23" s="72" t="s">
         <v>541</v>
       </c>
-      <c r="AH23" s="73" t="s">
+      <c r="AH23" s="72" t="s">
         <v>542</v>
       </c>
-      <c r="AI23" s="73" t="s">
+      <c r="AI23" s="72" t="s">
         <v>543</v>
       </c>
-      <c r="AJ23" s="77" t="s">
+      <c r="AJ23" s="84" t="s">
         <v>544</v>
       </c>
-      <c r="AK23" s="73" t="s">
+      <c r="AK23" s="72" t="s">
         <v>545</v>
       </c>
-      <c r="AL23" s="73" t="s">
+      <c r="AL23" s="72" t="s">
         <v>546</v>
       </c>
-      <c r="AM23" s="73" t="s">
+      <c r="AM23" s="72" t="s">
         <v>547</v>
       </c>
-      <c r="AN23" s="73" t="s">
+      <c r="AN23" s="72" t="s">
         <v>548</v>
       </c>
-      <c r="AO23" s="73" t="s">
+      <c r="AO23" s="72" t="s">
         <v>549</v>
       </c>
-      <c r="AP23" s="73" t="s">
+      <c r="AP23" s="72" t="s">
         <v>550</v>
       </c>
-      <c r="AQ23" s="73" t="s">
+      <c r="AQ23" s="72" t="s">
         <v>551</v>
       </c>
-      <c r="AR23" s="73" t="s">
+      <c r="AR23" s="72" t="s">
         <v>552</v>
       </c>
-      <c r="AS23" s="73" t="s">
+      <c r="AS23" s="72" t="s">
         <v>553</v>
       </c>
-      <c r="AT23" s="73" t="s">
+      <c r="AT23" s="72" t="s">
         <v>554</v>
       </c>
-      <c r="AU23" s="73" t="s">
+      <c r="AU23" s="72" t="s">
         <v>555</v>
       </c>
-      <c r="AV23" s="73" t="s">
+      <c r="AV23" s="72" t="s">
         <v>556</v>
       </c>
-      <c r="AW23" s="73" t="s">
+      <c r="AW23" s="72" t="s">
         <v>557</v>
       </c>
-      <c r="AX23" s="73" t="s">
+      <c r="AX23" s="72" t="s">
         <v>558</v>
       </c>
-      <c r="AY23" s="73" t="s">
+      <c r="AY23" s="72" t="s">
         <v>559</v>
       </c>
-      <c r="AZ23" s="74" t="s">
+      <c r="AZ23" s="82" t="s">
         <v>560</v>
       </c>
-      <c r="BA23" s="67" t="s">
+      <c r="BA23" s="36" t="s">
         <v>561</v>
       </c>
-      <c r="BB23" s="67" t="s">
+      <c r="BB23" s="36" t="s">
         <v>561</v>
       </c>
-      <c r="BC23" s="74" t="s">
+      <c r="BC23" s="82" t="s">
         <v>562</v>
       </c>
-      <c r="BD23" s="78" t="s">
+      <c r="BD23" s="83" t="s">
         <v>563</v>
       </c>
     </row>
@@ -9494,8 +9488,8 @@
       <c r="E24" s="37"/>
       <c r="F24" s="37"/>
       <c r="G24" s="37"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="74"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="82"/>
       <c r="J24" s="37"/>
       <c r="K24" s="37"/>
       <c r="L24" s="37"/>
@@ -9512,37 +9506,37 @@
       <c r="W24" s="37"/>
       <c r="X24" s="37"/>
       <c r="Y24" s="37"/>
-      <c r="Z24" s="76"/>
-      <c r="AA24" s="74"/>
-      <c r="AB24" s="74"/>
-      <c r="AC24" s="74"/>
-      <c r="AD24" s="74"/>
-      <c r="AE24" s="74"/>
-      <c r="AF24" s="74"/>
-      <c r="AG24" s="74"/>
-      <c r="AH24" s="74"/>
-      <c r="AI24" s="74"/>
-      <c r="AJ24" s="77"/>
-      <c r="AK24" s="74"/>
-      <c r="AL24" s="74"/>
-      <c r="AM24" s="74"/>
-      <c r="AN24" s="74"/>
-      <c r="AO24" s="74"/>
-      <c r="AP24" s="74"/>
-      <c r="AQ24" s="74"/>
-      <c r="AR24" s="74"/>
-      <c r="AS24" s="74"/>
-      <c r="AT24" s="74"/>
-      <c r="AU24" s="74"/>
-      <c r="AV24" s="74"/>
-      <c r="AW24" s="74"/>
-      <c r="AX24" s="74"/>
-      <c r="AY24" s="74"/>
-      <c r="AZ24" s="74"/>
-      <c r="BA24" s="67"/>
-      <c r="BB24" s="67"/>
-      <c r="BC24" s="74"/>
-      <c r="BD24" s="78"/>
+      <c r="Z24" s="86"/>
+      <c r="AA24" s="82"/>
+      <c r="AB24" s="82"/>
+      <c r="AC24" s="82"/>
+      <c r="AD24" s="82"/>
+      <c r="AE24" s="82"/>
+      <c r="AF24" s="82"/>
+      <c r="AG24" s="82"/>
+      <c r="AH24" s="82"/>
+      <c r="AI24" s="82"/>
+      <c r="AJ24" s="84"/>
+      <c r="AK24" s="82"/>
+      <c r="AL24" s="82"/>
+      <c r="AM24" s="82"/>
+      <c r="AN24" s="82"/>
+      <c r="AO24" s="82"/>
+      <c r="AP24" s="82"/>
+      <c r="AQ24" s="82"/>
+      <c r="AR24" s="82"/>
+      <c r="AS24" s="82"/>
+      <c r="AT24" s="82"/>
+      <c r="AU24" s="82"/>
+      <c r="AV24" s="82"/>
+      <c r="AW24" s="82"/>
+      <c r="AX24" s="82"/>
+      <c r="AY24" s="82"/>
+      <c r="AZ24" s="82"/>
+      <c r="BA24" s="36"/>
+      <c r="BB24" s="36"/>
+      <c r="BC24" s="82"/>
+      <c r="BD24" s="83"/>
     </row>
     <row r="25" spans="1:56">
       <c r="A25" s="37"/>
@@ -9552,8 +9546,8 @@
       <c r="E25" s="37"/>
       <c r="F25" s="37"/>
       <c r="G25" s="37"/>
-      <c r="H25" s="74"/>
-      <c r="I25" s="74"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="82"/>
       <c r="J25" s="37"/>
       <c r="K25" s="37"/>
       <c r="L25" s="37"/>
@@ -9570,37 +9564,37 @@
       <c r="W25" s="37"/>
       <c r="X25" s="37"/>
       <c r="Y25" s="37"/>
-      <c r="Z25" s="76"/>
-      <c r="AA25" s="74"/>
-      <c r="AB25" s="74"/>
-      <c r="AC25" s="74"/>
-      <c r="AD25" s="74"/>
-      <c r="AE25" s="74"/>
-      <c r="AF25" s="74"/>
-      <c r="AG25" s="74"/>
-      <c r="AH25" s="74"/>
-      <c r="AI25" s="74"/>
-      <c r="AJ25" s="77"/>
-      <c r="AK25" s="74"/>
-      <c r="AL25" s="74"/>
-      <c r="AM25" s="74"/>
-      <c r="AN25" s="74"/>
-      <c r="AO25" s="74"/>
-      <c r="AP25" s="74"/>
-      <c r="AQ25" s="74"/>
-      <c r="AR25" s="74"/>
-      <c r="AS25" s="74"/>
-      <c r="AT25" s="74"/>
-      <c r="AU25" s="74"/>
-      <c r="AV25" s="74"/>
-      <c r="AW25" s="74"/>
-      <c r="AX25" s="74"/>
-      <c r="AY25" s="74"/>
-      <c r="AZ25" s="74"/>
-      <c r="BA25" s="67"/>
-      <c r="BB25" s="67"/>
-      <c r="BC25" s="74"/>
-      <c r="BD25" s="78"/>
+      <c r="Z25" s="86"/>
+      <c r="AA25" s="82"/>
+      <c r="AB25" s="82"/>
+      <c r="AC25" s="82"/>
+      <c r="AD25" s="82"/>
+      <c r="AE25" s="82"/>
+      <c r="AF25" s="82"/>
+      <c r="AG25" s="82"/>
+      <c r="AH25" s="82"/>
+      <c r="AI25" s="82"/>
+      <c r="AJ25" s="84"/>
+      <c r="AK25" s="82"/>
+      <c r="AL25" s="82"/>
+      <c r="AM25" s="82"/>
+      <c r="AN25" s="82"/>
+      <c r="AO25" s="82"/>
+      <c r="AP25" s="82"/>
+      <c r="AQ25" s="82"/>
+      <c r="AR25" s="82"/>
+      <c r="AS25" s="82"/>
+      <c r="AT25" s="82"/>
+      <c r="AU25" s="82"/>
+      <c r="AV25" s="82"/>
+      <c r="AW25" s="82"/>
+      <c r="AX25" s="82"/>
+      <c r="AY25" s="82"/>
+      <c r="AZ25" s="82"/>
+      <c r="BA25" s="36"/>
+      <c r="BB25" s="36"/>
+      <c r="BC25" s="82"/>
+      <c r="BD25" s="83"/>
     </row>
     <row r="26" spans="1:56">
       <c r="A26" s="37"/>
@@ -9610,8 +9604,8 @@
       <c r="E26" s="37"/>
       <c r="F26" s="37"/>
       <c r="G26" s="37"/>
-      <c r="H26" s="74"/>
-      <c r="I26" s="74"/>
+      <c r="H26" s="82"/>
+      <c r="I26" s="82"/>
       <c r="J26" s="37"/>
       <c r="K26" s="37"/>
       <c r="L26" s="37"/>
@@ -9628,37 +9622,37 @@
       <c r="W26" s="37"/>
       <c r="X26" s="37"/>
       <c r="Y26" s="37"/>
-      <c r="Z26" s="76"/>
-      <c r="AA26" s="74"/>
-      <c r="AB26" s="74"/>
-      <c r="AC26" s="74"/>
-      <c r="AD26" s="74"/>
-      <c r="AE26" s="74"/>
-      <c r="AF26" s="74"/>
-      <c r="AG26" s="74"/>
-      <c r="AH26" s="74"/>
-      <c r="AI26" s="74"/>
-      <c r="AJ26" s="77"/>
-      <c r="AK26" s="74"/>
-      <c r="AL26" s="74"/>
-      <c r="AM26" s="74"/>
-      <c r="AN26" s="74"/>
-      <c r="AO26" s="74"/>
-      <c r="AP26" s="74"/>
-      <c r="AQ26" s="74"/>
-      <c r="AR26" s="74"/>
-      <c r="AS26" s="74"/>
-      <c r="AT26" s="74"/>
-      <c r="AU26" s="74"/>
-      <c r="AV26" s="74"/>
-      <c r="AW26" s="74"/>
-      <c r="AX26" s="74"/>
-      <c r="AY26" s="74"/>
-      <c r="AZ26" s="74"/>
-      <c r="BA26" s="67"/>
-      <c r="BB26" s="67"/>
-      <c r="BC26" s="74"/>
-      <c r="BD26" s="78"/>
+      <c r="Z26" s="86"/>
+      <c r="AA26" s="82"/>
+      <c r="AB26" s="82"/>
+      <c r="AC26" s="82"/>
+      <c r="AD26" s="82"/>
+      <c r="AE26" s="82"/>
+      <c r="AF26" s="82"/>
+      <c r="AG26" s="82"/>
+      <c r="AH26" s="82"/>
+      <c r="AI26" s="82"/>
+      <c r="AJ26" s="84"/>
+      <c r="AK26" s="82"/>
+      <c r="AL26" s="82"/>
+      <c r="AM26" s="82"/>
+      <c r="AN26" s="82"/>
+      <c r="AO26" s="82"/>
+      <c r="AP26" s="82"/>
+      <c r="AQ26" s="82"/>
+      <c r="AR26" s="82"/>
+      <c r="AS26" s="82"/>
+      <c r="AT26" s="82"/>
+      <c r="AU26" s="82"/>
+      <c r="AV26" s="82"/>
+      <c r="AW26" s="82"/>
+      <c r="AX26" s="82"/>
+      <c r="AY26" s="82"/>
+      <c r="AZ26" s="82"/>
+      <c r="BA26" s="36"/>
+      <c r="BB26" s="36"/>
+      <c r="BC26" s="82"/>
+      <c r="BD26" s="83"/>
     </row>
     <row r="27" spans="1:56">
       <c r="A27" s="37"/>
@@ -9668,8 +9662,8 @@
       <c r="E27" s="37"/>
       <c r="F27" s="37"/>
       <c r="G27" s="37"/>
-      <c r="H27" s="74"/>
-      <c r="I27" s="74"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="82"/>
       <c r="J27" s="37"/>
       <c r="K27" s="37"/>
       <c r="L27" s="37"/>
@@ -9686,37 +9680,37 @@
       <c r="W27" s="37"/>
       <c r="X27" s="37"/>
       <c r="Y27" s="37"/>
-      <c r="Z27" s="76"/>
-      <c r="AA27" s="74"/>
-      <c r="AB27" s="74"/>
-      <c r="AC27" s="74"/>
-      <c r="AD27" s="74"/>
-      <c r="AE27" s="74"/>
-      <c r="AF27" s="74"/>
-      <c r="AG27" s="74"/>
-      <c r="AH27" s="74"/>
-      <c r="AI27" s="74"/>
-      <c r="AJ27" s="77"/>
-      <c r="AK27" s="74"/>
-      <c r="AL27" s="74"/>
-      <c r="AM27" s="74"/>
-      <c r="AN27" s="74"/>
-      <c r="AO27" s="74"/>
-      <c r="AP27" s="74"/>
-      <c r="AQ27" s="74"/>
-      <c r="AR27" s="74"/>
-      <c r="AS27" s="74"/>
-      <c r="AT27" s="74"/>
-      <c r="AU27" s="74"/>
-      <c r="AV27" s="74"/>
-      <c r="AW27" s="74"/>
-      <c r="AX27" s="74"/>
-      <c r="AY27" s="74"/>
-      <c r="AZ27" s="74"/>
-      <c r="BA27" s="67"/>
-      <c r="BB27" s="67"/>
-      <c r="BC27" s="74"/>
-      <c r="BD27" s="78"/>
+      <c r="Z27" s="86"/>
+      <c r="AA27" s="82"/>
+      <c r="AB27" s="82"/>
+      <c r="AC27" s="82"/>
+      <c r="AD27" s="82"/>
+      <c r="AE27" s="82"/>
+      <c r="AF27" s="82"/>
+      <c r="AG27" s="82"/>
+      <c r="AH27" s="82"/>
+      <c r="AI27" s="82"/>
+      <c r="AJ27" s="84"/>
+      <c r="AK27" s="82"/>
+      <c r="AL27" s="82"/>
+      <c r="AM27" s="82"/>
+      <c r="AN27" s="82"/>
+      <c r="AO27" s="82"/>
+      <c r="AP27" s="82"/>
+      <c r="AQ27" s="82"/>
+      <c r="AR27" s="82"/>
+      <c r="AS27" s="82"/>
+      <c r="AT27" s="82"/>
+      <c r="AU27" s="82"/>
+      <c r="AV27" s="82"/>
+      <c r="AW27" s="82"/>
+      <c r="AX27" s="82"/>
+      <c r="AY27" s="82"/>
+      <c r="AZ27" s="82"/>
+      <c r="BA27" s="36"/>
+      <c r="BB27" s="36"/>
+      <c r="BC27" s="82"/>
+      <c r="BD27" s="83"/>
     </row>
     <row r="28" spans="1:56">
       <c r="H28" s="4"/>
@@ -9724,35 +9718,35 @@
       <c r="W28" s="12"/>
       <c r="X28" s="1"/>
       <c r="Z28" s="1"/>
-      <c r="AA28" s="74"/>
-      <c r="AB28" s="74"/>
-      <c r="AC28" s="74"/>
-      <c r="AD28" s="74"/>
-      <c r="AE28" s="74"/>
-      <c r="AF28" s="74"/>
-      <c r="AG28" s="74"/>
-      <c r="AH28" s="74"/>
-      <c r="AI28" s="74"/>
-      <c r="AJ28" s="77"/>
-      <c r="AK28" s="74"/>
-      <c r="AL28" s="74"/>
-      <c r="AM28" s="74"/>
-      <c r="AN28" s="74"/>
-      <c r="AO28" s="74"/>
-      <c r="AP28" s="74"/>
-      <c r="AQ28" s="74"/>
-      <c r="AR28" s="74"/>
-      <c r="AS28" s="74"/>
-      <c r="AT28" s="74"/>
-      <c r="AU28" s="74"/>
-      <c r="AV28" s="74"/>
-      <c r="AW28" s="74"/>
-      <c r="AX28" s="74"/>
-      <c r="AY28" s="74"/>
-      <c r="AZ28" s="74"/>
-      <c r="BA28" s="67"/>
-      <c r="BB28" s="67"/>
-      <c r="BC28" s="74"/>
+      <c r="AA28" s="82"/>
+      <c r="AB28" s="82"/>
+      <c r="AC28" s="82"/>
+      <c r="AD28" s="82"/>
+      <c r="AE28" s="82"/>
+      <c r="AF28" s="82"/>
+      <c r="AG28" s="82"/>
+      <c r="AH28" s="82"/>
+      <c r="AI28" s="82"/>
+      <c r="AJ28" s="84"/>
+      <c r="AK28" s="82"/>
+      <c r="AL28" s="82"/>
+      <c r="AM28" s="82"/>
+      <c r="AN28" s="82"/>
+      <c r="AO28" s="82"/>
+      <c r="AP28" s="82"/>
+      <c r="AQ28" s="82"/>
+      <c r="AR28" s="82"/>
+      <c r="AS28" s="82"/>
+      <c r="AT28" s="82"/>
+      <c r="AU28" s="82"/>
+      <c r="AV28" s="82"/>
+      <c r="AW28" s="82"/>
+      <c r="AX28" s="82"/>
+      <c r="AY28" s="82"/>
+      <c r="AZ28" s="82"/>
+      <c r="BA28" s="36"/>
+      <c r="BB28" s="36"/>
+      <c r="BC28" s="82"/>
     </row>
     <row r="29" spans="1:56">
       <c r="C29" s="21" t="s">
@@ -9771,35 +9765,35 @@
       <c r="Z29" s="25" t="s">
         <v>734</v>
       </c>
-      <c r="AA29" s="74"/>
-      <c r="AB29" s="74"/>
-      <c r="AC29" s="74"/>
-      <c r="AD29" s="74"/>
-      <c r="AE29" s="74"/>
-      <c r="AF29" s="74"/>
-      <c r="AG29" s="74"/>
-      <c r="AH29" s="74"/>
-      <c r="AI29" s="74"/>
-      <c r="AJ29" s="77"/>
-      <c r="AK29" s="74"/>
-      <c r="AL29" s="74"/>
-      <c r="AM29" s="74"/>
-      <c r="AN29" s="74"/>
-      <c r="AO29" s="74"/>
-      <c r="AP29" s="74"/>
-      <c r="AQ29" s="74"/>
-      <c r="AR29" s="74"/>
-      <c r="AS29" s="74"/>
-      <c r="AT29" s="74"/>
-      <c r="AU29" s="74"/>
-      <c r="AV29" s="74"/>
-      <c r="AW29" s="74"/>
-      <c r="AX29" s="74"/>
-      <c r="AY29" s="74"/>
-      <c r="AZ29" s="74"/>
-      <c r="BA29" s="67"/>
-      <c r="BB29" s="67"/>
-      <c r="BC29" s="74"/>
+      <c r="AA29" s="82"/>
+      <c r="AB29" s="82"/>
+      <c r="AC29" s="82"/>
+      <c r="AD29" s="82"/>
+      <c r="AE29" s="82"/>
+      <c r="AF29" s="82"/>
+      <c r="AG29" s="82"/>
+      <c r="AH29" s="82"/>
+      <c r="AI29" s="82"/>
+      <c r="AJ29" s="84"/>
+      <c r="AK29" s="82"/>
+      <c r="AL29" s="82"/>
+      <c r="AM29" s="82"/>
+      <c r="AN29" s="82"/>
+      <c r="AO29" s="82"/>
+      <c r="AP29" s="82"/>
+      <c r="AQ29" s="82"/>
+      <c r="AR29" s="82"/>
+      <c r="AS29" s="82"/>
+      <c r="AT29" s="82"/>
+      <c r="AU29" s="82"/>
+      <c r="AV29" s="82"/>
+      <c r="AW29" s="82"/>
+      <c r="AX29" s="82"/>
+      <c r="AY29" s="82"/>
+      <c r="AZ29" s="82"/>
+      <c r="BA29" s="36"/>
+      <c r="BB29" s="36"/>
+      <c r="BC29" s="82"/>
     </row>
     <row r="30" spans="1:56" ht="123.75">
       <c r="C30" s="14" t="s">
@@ -13135,42 +13129,24 @@
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="AY20:AY22"/>
-    <mergeCell ref="B20:AX22"/>
-    <mergeCell ref="AZ20:AZ22"/>
-    <mergeCell ref="BC20:BC22"/>
-    <mergeCell ref="BD20:BD22"/>
-    <mergeCell ref="AZ23:AZ29"/>
-    <mergeCell ref="BA23:BA29"/>
-    <mergeCell ref="BB23:BB29"/>
-    <mergeCell ref="BC23:BC29"/>
-    <mergeCell ref="BD23:BD27"/>
-    <mergeCell ref="AU23:AU29"/>
-    <mergeCell ref="AV23:AV29"/>
-    <mergeCell ref="AW23:AW29"/>
-    <mergeCell ref="AX23:AX29"/>
-    <mergeCell ref="AY23:AY29"/>
-    <mergeCell ref="AP23:AP29"/>
-    <mergeCell ref="AQ23:AQ29"/>
-    <mergeCell ref="AR23:AR29"/>
-    <mergeCell ref="AS23:AS29"/>
-    <mergeCell ref="AT23:AT29"/>
-    <mergeCell ref="AK23:AK29"/>
-    <mergeCell ref="AL23:AL29"/>
-    <mergeCell ref="AM23:AM29"/>
-    <mergeCell ref="AN23:AN29"/>
-    <mergeCell ref="AO23:AO29"/>
-    <mergeCell ref="AF23:AF29"/>
-    <mergeCell ref="AG23:AG29"/>
-    <mergeCell ref="AH23:AH29"/>
-    <mergeCell ref="AI23:AI29"/>
-    <mergeCell ref="AJ23:AJ29"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="E23:E27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="AC23:AC29"/>
+    <mergeCell ref="AB23:AB29"/>
+    <mergeCell ref="AD23:AD29"/>
+    <mergeCell ref="AE23:AE29"/>
+    <mergeCell ref="Y23:Y27"/>
+    <mergeCell ref="Q23:Q27"/>
+    <mergeCell ref="R23:R27"/>
+    <mergeCell ref="T23:T27"/>
+    <mergeCell ref="N23:N27"/>
+    <mergeCell ref="O23:O27"/>
+    <mergeCell ref="P23:P27"/>
+    <mergeCell ref="W23:W27"/>
+    <mergeCell ref="Z23:Z27"/>
+    <mergeCell ref="AA23:AA29"/>
+    <mergeCell ref="S23:S27"/>
+    <mergeCell ref="X23:X27"/>
+    <mergeCell ref="U23:U27"/>
+    <mergeCell ref="V23:V27"/>
     <mergeCell ref="J23:J27"/>
     <mergeCell ref="K23:K27"/>
     <mergeCell ref="L23:L27"/>
@@ -13179,24 +13155,42 @@
     <mergeCell ref="F23:F27"/>
     <mergeCell ref="G23:G27"/>
     <mergeCell ref="H23:I27"/>
-    <mergeCell ref="W23:W27"/>
-    <mergeCell ref="Z23:Z27"/>
-    <mergeCell ref="AA23:AA29"/>
-    <mergeCell ref="S23:S27"/>
-    <mergeCell ref="X23:X27"/>
-    <mergeCell ref="U23:U27"/>
-    <mergeCell ref="V23:V27"/>
-    <mergeCell ref="Q23:Q27"/>
-    <mergeCell ref="R23:R27"/>
-    <mergeCell ref="T23:T27"/>
-    <mergeCell ref="N23:N27"/>
-    <mergeCell ref="O23:O27"/>
-    <mergeCell ref="P23:P27"/>
-    <mergeCell ref="AC23:AC29"/>
-    <mergeCell ref="AB23:AB29"/>
-    <mergeCell ref="AD23:AD29"/>
-    <mergeCell ref="AE23:AE29"/>
-    <mergeCell ref="Y23:Y27"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E23:E27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="AF23:AF29"/>
+    <mergeCell ref="AG23:AG29"/>
+    <mergeCell ref="AH23:AH29"/>
+    <mergeCell ref="AI23:AI29"/>
+    <mergeCell ref="AJ23:AJ29"/>
+    <mergeCell ref="AK23:AK29"/>
+    <mergeCell ref="AL23:AL29"/>
+    <mergeCell ref="AM23:AM29"/>
+    <mergeCell ref="AN23:AN29"/>
+    <mergeCell ref="AO23:AO29"/>
+    <mergeCell ref="AP23:AP29"/>
+    <mergeCell ref="AQ23:AQ29"/>
+    <mergeCell ref="AR23:AR29"/>
+    <mergeCell ref="AS23:AS29"/>
+    <mergeCell ref="AT23:AT29"/>
+    <mergeCell ref="AU23:AU29"/>
+    <mergeCell ref="AV23:AV29"/>
+    <mergeCell ref="AW23:AW29"/>
+    <mergeCell ref="AX23:AX29"/>
+    <mergeCell ref="AY23:AY29"/>
+    <mergeCell ref="AZ23:AZ29"/>
+    <mergeCell ref="BA23:BA29"/>
+    <mergeCell ref="BB23:BB29"/>
+    <mergeCell ref="BC23:BC29"/>
+    <mergeCell ref="BD23:BD27"/>
+    <mergeCell ref="AY20:AY22"/>
+    <mergeCell ref="B20:AX22"/>
+    <mergeCell ref="AZ20:AZ22"/>
+    <mergeCell ref="BC20:BC22"/>
+    <mergeCell ref="BD20:BD22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -13210,8 +13204,8 @@
   </sheetPr>
   <dimension ref="A1:BW53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BM4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BN18" sqref="BN18:BN20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -13296,10 +13290,10 @@
       <c r="BW1" s="1"/>
     </row>
     <row r="2" spans="1:75" ht="21">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="56"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="17" t="s">
         <v>588</v>
       </c>
@@ -13307,10 +13301,10 @@
       <c r="BW2" s="1"/>
     </row>
     <row r="3" spans="1:75" ht="21">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="57"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="17" t="s">
         <v>844</v>
       </c>
@@ -14554,10 +14548,10 @@
         <v>11</v>
       </c>
       <c r="AA11" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="AB11" s="12" t="s">
         <v>863</v>
-      </c>
-      <c r="AB11" s="12" t="s">
-        <v>864</v>
       </c>
       <c r="AC11" s="12" t="s">
         <v>672</v>
@@ -15315,7 +15309,7 @@
       <c r="BG14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="BH14" s="36" t="s">
+      <c r="BH14" s="35" t="s">
         <v>3</v>
       </c>
       <c r="BI14" s="12" t="s">
@@ -15536,7 +15530,7 @@
       <c r="BG15" s="12" t="s">
         <v>717</v>
       </c>
-      <c r="BH15" s="36">
+      <c r="BH15" s="35">
         <v>40000</v>
       </c>
       <c r="BI15" s="12" t="s">
@@ -15757,7 +15751,7 @@
       <c r="BG16" s="12" t="s">
         <v>703</v>
       </c>
-      <c r="BH16" s="36">
+      <c r="BH16" s="35">
         <v>40000</v>
       </c>
       <c r="BI16" s="12" t="s">
@@ -15846,303 +15840,303 @@
       <c r="BS17" s="12"/>
     </row>
     <row r="18" spans="1:73" ht="11.25" customHeight="1">
-      <c r="B18" s="58" t="s">
-        <v>867</v>
-      </c>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="59"/>
-      <c r="N18" s="59"/>
-      <c r="O18" s="59"/>
-      <c r="P18" s="59"/>
-      <c r="Q18" s="59"/>
-      <c r="R18" s="59"/>
-      <c r="S18" s="59"/>
-      <c r="T18" s="59"/>
-      <c r="U18" s="59"/>
-      <c r="V18" s="59"/>
-      <c r="W18" s="59"/>
-      <c r="X18" s="59"/>
-      <c r="Y18" s="59"/>
-      <c r="Z18" s="59"/>
-      <c r="AA18" s="59"/>
-      <c r="AB18" s="59"/>
-      <c r="AC18" s="59"/>
-      <c r="AD18" s="59"/>
-      <c r="AE18" s="59"/>
-      <c r="AF18" s="59"/>
-      <c r="AG18" s="59"/>
-      <c r="AH18" s="59"/>
-      <c r="AI18" s="59"/>
-      <c r="AJ18" s="59"/>
-      <c r="AK18" s="59"/>
-      <c r="AL18" s="59"/>
-      <c r="AM18" s="59"/>
-      <c r="AN18" s="59"/>
-      <c r="AO18" s="59"/>
-      <c r="AP18" s="59"/>
-      <c r="AQ18" s="59"/>
-      <c r="AR18" s="59"/>
-      <c r="AS18" s="59"/>
-      <c r="AT18" s="59"/>
-      <c r="AU18" s="59"/>
-      <c r="AV18" s="59"/>
-      <c r="AW18" s="59"/>
-      <c r="AX18" s="59"/>
-      <c r="AY18" s="59"/>
-      <c r="AZ18" s="59"/>
-      <c r="BA18" s="59"/>
-      <c r="BB18" s="59"/>
-      <c r="BC18" s="59"/>
-      <c r="BD18" s="59"/>
-      <c r="BE18" s="59"/>
-      <c r="BF18" s="59"/>
-      <c r="BG18" s="59"/>
-      <c r="BH18" s="59"/>
-      <c r="BI18" s="59"/>
-      <c r="BJ18" s="59"/>
-      <c r="BK18" s="59"/>
-      <c r="BL18" s="59"/>
-      <c r="BM18" s="60"/>
-      <c r="BN18" s="70" t="s">
+      <c r="B18" s="41" t="s">
+        <v>866</v>
+      </c>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="42"/>
+      <c r="Q18" s="42"/>
+      <c r="R18" s="42"/>
+      <c r="S18" s="42"/>
+      <c r="T18" s="42"/>
+      <c r="U18" s="42"/>
+      <c r="V18" s="42"/>
+      <c r="W18" s="42"/>
+      <c r="X18" s="42"/>
+      <c r="Y18" s="42"/>
+      <c r="Z18" s="42"/>
+      <c r="AA18" s="42"/>
+      <c r="AB18" s="42"/>
+      <c r="AC18" s="42"/>
+      <c r="AD18" s="42"/>
+      <c r="AE18" s="42"/>
+      <c r="AF18" s="42"/>
+      <c r="AG18" s="42"/>
+      <c r="AH18" s="42"/>
+      <c r="AI18" s="42"/>
+      <c r="AJ18" s="42"/>
+      <c r="AK18" s="42"/>
+      <c r="AL18" s="42"/>
+      <c r="AM18" s="42"/>
+      <c r="AN18" s="42"/>
+      <c r="AO18" s="42"/>
+      <c r="AP18" s="42"/>
+      <c r="AQ18" s="42"/>
+      <c r="AR18" s="42"/>
+      <c r="AS18" s="42"/>
+      <c r="AT18" s="42"/>
+      <c r="AU18" s="42"/>
+      <c r="AV18" s="42"/>
+      <c r="AW18" s="42"/>
+      <c r="AX18" s="42"/>
+      <c r="AY18" s="42"/>
+      <c r="AZ18" s="42"/>
+      <c r="BA18" s="42"/>
+      <c r="BB18" s="42"/>
+      <c r="BC18" s="42"/>
+      <c r="BD18" s="42"/>
+      <c r="BE18" s="42"/>
+      <c r="BF18" s="42"/>
+      <c r="BG18" s="42"/>
+      <c r="BH18" s="42"/>
+      <c r="BI18" s="42"/>
+      <c r="BJ18" s="42"/>
+      <c r="BK18" s="42"/>
+      <c r="BL18" s="42"/>
+      <c r="BM18" s="43"/>
+      <c r="BN18" s="69" t="s">
         <v>765</v>
       </c>
-      <c r="BO18" s="70" t="s">
+      <c r="BO18" s="69" t="s">
         <v>766</v>
       </c>
-      <c r="BP18" s="70" t="s">
+      <c r="BP18" s="69" t="s">
         <v>843</v>
       </c>
-      <c r="BQ18" s="70" t="s">
+      <c r="BQ18" s="69" t="s">
         <v>585</v>
       </c>
-      <c r="BR18" s="70" t="s">
+      <c r="BR18" s="69" t="s">
         <v>586</v>
       </c>
       <c r="BS18" s="30"/>
-      <c r="BT18" s="94" t="s">
+      <c r="BT18" s="93" t="s">
         <v>819</v>
       </c>
-      <c r="BU18" s="94"/>
+      <c r="BU18" s="93"/>
     </row>
     <row r="19" spans="1:73" ht="11.25" customHeight="1">
-      <c r="B19" s="61"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="62"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="62"/>
-      <c r="K19" s="62"/>
-      <c r="L19" s="62"/>
-      <c r="M19" s="62"/>
-      <c r="N19" s="62"/>
-      <c r="O19" s="62"/>
-      <c r="P19" s="62"/>
-      <c r="Q19" s="62"/>
-      <c r="R19" s="62"/>
-      <c r="S19" s="62"/>
-      <c r="T19" s="62"/>
-      <c r="U19" s="62"/>
-      <c r="V19" s="62"/>
-      <c r="W19" s="62"/>
-      <c r="X19" s="62"/>
-      <c r="Y19" s="62"/>
-      <c r="Z19" s="62"/>
-      <c r="AA19" s="62"/>
-      <c r="AB19" s="62"/>
-      <c r="AC19" s="62"/>
-      <c r="AD19" s="62"/>
-      <c r="AE19" s="62"/>
-      <c r="AF19" s="62"/>
-      <c r="AG19" s="62"/>
-      <c r="AH19" s="62"/>
-      <c r="AI19" s="62"/>
-      <c r="AJ19" s="62"/>
-      <c r="AK19" s="62"/>
-      <c r="AL19" s="62"/>
-      <c r="AM19" s="62"/>
-      <c r="AN19" s="62"/>
-      <c r="AO19" s="62"/>
-      <c r="AP19" s="62"/>
-      <c r="AQ19" s="62"/>
-      <c r="AR19" s="62"/>
-      <c r="AS19" s="62"/>
-      <c r="AT19" s="62"/>
-      <c r="AU19" s="62"/>
-      <c r="AV19" s="62"/>
-      <c r="AW19" s="62"/>
-      <c r="AX19" s="62"/>
-      <c r="AY19" s="62"/>
-      <c r="AZ19" s="62"/>
-      <c r="BA19" s="62"/>
-      <c r="BB19" s="62"/>
-      <c r="BC19" s="62"/>
-      <c r="BD19" s="62"/>
-      <c r="BE19" s="62"/>
-      <c r="BF19" s="62"/>
-      <c r="BG19" s="62"/>
-      <c r="BH19" s="62"/>
-      <c r="BI19" s="62"/>
-      <c r="BJ19" s="62"/>
-      <c r="BK19" s="62"/>
-      <c r="BL19" s="62"/>
-      <c r="BM19" s="63"/>
-      <c r="BN19" s="70"/>
-      <c r="BO19" s="70"/>
-      <c r="BP19" s="70"/>
-      <c r="BQ19" s="70"/>
-      <c r="BR19" s="70"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="45"/>
+      <c r="P19" s="45"/>
+      <c r="Q19" s="45"/>
+      <c r="R19" s="45"/>
+      <c r="S19" s="45"/>
+      <c r="T19" s="45"/>
+      <c r="U19" s="45"/>
+      <c r="V19" s="45"/>
+      <c r="W19" s="45"/>
+      <c r="X19" s="45"/>
+      <c r="Y19" s="45"/>
+      <c r="Z19" s="45"/>
+      <c r="AA19" s="45"/>
+      <c r="AB19" s="45"/>
+      <c r="AC19" s="45"/>
+      <c r="AD19" s="45"/>
+      <c r="AE19" s="45"/>
+      <c r="AF19" s="45"/>
+      <c r="AG19" s="45"/>
+      <c r="AH19" s="45"/>
+      <c r="AI19" s="45"/>
+      <c r="AJ19" s="45"/>
+      <c r="AK19" s="45"/>
+      <c r="AL19" s="45"/>
+      <c r="AM19" s="45"/>
+      <c r="AN19" s="45"/>
+      <c r="AO19" s="45"/>
+      <c r="AP19" s="45"/>
+      <c r="AQ19" s="45"/>
+      <c r="AR19" s="45"/>
+      <c r="AS19" s="45"/>
+      <c r="AT19" s="45"/>
+      <c r="AU19" s="45"/>
+      <c r="AV19" s="45"/>
+      <c r="AW19" s="45"/>
+      <c r="AX19" s="45"/>
+      <c r="AY19" s="45"/>
+      <c r="AZ19" s="45"/>
+      <c r="BA19" s="45"/>
+      <c r="BB19" s="45"/>
+      <c r="BC19" s="45"/>
+      <c r="BD19" s="45"/>
+      <c r="BE19" s="45"/>
+      <c r="BF19" s="45"/>
+      <c r="BG19" s="45"/>
+      <c r="BH19" s="45"/>
+      <c r="BI19" s="45"/>
+      <c r="BJ19" s="45"/>
+      <c r="BK19" s="45"/>
+      <c r="BL19" s="45"/>
+      <c r="BM19" s="46"/>
+      <c r="BN19" s="69"/>
+      <c r="BO19" s="69"/>
+      <c r="BP19" s="69"/>
+      <c r="BQ19" s="69"/>
+      <c r="BR19" s="69"/>
       <c r="BS19" s="31"/>
-      <c r="BT19" s="94"/>
-      <c r="BU19" s="94"/>
+      <c r="BT19" s="93"/>
+      <c r="BU19" s="93"/>
     </row>
     <row r="20" spans="1:73" ht="11.25" customHeight="1">
-      <c r="B20" s="64"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="65"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="65"/>
-      <c r="M20" s="65"/>
-      <c r="N20" s="65"/>
-      <c r="O20" s="65"/>
-      <c r="P20" s="65"/>
-      <c r="Q20" s="65"/>
-      <c r="R20" s="65"/>
-      <c r="S20" s="65"/>
-      <c r="T20" s="65"/>
-      <c r="U20" s="65"/>
-      <c r="V20" s="65"/>
-      <c r="W20" s="65"/>
-      <c r="X20" s="65"/>
-      <c r="Y20" s="65"/>
-      <c r="Z20" s="65"/>
-      <c r="AA20" s="65"/>
-      <c r="AB20" s="65"/>
-      <c r="AC20" s="65"/>
-      <c r="AD20" s="65"/>
-      <c r="AE20" s="65"/>
-      <c r="AF20" s="65"/>
-      <c r="AG20" s="65"/>
-      <c r="AH20" s="65"/>
-      <c r="AI20" s="65"/>
-      <c r="AJ20" s="65"/>
-      <c r="AK20" s="65"/>
-      <c r="AL20" s="65"/>
-      <c r="AM20" s="65"/>
-      <c r="AN20" s="65"/>
-      <c r="AO20" s="65"/>
-      <c r="AP20" s="65"/>
-      <c r="AQ20" s="65"/>
-      <c r="AR20" s="65"/>
-      <c r="AS20" s="65"/>
-      <c r="AT20" s="65"/>
-      <c r="AU20" s="65"/>
-      <c r="AV20" s="65"/>
-      <c r="AW20" s="65"/>
-      <c r="AX20" s="65"/>
-      <c r="AY20" s="65"/>
-      <c r="AZ20" s="65"/>
-      <c r="BA20" s="65"/>
-      <c r="BB20" s="65"/>
-      <c r="BC20" s="65"/>
-      <c r="BD20" s="65"/>
-      <c r="BE20" s="65"/>
-      <c r="BF20" s="65"/>
-      <c r="BG20" s="65"/>
-      <c r="BH20" s="65"/>
-      <c r="BI20" s="65"/>
-      <c r="BJ20" s="65"/>
-      <c r="BK20" s="65"/>
-      <c r="BL20" s="65"/>
-      <c r="BM20" s="66"/>
-      <c r="BN20" s="70"/>
-      <c r="BO20" s="70"/>
-      <c r="BP20" s="70"/>
-      <c r="BQ20" s="70"/>
-      <c r="BR20" s="70"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
+      <c r="R20" s="48"/>
+      <c r="S20" s="48"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="48"/>
+      <c r="V20" s="48"/>
+      <c r="W20" s="48"/>
+      <c r="X20" s="48"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="48"/>
+      <c r="AA20" s="48"/>
+      <c r="AB20" s="48"/>
+      <c r="AC20" s="48"/>
+      <c r="AD20" s="48"/>
+      <c r="AE20" s="48"/>
+      <c r="AF20" s="48"/>
+      <c r="AG20" s="48"/>
+      <c r="AH20" s="48"/>
+      <c r="AI20" s="48"/>
+      <c r="AJ20" s="48"/>
+      <c r="AK20" s="48"/>
+      <c r="AL20" s="48"/>
+      <c r="AM20" s="48"/>
+      <c r="AN20" s="48"/>
+      <c r="AO20" s="48"/>
+      <c r="AP20" s="48"/>
+      <c r="AQ20" s="48"/>
+      <c r="AR20" s="48"/>
+      <c r="AS20" s="48"/>
+      <c r="AT20" s="48"/>
+      <c r="AU20" s="48"/>
+      <c r="AV20" s="48"/>
+      <c r="AW20" s="48"/>
+      <c r="AX20" s="48"/>
+      <c r="AY20" s="48"/>
+      <c r="AZ20" s="48"/>
+      <c r="BA20" s="48"/>
+      <c r="BB20" s="48"/>
+      <c r="BC20" s="48"/>
+      <c r="BD20" s="48"/>
+      <c r="BE20" s="48"/>
+      <c r="BF20" s="48"/>
+      <c r="BG20" s="48"/>
+      <c r="BH20" s="48"/>
+      <c r="BI20" s="48"/>
+      <c r="BJ20" s="48"/>
+      <c r="BK20" s="48"/>
+      <c r="BL20" s="48"/>
+      <c r="BM20" s="49"/>
+      <c r="BN20" s="69"/>
+      <c r="BO20" s="69"/>
+      <c r="BP20" s="69"/>
+      <c r="BQ20" s="69"/>
+      <c r="BR20" s="69"/>
       <c r="BS20" s="32"/>
-      <c r="BT20" s="94"/>
-      <c r="BU20" s="94"/>
+      <c r="BT20" s="93"/>
+      <c r="BU20" s="93"/>
     </row>
     <row r="21" spans="1:73" s="29" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A21" s="74" t="s">
+      <c r="A21" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="73" t="s">
+      <c r="B21" s="72" t="s">
         <v>448</v>
       </c>
-      <c r="C21" s="73" t="s">
+      <c r="C21" s="72" t="s">
         <v>498</v>
       </c>
-      <c r="D21" s="73" t="s">
+      <c r="D21" s="72" t="s">
         <v>499</v>
       </c>
-      <c r="E21" s="73" t="s">
+      <c r="E21" s="72" t="s">
         <v>675</v>
       </c>
-      <c r="F21" s="73" t="s">
+      <c r="F21" s="72" t="s">
         <v>676</v>
       </c>
-      <c r="G21" s="73" t="s">
+      <c r="G21" s="72" t="s">
         <v>677</v>
       </c>
-      <c r="H21" s="73" t="s">
+      <c r="H21" s="72" t="s">
         <v>678</v>
       </c>
-      <c r="I21" s="73" t="s">
+      <c r="I21" s="72" t="s">
         <v>679</v>
       </c>
-      <c r="J21" s="73" t="s">
+      <c r="J21" s="72" t="s">
         <v>681</v>
       </c>
-      <c r="K21" s="73" t="s">
+      <c r="K21" s="72" t="s">
         <v>682</v>
       </c>
-      <c r="L21" s="73" t="s">
+      <c r="L21" s="72" t="s">
         <v>686</v>
       </c>
-      <c r="M21" s="73" t="s">
+      <c r="M21" s="72" t="s">
         <v>680</v>
       </c>
-      <c r="N21" s="73" t="s">
+      <c r="N21" s="72" t="s">
         <v>683</v>
       </c>
-      <c r="O21" s="73" t="s">
+      <c r="O21" s="72" t="s">
         <v>684</v>
       </c>
-      <c r="P21" s="73" t="s">
+      <c r="P21" s="72" t="s">
         <v>685</v>
       </c>
-      <c r="Q21" s="73" t="s">
+      <c r="Q21" s="72" t="s">
         <v>687</v>
       </c>
-      <c r="R21" s="73" t="s">
+      <c r="R21" s="72" t="s">
         <v>688</v>
       </c>
-      <c r="S21" s="73" t="s">
+      <c r="S21" s="72" t="s">
         <v>689</v>
       </c>
-      <c r="T21" s="73" t="s">
+      <c r="T21" s="72" t="s">
         <v>690</v>
       </c>
-      <c r="U21" s="73" t="s">
+      <c r="U21" s="72" t="s">
         <v>691</v>
       </c>
       <c r="V21" s="89" t="s">
@@ -16151,7 +16145,7 @@
       <c r="W21" s="89" t="s">
         <v>746</v>
       </c>
-      <c r="X21" s="73" t="s">
+      <c r="X21" s="72" t="s">
         <v>755</v>
       </c>
       <c r="Y21" s="89" t="s">
@@ -16160,49 +16154,49 @@
       <c r="Z21" s="89" t="s">
         <v>748</v>
       </c>
-      <c r="AA21" s="73" t="s">
+      <c r="AA21" s="72" t="s">
+        <v>864</v>
+      </c>
+      <c r="AB21" s="72" t="s">
         <v>865</v>
       </c>
-      <c r="AB21" s="73" t="s">
-        <v>866</v>
-      </c>
-      <c r="AC21" s="73" t="s">
+      <c r="AC21" s="72" t="s">
         <v>745</v>
       </c>
-      <c r="AD21" s="91" t="s">
+      <c r="AD21" s="94" t="s">
         <v>723</v>
       </c>
-      <c r="AE21" s="73" t="s">
+      <c r="AE21" s="72" t="s">
         <v>719</v>
       </c>
-      <c r="AF21" s="73" t="s">
+      <c r="AF21" s="72" t="s">
         <v>720</v>
       </c>
-      <c r="AG21" s="73" t="s">
+      <c r="AG21" s="72" t="s">
         <v>751</v>
       </c>
-      <c r="AH21" s="73" t="s">
+      <c r="AH21" s="72" t="s">
         <v>721</v>
       </c>
-      <c r="AI21" s="73" t="s">
+      <c r="AI21" s="72" t="s">
         <v>722</v>
       </c>
-      <c r="AJ21" s="73" t="s">
+      <c r="AJ21" s="72" t="s">
         <v>724</v>
       </c>
-      <c r="AK21" s="73" t="s">
+      <c r="AK21" s="72" t="s">
         <v>725</v>
       </c>
-      <c r="AL21" s="73" t="s">
+      <c r="AL21" s="72" t="s">
         <v>726</v>
       </c>
-      <c r="AM21" s="73" t="s">
+      <c r="AM21" s="72" t="s">
         <v>727</v>
       </c>
-      <c r="AN21" s="73" t="s">
+      <c r="AN21" s="72" t="s">
         <v>753</v>
       </c>
-      <c r="AO21" s="73" t="s">
+      <c r="AO21" s="72" t="s">
         <v>758</v>
       </c>
       <c r="AP21" s="89" t="s">
@@ -16211,16 +16205,16 @@
       <c r="AQ21" s="89" t="s">
         <v>825</v>
       </c>
-      <c r="AR21" s="73" t="s">
+      <c r="AR21" s="72" t="s">
         <v>728</v>
       </c>
-      <c r="AS21" s="73" t="s">
+      <c r="AS21" s="72" t="s">
         <v>729</v>
       </c>
-      <c r="AT21" s="73" t="s">
+      <c r="AT21" s="72" t="s">
         <v>752</v>
       </c>
-      <c r="AU21" s="73" t="s">
+      <c r="AU21" s="72" t="s">
         <v>759</v>
       </c>
       <c r="AV21" s="89" t="s">
@@ -16229,13 +16223,13 @@
       <c r="AW21" s="89" t="s">
         <v>823</v>
       </c>
-      <c r="AX21" s="73" t="s">
+      <c r="AX21" s="72" t="s">
         <v>730</v>
       </c>
-      <c r="AY21" s="73" t="s">
+      <c r="AY21" s="72" t="s">
         <v>731</v>
       </c>
-      <c r="AZ21" s="73" t="s">
+      <c r="AZ21" s="72" t="s">
         <v>754</v>
       </c>
       <c r="BA21" s="89" t="s">
@@ -16244,357 +16238,357 @@
       <c r="BB21" s="89" t="s">
         <v>757</v>
       </c>
-      <c r="BC21" s="73" t="s">
+      <c r="BC21" s="72" t="s">
         <v>733</v>
       </c>
-      <c r="BD21" s="73" t="s">
+      <c r="BD21" s="72" t="s">
         <v>732</v>
       </c>
-      <c r="BE21" s="73" t="s">
+      <c r="BE21" s="72" t="s">
         <v>735</v>
       </c>
-      <c r="BF21" s="73" t="s">
+      <c r="BF21" s="72" t="s">
         <v>744</v>
       </c>
-      <c r="BG21" s="73" t="s">
+      <c r="BG21" s="72" t="s">
         <v>761</v>
       </c>
-      <c r="BH21" s="73" t="s">
+      <c r="BH21" s="72" t="s">
         <v>760</v>
       </c>
-      <c r="BI21" s="73" t="s">
+      <c r="BI21" s="72" t="s">
         <v>535</v>
       </c>
-      <c r="BJ21" s="73" t="s">
+      <c r="BJ21" s="72" t="s">
         <v>749</v>
       </c>
-      <c r="BK21" s="73" t="s">
+      <c r="BK21" s="72" t="s">
         <v>750</v>
       </c>
-      <c r="BL21" s="88" t="s">
+      <c r="BL21" s="91" t="s">
         <v>816</v>
       </c>
-      <c r="BM21" s="34"/>
-      <c r="BN21" s="74" t="s">
+      <c r="BM21" s="33"/>
+      <c r="BN21" s="82" t="s">
         <v>764</v>
       </c>
-      <c r="BO21" s="74" t="s">
+      <c r="BO21" s="82" t="s">
         <v>763</v>
       </c>
-      <c r="BP21" s="74" t="s">
+      <c r="BP21" s="82" t="s">
         <v>762</v>
       </c>
-      <c r="BQ21" s="74" t="s">
+      <c r="BQ21" s="82" t="s">
         <v>562</v>
       </c>
-      <c r="BR21" s="78" t="s">
+      <c r="BR21" s="83" t="s">
         <v>563</v>
       </c>
-      <c r="BS21" s="73" t="s">
+      <c r="BS21" s="72" t="s">
         <v>784</v>
       </c>
-      <c r="BT21" s="94"/>
-      <c r="BU21" s="94"/>
+      <c r="BT21" s="93"/>
+      <c r="BU21" s="93"/>
     </row>
     <row r="22" spans="1:73" s="29" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A22" s="74"/>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="74"/>
-      <c r="L22" s="74"/>
-      <c r="M22" s="74"/>
-      <c r="N22" s="74"/>
-      <c r="O22" s="74"/>
-      <c r="P22" s="74"/>
-      <c r="Q22" s="74"/>
-      <c r="R22" s="74"/>
-      <c r="S22" s="74"/>
-      <c r="T22" s="74"/>
-      <c r="U22" s="74"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="82"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="82"/>
+      <c r="I22" s="82"/>
+      <c r="J22" s="82"/>
+      <c r="K22" s="82"/>
+      <c r="L22" s="82"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="82"/>
+      <c r="O22" s="82"/>
+      <c r="P22" s="82"/>
+      <c r="Q22" s="82"/>
+      <c r="R22" s="82"/>
+      <c r="S22" s="82"/>
+      <c r="T22" s="82"/>
+      <c r="U22" s="82"/>
       <c r="V22" s="90"/>
       <c r="W22" s="90"/>
-      <c r="X22" s="74"/>
+      <c r="X22" s="82"/>
       <c r="Y22" s="90"/>
       <c r="Z22" s="90"/>
-      <c r="AA22" s="74"/>
-      <c r="AB22" s="74"/>
-      <c r="AC22" s="74"/>
-      <c r="AD22" s="92"/>
-      <c r="AE22" s="74"/>
-      <c r="AF22" s="74"/>
-      <c r="AG22" s="74"/>
-      <c r="AH22" s="74"/>
-      <c r="AI22" s="74"/>
-      <c r="AJ22" s="74"/>
-      <c r="AK22" s="74"/>
-      <c r="AL22" s="74"/>
-      <c r="AM22" s="74"/>
-      <c r="AN22" s="74"/>
-      <c r="AO22" s="74"/>
+      <c r="AA22" s="82"/>
+      <c r="AB22" s="82"/>
+      <c r="AC22" s="82"/>
+      <c r="AD22" s="95"/>
+      <c r="AE22" s="82"/>
+      <c r="AF22" s="82"/>
+      <c r="AG22" s="82"/>
+      <c r="AH22" s="82"/>
+      <c r="AI22" s="82"/>
+      <c r="AJ22" s="82"/>
+      <c r="AK22" s="82"/>
+      <c r="AL22" s="82"/>
+      <c r="AM22" s="82"/>
+      <c r="AN22" s="82"/>
+      <c r="AO22" s="82"/>
       <c r="AP22" s="90"/>
       <c r="AQ22" s="90"/>
-      <c r="AR22" s="74"/>
-      <c r="AS22" s="74"/>
-      <c r="AT22" s="74"/>
-      <c r="AU22" s="74"/>
+      <c r="AR22" s="82"/>
+      <c r="AS22" s="82"/>
+      <c r="AT22" s="82"/>
+      <c r="AU22" s="82"/>
       <c r="AV22" s="90"/>
       <c r="AW22" s="90"/>
-      <c r="AX22" s="74"/>
-      <c r="AY22" s="74"/>
-      <c r="AZ22" s="74"/>
+      <c r="AX22" s="82"/>
+      <c r="AY22" s="82"/>
+      <c r="AZ22" s="82"/>
       <c r="BA22" s="90"/>
       <c r="BB22" s="90"/>
-      <c r="BC22" s="74"/>
-      <c r="BD22" s="74"/>
-      <c r="BE22" s="74"/>
-      <c r="BF22" s="74"/>
-      <c r="BG22" s="74"/>
-      <c r="BH22" s="74"/>
-      <c r="BI22" s="74"/>
-      <c r="BJ22" s="74"/>
-      <c r="BK22" s="74"/>
-      <c r="BL22" s="88"/>
-      <c r="BM22" s="34"/>
-      <c r="BN22" s="74"/>
-      <c r="BO22" s="74"/>
-      <c r="BP22" s="74"/>
-      <c r="BQ22" s="74"/>
-      <c r="BR22" s="78"/>
-      <c r="BS22" s="74"/>
-      <c r="BT22" s="94"/>
-      <c r="BU22" s="94"/>
+      <c r="BC22" s="82"/>
+      <c r="BD22" s="82"/>
+      <c r="BE22" s="82"/>
+      <c r="BF22" s="82"/>
+      <c r="BG22" s="82"/>
+      <c r="BH22" s="82"/>
+      <c r="BI22" s="82"/>
+      <c r="BJ22" s="82"/>
+      <c r="BK22" s="82"/>
+      <c r="BL22" s="91"/>
+      <c r="BM22" s="33"/>
+      <c r="BN22" s="82"/>
+      <c r="BO22" s="82"/>
+      <c r="BP22" s="82"/>
+      <c r="BQ22" s="82"/>
+      <c r="BR22" s="83"/>
+      <c r="BS22" s="82"/>
+      <c r="BT22" s="93"/>
+      <c r="BU22" s="93"/>
     </row>
     <row r="23" spans="1:73" s="29" customFormat="1">
-      <c r="A23" s="74"/>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
-      <c r="I23" s="74"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="74"/>
-      <c r="L23" s="74"/>
-      <c r="M23" s="74"/>
-      <c r="N23" s="74"/>
-      <c r="O23" s="74"/>
-      <c r="P23" s="74"/>
-      <c r="Q23" s="74"/>
-      <c r="R23" s="74"/>
-      <c r="S23" s="74"/>
-      <c r="T23" s="74"/>
-      <c r="U23" s="74"/>
+      <c r="A23" s="71"/>
+      <c r="B23" s="82"/>
+      <c r="C23" s="82"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="82"/>
+      <c r="G23" s="82"/>
+      <c r="H23" s="82"/>
+      <c r="I23" s="82"/>
+      <c r="J23" s="82"/>
+      <c r="K23" s="82"/>
+      <c r="L23" s="82"/>
+      <c r="M23" s="82"/>
+      <c r="N23" s="82"/>
+      <c r="O23" s="82"/>
+      <c r="P23" s="82"/>
+      <c r="Q23" s="82"/>
+      <c r="R23" s="82"/>
+      <c r="S23" s="82"/>
+      <c r="T23" s="82"/>
+      <c r="U23" s="82"/>
       <c r="V23" s="90"/>
       <c r="W23" s="90"/>
-      <c r="X23" s="74"/>
+      <c r="X23" s="82"/>
       <c r="Y23" s="90"/>
       <c r="Z23" s="90"/>
-      <c r="AA23" s="74"/>
-      <c r="AB23" s="74"/>
-      <c r="AC23" s="74"/>
-      <c r="AD23" s="92"/>
-      <c r="AE23" s="74"/>
-      <c r="AF23" s="74"/>
-      <c r="AG23" s="74"/>
-      <c r="AH23" s="74"/>
-      <c r="AI23" s="74"/>
-      <c r="AJ23" s="74"/>
-      <c r="AK23" s="74"/>
-      <c r="AL23" s="74"/>
-      <c r="AM23" s="74"/>
-      <c r="AN23" s="74"/>
-      <c r="AO23" s="74"/>
+      <c r="AA23" s="82"/>
+      <c r="AB23" s="82"/>
+      <c r="AC23" s="82"/>
+      <c r="AD23" s="95"/>
+      <c r="AE23" s="82"/>
+      <c r="AF23" s="82"/>
+      <c r="AG23" s="82"/>
+      <c r="AH23" s="82"/>
+      <c r="AI23" s="82"/>
+      <c r="AJ23" s="82"/>
+      <c r="AK23" s="82"/>
+      <c r="AL23" s="82"/>
+      <c r="AM23" s="82"/>
+      <c r="AN23" s="82"/>
+      <c r="AO23" s="82"/>
       <c r="AP23" s="90"/>
       <c r="AQ23" s="90"/>
-      <c r="AR23" s="74"/>
-      <c r="AS23" s="74"/>
-      <c r="AT23" s="74"/>
-      <c r="AU23" s="74"/>
+      <c r="AR23" s="82"/>
+      <c r="AS23" s="82"/>
+      <c r="AT23" s="82"/>
+      <c r="AU23" s="82"/>
       <c r="AV23" s="90"/>
       <c r="AW23" s="90"/>
-      <c r="AX23" s="74"/>
-      <c r="AY23" s="74"/>
-      <c r="AZ23" s="74"/>
+      <c r="AX23" s="82"/>
+      <c r="AY23" s="82"/>
+      <c r="AZ23" s="82"/>
       <c r="BA23" s="90"/>
       <c r="BB23" s="90"/>
-      <c r="BC23" s="74"/>
-      <c r="BD23" s="74"/>
-      <c r="BE23" s="74"/>
-      <c r="BF23" s="74"/>
-      <c r="BG23" s="74"/>
-      <c r="BH23" s="74"/>
-      <c r="BI23" s="74"/>
-      <c r="BJ23" s="74"/>
-      <c r="BK23" s="74"/>
-      <c r="BL23" s="88"/>
-      <c r="BM23" s="34"/>
-      <c r="BN23" s="74"/>
-      <c r="BO23" s="74"/>
-      <c r="BP23" s="74"/>
-      <c r="BQ23" s="74"/>
-      <c r="BR23" s="78"/>
-      <c r="BS23" s="74"/>
-      <c r="BT23" s="94"/>
-      <c r="BU23" s="94"/>
+      <c r="BC23" s="82"/>
+      <c r="BD23" s="82"/>
+      <c r="BE23" s="82"/>
+      <c r="BF23" s="82"/>
+      <c r="BG23" s="82"/>
+      <c r="BH23" s="82"/>
+      <c r="BI23" s="82"/>
+      <c r="BJ23" s="82"/>
+      <c r="BK23" s="82"/>
+      <c r="BL23" s="91"/>
+      <c r="BM23" s="33"/>
+      <c r="BN23" s="82"/>
+      <c r="BO23" s="82"/>
+      <c r="BP23" s="82"/>
+      <c r="BQ23" s="82"/>
+      <c r="BR23" s="83"/>
+      <c r="BS23" s="82"/>
+      <c r="BT23" s="93"/>
+      <c r="BU23" s="93"/>
     </row>
     <row r="24" spans="1:73" s="29" customFormat="1">
-      <c r="A24" s="74"/>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="74"/>
-      <c r="J24" s="74"/>
-      <c r="K24" s="74"/>
-      <c r="L24" s="74"/>
-      <c r="M24" s="74"/>
-      <c r="N24" s="74"/>
-      <c r="O24" s="74"/>
-      <c r="P24" s="74"/>
-      <c r="Q24" s="74"/>
-      <c r="R24" s="74"/>
-      <c r="S24" s="74"/>
-      <c r="T24" s="74"/>
-      <c r="U24" s="74"/>
+      <c r="A24" s="71"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="82"/>
+      <c r="G24" s="82"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="82"/>
+      <c r="J24" s="82"/>
+      <c r="K24" s="82"/>
+      <c r="L24" s="82"/>
+      <c r="M24" s="82"/>
+      <c r="N24" s="82"/>
+      <c r="O24" s="82"/>
+      <c r="P24" s="82"/>
+      <c r="Q24" s="82"/>
+      <c r="R24" s="82"/>
+      <c r="S24" s="82"/>
+      <c r="T24" s="82"/>
+      <c r="U24" s="82"/>
       <c r="V24" s="90"/>
       <c r="W24" s="90"/>
-      <c r="X24" s="74"/>
+      <c r="X24" s="82"/>
       <c r="Y24" s="90"/>
       <c r="Z24" s="90"/>
-      <c r="AA24" s="74"/>
-      <c r="AB24" s="74"/>
-      <c r="AC24" s="74"/>
-      <c r="AD24" s="92"/>
-      <c r="AE24" s="74"/>
-      <c r="AF24" s="74"/>
-      <c r="AG24" s="74"/>
-      <c r="AH24" s="74"/>
-      <c r="AI24" s="74"/>
-      <c r="AJ24" s="74"/>
-      <c r="AK24" s="74"/>
-      <c r="AL24" s="74"/>
-      <c r="AM24" s="74"/>
-      <c r="AN24" s="74"/>
-      <c r="AO24" s="74"/>
+      <c r="AA24" s="82"/>
+      <c r="AB24" s="82"/>
+      <c r="AC24" s="82"/>
+      <c r="AD24" s="95"/>
+      <c r="AE24" s="82"/>
+      <c r="AF24" s="82"/>
+      <c r="AG24" s="82"/>
+      <c r="AH24" s="82"/>
+      <c r="AI24" s="82"/>
+      <c r="AJ24" s="82"/>
+      <c r="AK24" s="82"/>
+      <c r="AL24" s="82"/>
+      <c r="AM24" s="82"/>
+      <c r="AN24" s="82"/>
+      <c r="AO24" s="82"/>
       <c r="AP24" s="90"/>
       <c r="AQ24" s="90"/>
-      <c r="AR24" s="74"/>
-      <c r="AS24" s="74"/>
-      <c r="AT24" s="74"/>
-      <c r="AU24" s="74"/>
+      <c r="AR24" s="82"/>
+      <c r="AS24" s="82"/>
+      <c r="AT24" s="82"/>
+      <c r="AU24" s="82"/>
       <c r="AV24" s="90"/>
       <c r="AW24" s="90"/>
-      <c r="AX24" s="74"/>
-      <c r="AY24" s="74"/>
-      <c r="AZ24" s="74"/>
+      <c r="AX24" s="82"/>
+      <c r="AY24" s="82"/>
+      <c r="AZ24" s="82"/>
       <c r="BA24" s="90"/>
       <c r="BB24" s="90"/>
-      <c r="BC24" s="74"/>
-      <c r="BD24" s="74"/>
-      <c r="BE24" s="74"/>
-      <c r="BF24" s="74"/>
-      <c r="BG24" s="74"/>
-      <c r="BH24" s="74"/>
-      <c r="BI24" s="74"/>
-      <c r="BJ24" s="74"/>
-      <c r="BK24" s="74"/>
-      <c r="BL24" s="88"/>
-      <c r="BM24" s="34"/>
-      <c r="BN24" s="74"/>
-      <c r="BO24" s="74"/>
-      <c r="BP24" s="74"/>
-      <c r="BQ24" s="74"/>
-      <c r="BR24" s="78"/>
-      <c r="BS24" s="74"/>
-      <c r="BT24" s="94"/>
-      <c r="BU24" s="94"/>
+      <c r="BC24" s="82"/>
+      <c r="BD24" s="82"/>
+      <c r="BE24" s="82"/>
+      <c r="BF24" s="82"/>
+      <c r="BG24" s="82"/>
+      <c r="BH24" s="82"/>
+      <c r="BI24" s="82"/>
+      <c r="BJ24" s="82"/>
+      <c r="BK24" s="82"/>
+      <c r="BL24" s="91"/>
+      <c r="BM24" s="33"/>
+      <c r="BN24" s="82"/>
+      <c r="BO24" s="82"/>
+      <c r="BP24" s="82"/>
+      <c r="BQ24" s="82"/>
+      <c r="BR24" s="83"/>
+      <c r="BS24" s="82"/>
+      <c r="BT24" s="93"/>
+      <c r="BU24" s="93"/>
     </row>
     <row r="25" spans="1:73" s="29" customFormat="1">
-      <c r="A25" s="74"/>
-      <c r="B25" s="74"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="74"/>
-      <c r="I25" s="74"/>
-      <c r="J25" s="74"/>
-      <c r="K25" s="74"/>
-      <c r="L25" s="74"/>
-      <c r="M25" s="74"/>
-      <c r="N25" s="74"/>
-      <c r="O25" s="74"/>
-      <c r="P25" s="74"/>
-      <c r="Q25" s="74"/>
-      <c r="R25" s="74"/>
-      <c r="S25" s="74"/>
-      <c r="T25" s="74"/>
-      <c r="U25" s="74"/>
+      <c r="A25" s="72"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="82"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="82"/>
+      <c r="J25" s="82"/>
+      <c r="K25" s="82"/>
+      <c r="L25" s="82"/>
+      <c r="M25" s="82"/>
+      <c r="N25" s="82"/>
+      <c r="O25" s="82"/>
+      <c r="P25" s="82"/>
+      <c r="Q25" s="82"/>
+      <c r="R25" s="82"/>
+      <c r="S25" s="82"/>
+      <c r="T25" s="82"/>
+      <c r="U25" s="82"/>
       <c r="V25" s="90"/>
       <c r="W25" s="90"/>
-      <c r="X25" s="74"/>
+      <c r="X25" s="82"/>
       <c r="Y25" s="90"/>
       <c r="Z25" s="90"/>
-      <c r="AA25" s="74"/>
-      <c r="AB25" s="74"/>
-      <c r="AC25" s="74"/>
-      <c r="AD25" s="92"/>
-      <c r="AE25" s="74"/>
-      <c r="AF25" s="74"/>
-      <c r="AG25" s="74"/>
-      <c r="AH25" s="74"/>
-      <c r="AI25" s="74"/>
-      <c r="AJ25" s="74"/>
-      <c r="AK25" s="74"/>
-      <c r="AL25" s="74"/>
-      <c r="AM25" s="74"/>
-      <c r="AN25" s="74"/>
-      <c r="AO25" s="74"/>
+      <c r="AA25" s="82"/>
+      <c r="AB25" s="82"/>
+      <c r="AC25" s="82"/>
+      <c r="AD25" s="95"/>
+      <c r="AE25" s="82"/>
+      <c r="AF25" s="82"/>
+      <c r="AG25" s="82"/>
+      <c r="AH25" s="82"/>
+      <c r="AI25" s="82"/>
+      <c r="AJ25" s="82"/>
+      <c r="AK25" s="82"/>
+      <c r="AL25" s="82"/>
+      <c r="AM25" s="82"/>
+      <c r="AN25" s="82"/>
+      <c r="AO25" s="82"/>
       <c r="AP25" s="90"/>
       <c r="AQ25" s="90"/>
-      <c r="AR25" s="74"/>
-      <c r="AS25" s="74"/>
-      <c r="AT25" s="74"/>
-      <c r="AU25" s="74"/>
+      <c r="AR25" s="82"/>
+      <c r="AS25" s="82"/>
+      <c r="AT25" s="82"/>
+      <c r="AU25" s="82"/>
       <c r="AV25" s="90"/>
       <c r="AW25" s="90"/>
-      <c r="AX25" s="74"/>
-      <c r="AY25" s="74"/>
-      <c r="AZ25" s="74"/>
+      <c r="AX25" s="82"/>
+      <c r="AY25" s="82"/>
+      <c r="AZ25" s="82"/>
       <c r="BA25" s="90"/>
       <c r="BB25" s="90"/>
-      <c r="BC25" s="74"/>
-      <c r="BD25" s="74"/>
-      <c r="BE25" s="74"/>
-      <c r="BF25" s="74"/>
-      <c r="BG25" s="74"/>
-      <c r="BH25" s="74"/>
-      <c r="BI25" s="74"/>
-      <c r="BJ25" s="74"/>
-      <c r="BK25" s="74"/>
-      <c r="BL25" s="88"/>
-      <c r="BM25" s="34"/>
-      <c r="BN25" s="74"/>
-      <c r="BO25" s="74"/>
-      <c r="BP25" s="74"/>
-      <c r="BQ25" s="74"/>
-      <c r="BR25" s="78"/>
-      <c r="BS25" s="74"/>
-      <c r="BT25" s="94"/>
-      <c r="BU25" s="94"/>
+      <c r="BC25" s="82"/>
+      <c r="BD25" s="82"/>
+      <c r="BE25" s="82"/>
+      <c r="BF25" s="82"/>
+      <c r="BG25" s="82"/>
+      <c r="BH25" s="82"/>
+      <c r="BI25" s="82"/>
+      <c r="BJ25" s="82"/>
+      <c r="BK25" s="82"/>
+      <c r="BL25" s="91"/>
+      <c r="BM25" s="33"/>
+      <c r="BN25" s="82"/>
+      <c r="BO25" s="82"/>
+      <c r="BP25" s="82"/>
+      <c r="BQ25" s="82"/>
+      <c r="BR25" s="83"/>
+      <c r="BS25" s="82"/>
+      <c r="BT25" s="93"/>
+      <c r="BU25" s="93"/>
     </row>
     <row r="26" spans="1:73" ht="11.25" customHeight="1">
       <c r="E26" s="1"/>
@@ -16630,7 +16624,7 @@
       <c r="BE26" s="12"/>
       <c r="BH26" s="1"/>
       <c r="BK26" s="6"/>
-      <c r="BL26" s="88" t="s">
+      <c r="BL26" s="91" t="s">
         <v>817</v>
       </c>
       <c r="BN26" s="1"/>
@@ -16657,7 +16651,7 @@
       <c r="Y27" s="37" t="s">
         <v>820</v>
       </c>
-      <c r="Z27" s="74" t="s">
+      <c r="Z27" s="82" t="s">
         <v>821</v>
       </c>
       <c r="AA27" s="12"/>
@@ -16668,27 +16662,27 @@
       <c r="AK27" s="12"/>
       <c r="AL27" s="1"/>
       <c r="AO27" s="12"/>
-      <c r="AP27" s="95" t="s">
+      <c r="AP27" s="88" t="s">
         <v>820</v>
       </c>
-      <c r="AQ27" s="96" t="s">
+      <c r="AQ27" s="87" t="s">
         <v>821</v>
       </c>
       <c r="AT27" s="1"/>
       <c r="AU27" s="1"/>
-      <c r="AV27" s="95" t="s">
+      <c r="AV27" s="88" t="s">
         <v>820</v>
       </c>
-      <c r="AW27" s="96" t="s">
+      <c r="AW27" s="87" t="s">
         <v>821</v>
       </c>
       <c r="AX27" s="12"/>
       <c r="AY27" s="12"/>
       <c r="AZ27" s="12"/>
-      <c r="BA27" s="95" t="s">
+      <c r="BA27" s="88" t="s">
         <v>820</v>
       </c>
-      <c r="BB27" s="96" t="s">
+      <c r="BB27" s="87" t="s">
         <v>821</v>
       </c>
       <c r="BC27" s="6"/>
@@ -16698,7 +16692,7 @@
       </c>
       <c r="BH27" s="1"/>
       <c r="BK27" s="6"/>
-      <c r="BL27" s="88"/>
+      <c r="BL27" s="91"/>
       <c r="BN27" s="1"/>
       <c r="BO27" s="4"/>
       <c r="BP27" s="6"/>
@@ -16721,7 +16715,7 @@
       <c r="T28" s="1"/>
       <c r="X28" s="6"/>
       <c r="Y28" s="37"/>
-      <c r="Z28" s="74"/>
+      <c r="Z28" s="82"/>
       <c r="AA28" s="12"/>
       <c r="AF28" s="1"/>
       <c r="AI28" s="12"/>
@@ -16730,17 +16724,17 @@
       <c r="AL28" s="1"/>
       <c r="AN28" s="1"/>
       <c r="AO28" s="6"/>
-      <c r="AP28" s="95"/>
-      <c r="AQ28" s="96"/>
+      <c r="AP28" s="88"/>
+      <c r="AQ28" s="87"/>
       <c r="AT28" s="1"/>
       <c r="AU28" s="6"/>
-      <c r="AV28" s="95"/>
-      <c r="AW28" s="96"/>
+      <c r="AV28" s="88"/>
+      <c r="AW28" s="87"/>
       <c r="AX28" s="12"/>
       <c r="AY28" s="12"/>
       <c r="AZ28" s="12"/>
-      <c r="BA28" s="95"/>
-      <c r="BB28" s="96"/>
+      <c r="BA28" s="88"/>
+      <c r="BB28" s="87"/>
       <c r="BC28" s="6"/>
       <c r="BD28" s="6"/>
       <c r="BE28" s="24" t="s">
@@ -16748,7 +16742,7 @@
       </c>
       <c r="BH28" s="1"/>
       <c r="BK28" s="6"/>
-      <c r="BL28" s="88"/>
+      <c r="BL28" s="91"/>
       <c r="BN28" s="1"/>
       <c r="BO28" s="4"/>
       <c r="BP28" s="6"/>
@@ -16789,7 +16783,7 @@
       <c r="BE29" s="12"/>
       <c r="BH29" s="1"/>
       <c r="BK29" s="6"/>
-      <c r="BL29" s="88" t="s">
+      <c r="BL29" s="91" t="s">
         <v>818</v>
       </c>
       <c r="BN29" s="1"/>
@@ -16832,7 +16826,7 @@
       <c r="BE30" s="12"/>
       <c r="BH30" s="1"/>
       <c r="BK30" s="6"/>
-      <c r="BL30" s="88"/>
+      <c r="BL30" s="91"/>
       <c r="BN30" s="1"/>
       <c r="BO30" s="4"/>
       <c r="BP30" s="6"/>
@@ -16873,7 +16867,7 @@
       <c r="BE31" s="12"/>
       <c r="BH31" s="1"/>
       <c r="BK31" s="6"/>
-      <c r="BL31" s="88"/>
+      <c r="BL31" s="91"/>
       <c r="BN31" s="1"/>
       <c r="BO31" s="4"/>
       <c r="BP31" s="6"/>
@@ -16914,7 +16908,7 @@
       <c r="BE32" s="12"/>
       <c r="BH32" s="1"/>
       <c r="BK32" s="6"/>
-      <c r="BL32" s="88"/>
+      <c r="BL32" s="91"/>
       <c r="BN32" s="1"/>
       <c r="BO32" s="4"/>
       <c r="BP32" s="6"/>
@@ -16955,7 +16949,7 @@
       <c r="BE33" s="12"/>
       <c r="BH33" s="1"/>
       <c r="BK33" s="6"/>
-      <c r="BL33" s="93"/>
+      <c r="BL33" s="92"/>
       <c r="BN33" s="1"/>
       <c r="BO33" s="4"/>
       <c r="BP33" s="6"/>
@@ -17607,26 +17601,59 @@
     </row>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="AQ27:AQ28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="Z27:Z28"/>
-    <mergeCell ref="AG21:AG25"/>
-    <mergeCell ref="BA27:BA28"/>
-    <mergeCell ref="BB27:BB28"/>
-    <mergeCell ref="AV21:AV25"/>
-    <mergeCell ref="AJ21:AJ25"/>
-    <mergeCell ref="AK21:AK25"/>
-    <mergeCell ref="AO21:AO25"/>
-    <mergeCell ref="AU21:AU25"/>
-    <mergeCell ref="AT21:AT25"/>
-    <mergeCell ref="AN21:AN25"/>
-    <mergeCell ref="AZ21:AZ25"/>
-    <mergeCell ref="AW21:AW25"/>
-    <mergeCell ref="AV27:AV28"/>
-    <mergeCell ref="AW27:AW28"/>
-    <mergeCell ref="AP21:AP25"/>
-    <mergeCell ref="AQ21:AQ25"/>
-    <mergeCell ref="AP27:AP28"/>
+    <mergeCell ref="BL21:BL25"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="BQ18:BQ20"/>
+    <mergeCell ref="BQ21:BQ25"/>
+    <mergeCell ref="BR18:BR20"/>
+    <mergeCell ref="BR21:BR25"/>
+    <mergeCell ref="BP21:BP25"/>
+    <mergeCell ref="BO21:BO25"/>
+    <mergeCell ref="BN21:BN25"/>
+    <mergeCell ref="BN18:BN20"/>
+    <mergeCell ref="BO18:BO20"/>
+    <mergeCell ref="BP18:BP20"/>
+    <mergeCell ref="X21:X25"/>
+    <mergeCell ref="BA21:BA25"/>
+    <mergeCell ref="BB21:BB25"/>
+    <mergeCell ref="K21:K25"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="W21:W25"/>
+    <mergeCell ref="AH21:AH25"/>
+    <mergeCell ref="AI21:AI25"/>
+    <mergeCell ref="AE21:AE25"/>
+    <mergeCell ref="AF21:AF25"/>
+    <mergeCell ref="AD21:AD25"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="L21:L25"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="F21:F25"/>
+    <mergeCell ref="G21:G25"/>
+    <mergeCell ref="H21:H25"/>
+    <mergeCell ref="I21:I25"/>
+    <mergeCell ref="J21:J25"/>
+    <mergeCell ref="BS21:BS25"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="Z21:Z25"/>
+    <mergeCell ref="AC21:AC25"/>
+    <mergeCell ref="AA21:AA25"/>
+    <mergeCell ref="AB21:AB25"/>
+    <mergeCell ref="BK21:BK25"/>
+    <mergeCell ref="BH21:BH25"/>
+    <mergeCell ref="BG21:BG25"/>
+    <mergeCell ref="BD21:BD25"/>
+    <mergeCell ref="BC21:BC25"/>
+    <mergeCell ref="BI21:BI25"/>
+    <mergeCell ref="BJ21:BJ25"/>
+    <mergeCell ref="M21:M25"/>
+    <mergeCell ref="E21:E25"/>
+    <mergeCell ref="O21:O25"/>
+    <mergeCell ref="P21:P25"/>
+    <mergeCell ref="N21:N25"/>
+    <mergeCell ref="Q21:Q25"/>
+    <mergeCell ref="R21:R25"/>
     <mergeCell ref="BL26:BL28"/>
     <mergeCell ref="BL29:BL33"/>
     <mergeCell ref="BT18:BU25"/>
@@ -17643,59 +17670,26 @@
     <mergeCell ref="AS21:AS25"/>
     <mergeCell ref="AX21:AX25"/>
     <mergeCell ref="AY21:AY25"/>
-    <mergeCell ref="O21:O25"/>
-    <mergeCell ref="P21:P25"/>
-    <mergeCell ref="N21:N25"/>
-    <mergeCell ref="Q21:Q25"/>
-    <mergeCell ref="R21:R25"/>
-    <mergeCell ref="BS21:BS25"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="D21:D25"/>
-    <mergeCell ref="Z21:Z25"/>
-    <mergeCell ref="AC21:AC25"/>
-    <mergeCell ref="AA21:AA25"/>
-    <mergeCell ref="AB21:AB25"/>
-    <mergeCell ref="BK21:BK25"/>
-    <mergeCell ref="BH21:BH25"/>
-    <mergeCell ref="BG21:BG25"/>
-    <mergeCell ref="BD21:BD25"/>
-    <mergeCell ref="BC21:BC25"/>
-    <mergeCell ref="BI21:BI25"/>
-    <mergeCell ref="BJ21:BJ25"/>
-    <mergeCell ref="M21:M25"/>
-    <mergeCell ref="E21:E25"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="W21:W25"/>
-    <mergeCell ref="AH21:AH25"/>
-    <mergeCell ref="AI21:AI25"/>
-    <mergeCell ref="AE21:AE25"/>
-    <mergeCell ref="AF21:AF25"/>
-    <mergeCell ref="AD21:AD25"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="L21:L25"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="F21:F25"/>
-    <mergeCell ref="G21:G25"/>
-    <mergeCell ref="H21:H25"/>
-    <mergeCell ref="I21:I25"/>
-    <mergeCell ref="J21:J25"/>
-    <mergeCell ref="BL21:BL25"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="BQ18:BQ20"/>
-    <mergeCell ref="BQ21:BQ25"/>
-    <mergeCell ref="BR18:BR20"/>
-    <mergeCell ref="BR21:BR25"/>
-    <mergeCell ref="BP21:BP25"/>
-    <mergeCell ref="BO21:BO25"/>
-    <mergeCell ref="BN21:BN25"/>
-    <mergeCell ref="BN18:BN20"/>
-    <mergeCell ref="BO18:BO20"/>
-    <mergeCell ref="BP18:BP20"/>
-    <mergeCell ref="X21:X25"/>
-    <mergeCell ref="BA21:BA25"/>
-    <mergeCell ref="BB21:BB25"/>
-    <mergeCell ref="K21:K25"/>
+    <mergeCell ref="BB27:BB28"/>
+    <mergeCell ref="AV21:AV25"/>
+    <mergeCell ref="AJ21:AJ25"/>
+    <mergeCell ref="AK21:AK25"/>
+    <mergeCell ref="AO21:AO25"/>
+    <mergeCell ref="AU21:AU25"/>
+    <mergeCell ref="AT21:AT25"/>
+    <mergeCell ref="AN21:AN25"/>
+    <mergeCell ref="AZ21:AZ25"/>
+    <mergeCell ref="AW21:AW25"/>
+    <mergeCell ref="AV27:AV28"/>
+    <mergeCell ref="AW27:AW28"/>
+    <mergeCell ref="AP21:AP25"/>
+    <mergeCell ref="AQ21:AQ25"/>
+    <mergeCell ref="AP27:AP28"/>
+    <mergeCell ref="AQ27:AQ28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="Z27:Z28"/>
+    <mergeCell ref="AG21:AG25"/>
+    <mergeCell ref="BA27:BA28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -17791,27 +17785,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:75">
-      <c r="BJ1" s="35"/>
+      <c r="BJ1" s="34"/>
       <c r="BV1" s="1"/>
       <c r="BW1" s="1"/>
     </row>
     <row r="2" spans="1:75" ht="21">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="56"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="17" t="s">
         <v>826</v>
       </c>
-      <c r="BJ2" s="35"/>
+      <c r="BJ2" s="34"/>
       <c r="BV2" s="1"/>
       <c r="BW2" s="1"/>
     </row>
     <row r="3" spans="1:75" ht="21">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="57"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="17" t="s">
         <v>860</v>
       </c>
@@ -17921,7 +17915,7 @@
       <c r="BF6" s="1"/>
       <c r="BI6" s="6"/>
       <c r="BJ6" s="12"/>
-      <c r="BL6" s="88" t="s">
+      <c r="BL6" s="91" t="s">
         <v>818</v>
       </c>
       <c r="BN6" s="1"/>
@@ -17981,7 +17975,7 @@
       <c r="BF7" s="1"/>
       <c r="BI7" s="6"/>
       <c r="BJ7" s="12"/>
-      <c r="BL7" s="88"/>
+      <c r="BL7" s="91"/>
       <c r="BN7" s="1"/>
       <c r="BO7" s="4"/>
       <c r="BP7" s="6"/>
@@ -18039,7 +18033,7 @@
       <c r="BF8" s="1"/>
       <c r="BI8" s="6"/>
       <c r="BJ8" s="12"/>
-      <c r="BL8" s="88"/>
+      <c r="BL8" s="91"/>
       <c r="BN8" s="1"/>
       <c r="BO8" s="4"/>
       <c r="BP8" s="6"/>
@@ -18097,7 +18091,7 @@
       <c r="BF9" s="1"/>
       <c r="BI9" s="6"/>
       <c r="BJ9" s="12"/>
-      <c r="BL9" s="88"/>
+      <c r="BL9" s="91"/>
       <c r="BN9" s="1"/>
       <c r="BO9" s="4"/>
       <c r="BP9" s="6"/>
@@ -18151,7 +18145,7 @@
       <c r="BI10" s="6"/>
       <c r="BJ10" s="12"/>
       <c r="BK10" s="6"/>
-      <c r="BL10" s="93"/>
+      <c r="BL10" s="92"/>
       <c r="BM10" s="12"/>
       <c r="BO10" s="4"/>
       <c r="BP10" s="6"/>
@@ -18359,18 +18353,18 @@
       <c r="BW14" s="6"/>
     </row>
     <row r="15" spans="1:75" s="1" customFormat="1">
-      <c r="A15" s="98" t="s">
+      <c r="A15" s="97" t="s">
         <v>854</v>
       </c>
-      <c r="B15" s="99"/>
-      <c r="C15" s="100"/>
-      <c r="D15" s="70" t="s">
+      <c r="B15" s="98"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="69" t="s">
         <v>856</v>
       </c>
-      <c r="E15" s="70" t="s">
+      <c r="E15" s="69" t="s">
         <v>858</v>
       </c>
-      <c r="F15" s="70" t="s">
+      <c r="F15" s="69" t="s">
         <v>858</v>
       </c>
       <c r="I15" s="6"/>
@@ -18410,12 +18404,12 @@
       <c r="BW15" s="6"/>
     </row>
     <row r="16" spans="1:75" s="1" customFormat="1">
-      <c r="A16" s="101"/>
-      <c r="B16" s="102"/>
-      <c r="C16" s="103"/>
-      <c r="D16" s="70"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
+      <c r="A16" s="100"/>
+      <c r="B16" s="101"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
@@ -18453,12 +18447,12 @@
       <c r="BW16" s="6"/>
     </row>
     <row r="17" spans="1:75" s="1" customFormat="1">
-      <c r="A17" s="104"/>
-      <c r="B17" s="105"/>
-      <c r="C17" s="106"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
+      <c r="A17" s="103"/>
+      <c r="B17" s="104"/>
+      <c r="C17" s="105"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
@@ -18742,12 +18736,12 @@
       <c r="BW23" s="6"/>
     </row>
     <row r="24" spans="1:75" s="1" customFormat="1">
-      <c r="A24" s="97" t="s">
+      <c r="A24" s="96" t="s">
         <v>861</v>
       </c>
-      <c r="B24" s="97"/>
-      <c r="C24" s="97"/>
-      <c r="D24" s="97"/>
+      <c r="B24" s="96"/>
+      <c r="C24" s="96"/>
+      <c r="D24" s="96"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
@@ -18901,7 +18895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:M77"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F75" sqref="F3:F75"/>
     </sheetView>
   </sheetViews>
@@ -19194,7 +19188,7 @@
       </c>
     </row>
     <row r="27" spans="3:6">
-      <c r="C27" s="33" t="s">
+      <c r="C27" s="27" t="s">
         <v>604</v>
       </c>
       <c r="F27" t="str">
@@ -19203,7 +19197,7 @@
       </c>
     </row>
     <row r="28" spans="3:6">
-      <c r="C28" s="33" t="s">
+      <c r="C28" s="27" t="s">
         <v>605</v>
       </c>
       <c r="F28" t="str">
@@ -19213,335 +19207,335 @@
     </row>
     <row r="29" spans="3:6">
       <c r="C29" s="27" t="s">
-        <v>625</v>
+        <v>602</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>VL_IVA,</v>
+        <v>VL_BASE_ICMS_NAO_REDUTOR,</v>
       </c>
     </row>
     <row r="30" spans="3:6">
       <c r="C30" s="27" t="s">
-        <v>351</v>
+        <v>619</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>VL_BASE_IPI,</v>
+        <v>VL_PERCENTUAL_REDUTOR_ICMS,</v>
       </c>
     </row>
     <row r="31" spans="3:6">
       <c r="C31" s="27" t="s">
-        <v>594</v>
+        <v>625</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>VL_PERCENTUAL_IPI,</v>
+        <v>VL_IVA,</v>
       </c>
     </row>
     <row r="32" spans="3:6">
       <c r="C32" s="27" t="s">
-        <v>34</v>
+        <v>351</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>VL_IPI,</v>
+        <v>VL_BASE_IPI,</v>
       </c>
     </row>
     <row r="33" spans="3:6">
       <c r="C33" s="27" t="s">
-        <v>352</v>
+        <v>594</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v>VL_IPI_DESTACADO,</v>
+        <v>VL_PERCENTUAL_IPI,</v>
       </c>
     </row>
     <row r="34" spans="3:6">
       <c r="C34" s="27" t="s">
-        <v>597</v>
+        <v>34</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v>VL_PERCENTUAL_ISS,</v>
+        <v>VL_IPI,</v>
       </c>
     </row>
     <row r="35" spans="3:6">
       <c r="C35" s="27" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>VL_ISS,</v>
+        <v>VL_IPI_DESTACADO,</v>
       </c>
     </row>
     <row r="36" spans="3:6">
       <c r="C36" s="27" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v>VL_PERCENTUAL_IRPF,</v>
+        <v>VL_PERCENTUAL_ISS,</v>
       </c>
     </row>
     <row r="37" spans="3:6">
       <c r="C37" s="27" t="s">
-        <v>599</v>
+        <v>354</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v>VL_IRPF,</v>
+        <v>VL_ISS,</v>
       </c>
     </row>
     <row r="38" spans="3:6">
       <c r="C38" s="27" t="s">
-        <v>612</v>
+        <v>598</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v>VL_PERCENTUAL_PIS,</v>
+        <v>VL_PERCENTUAL_IRPF,</v>
       </c>
     </row>
     <row r="39" spans="3:6">
       <c r="C39" s="27" t="s">
-        <v>365</v>
+        <v>599</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
-        <v>VL_PIS,</v>
+        <v>VL_IRPF,</v>
       </c>
     </row>
     <row r="40" spans="3:6">
       <c r="C40" s="27" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
-        <v>VL_PIS_MERCADORIA,</v>
+        <v>VL_PERCENTUAL_PIS,</v>
       </c>
     </row>
     <row r="41" spans="3:6">
       <c r="C41" s="27" t="s">
-        <v>54</v>
+        <v>365</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
-        <v>VL_PIS_IMPORTACAO,</v>
+        <v>VL_PIS,</v>
       </c>
     </row>
     <row r="42" spans="3:6">
       <c r="C42" s="27" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
-        <v>VL_PIS_FRETE,</v>
+        <v>VL_PIS_MERCADORIA,</v>
       </c>
     </row>
     <row r="43" spans="3:6">
       <c r="C43" s="27" t="s">
-        <v>611</v>
+        <v>54</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
-        <v>VL_PIS_OUTROS,</v>
+        <v>VL_PIS_IMPORTACAO,</v>
       </c>
     </row>
     <row r="44" spans="3:6">
       <c r="C44" s="27" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
-        <v>VL_PERCENTUAL_COFINS,</v>
+        <v>VL_PIS_FRETE,</v>
       </c>
     </row>
     <row r="45" spans="3:6">
       <c r="C45" s="27" t="s">
-        <v>366</v>
+        <v>611</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
-        <v>VL_COFINS,</v>
+        <v>VL_PIS_OUTROS,</v>
       </c>
     </row>
     <row r="46" spans="3:6">
       <c r="C46" s="27" t="s">
-        <v>606</v>
+        <v>613</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
-        <v>VL_COFINS_MERCADORIA,</v>
+        <v>VL_PERCENTUAL_COFINS,</v>
       </c>
     </row>
     <row r="47" spans="3:6">
       <c r="C47" s="27" t="s">
-        <v>55</v>
+        <v>366</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
-        <v>VL_COFINS_IMPORTACAO,</v>
+        <v>VL_COFINS,</v>
       </c>
     </row>
     <row r="48" spans="3:6">
       <c r="C48" s="27" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
-        <v>VL_COFINS_FRETE,</v>
+        <v>VL_COFINS_MERCADORIA,</v>
       </c>
     </row>
     <row r="49" spans="3:6">
       <c r="C49" s="27" t="s">
-        <v>608</v>
+        <v>55</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
-        <v>VL_COFINS_OUTROS,</v>
+        <v>VL_COFINS_IMPORTACAO,</v>
       </c>
     </row>
     <row r="50" spans="3:6">
       <c r="C50" s="27" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
-        <v>VL_PERCENTUAL_CSLL,</v>
+        <v>VL_COFINS_FRETE,</v>
       </c>
     </row>
     <row r="51" spans="3:6">
       <c r="C51" s="27" t="s">
-        <v>367</v>
+        <v>608</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
-        <v>VL_CSLL,</v>
+        <v>VL_COFINS_OUTROS,</v>
       </c>
     </row>
     <row r="52" spans="3:6">
       <c r="C52" s="27" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
-        <v>VL_CSLL_MERCADORIA,</v>
+        <v>VL_PERCENTUAL_CSLL,</v>
       </c>
     </row>
     <row r="53" spans="3:6">
       <c r="C53" s="27" t="s">
-        <v>616</v>
+        <v>367</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
-        <v>VL_CSLL_FRETE,</v>
+        <v>VL_CSLL,</v>
       </c>
     </row>
     <row r="54" spans="3:6">
       <c r="C54" s="27" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
-        <v>VL_CSLL_OUTROS,</v>
+        <v>VL_CSLL_MERCADORIA,</v>
       </c>
     </row>
     <row r="55" spans="3:6">
       <c r="C55" s="27" t="s">
-        <v>369</v>
+        <v>616</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
-        <v>VL_BASE_IMPOSTO_IMPORTACAO,</v>
+        <v>VL_CSLL_FRETE,</v>
       </c>
     </row>
     <row r="56" spans="3:6">
       <c r="C56" s="27" t="s">
-        <v>51</v>
+        <v>617</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
-        <v>VL_IMPOSTO_IMPORTACAO,</v>
+        <v>VL_CSLL_OUTROS,</v>
       </c>
     </row>
     <row r="57" spans="3:6">
       <c r="C57" s="27" t="s">
-        <v>353</v>
+        <v>369</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="0"/>
-        <v>VL_SERVICO,</v>
+        <v>VL_BASE_IMPOSTO_IMPORTACAO,</v>
       </c>
     </row>
     <row r="58" spans="3:6">
       <c r="C58" s="27" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
-        <v>NR_PEDIDO_COMPRA,</v>
+        <v>VL_IMPOSTO_IMPORTACAO,</v>
       </c>
     </row>
     <row r="59" spans="3:6">
       <c r="C59" s="27" t="s">
-        <v>336</v>
+        <v>353</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" si="0"/>
-        <v>NR_NFR,</v>
+        <v>VL_SERVICO,</v>
       </c>
     </row>
     <row r="60" spans="3:6">
       <c r="C60" s="27" t="s">
-        <v>593</v>
+        <v>30</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
-        <v>QT_RECEBIDA,</v>
+        <v>NR_PEDIDO_COMPRA,</v>
       </c>
     </row>
     <row r="61" spans="3:6">
       <c r="C61" s="27" t="s">
-        <v>53</v>
+        <v>336</v>
       </c>
       <c r="F61" t="str">
         <f t="shared" si="0"/>
-        <v>VL_ADICIONAL_IMPORTACAO,</v>
+        <v>NR_NFR,</v>
       </c>
     </row>
     <row r="62" spans="3:6">
       <c r="C62" s="27" t="s">
-        <v>56</v>
+        <v>593</v>
       </c>
       <c r="F62" t="str">
         <f t="shared" si="0"/>
-        <v>VL_CIF_IMPORTACAO,</v>
+        <v>QT_RECEBIDA,</v>
       </c>
     </row>
     <row r="63" spans="3:6">
       <c r="C63" s="27" t="s">
-        <v>622</v>
+        <v>53</v>
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
-        <v>VL_CUSTO_IMPORTACAO,</v>
+        <v>VL_ADICIONAL_IMPORTACAO,</v>
       </c>
     </row>
     <row r="64" spans="3:6">
       <c r="C64" s="27" t="s">
-        <v>602</v>
+        <v>56</v>
       </c>
       <c r="F64" t="str">
         <f t="shared" si="0"/>
-        <v>VL_BASE_ICMS_NAO_REDUTOR,</v>
+        <v>VL_CIF_IMPORTACAO,</v>
       </c>
     </row>
     <row r="65" spans="3:6">
       <c r="C65" s="27" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="F65" t="str">
         <f t="shared" si="0"/>
-        <v>VL_PERCENTUAL_REDUTOR_ICMS,</v>
+        <v>VL_CUSTO_IMPORTACAO,</v>
       </c>
     </row>
     <row r="66" spans="3:6">
@@ -19654,5 +19648,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>